<commit_message>
Update Australian COVID-19 Infection Projections 20200315.xlsx
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\COVID-19 At Risk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99308C3C-94F7-48EF-BBC6-0C0599E52A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAF91C8-95F9-4134-9B0E-E2CE7923932A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1619,7 +1619,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> COVID-19 Accumulative Infections by Age</a:t>
+              <a:t> COVID-19 Cumulative Infections by Age</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -3420,7 +3420,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Accumulative Deaths by Age</a:t>
+              <a:t> Cumulative Deaths by Age</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -5211,7 +5211,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-AU"/>
-              <a:t>Projected COVID-19 Accumulative Infections</a:t>
+              <a:t>Projected COVID-19 Cumulative Infections</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
@@ -6504,7 +6504,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Accumulative Deaths by Comorbidity</a:t>
+              <a:t> Cumulative Deaths by Comorbidity</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -10538,10 +10538,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10842,7 +10838,7 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL29" sqref="AL29"/>
+      <selection activeCell="W74" sqref="W74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10943,71 +10939,71 @@
         <v>43904</v>
       </c>
       <c r="H7" s="75">
-        <f>G7+$B$7</f>
+        <f t="shared" ref="H7:X7" si="0">G7+$B$7</f>
         <v>43908</v>
       </c>
       <c r="I7" s="75">
-        <f>H7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43912</v>
       </c>
       <c r="J7" s="75">
-        <f>I7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43916</v>
       </c>
       <c r="K7" s="75">
-        <f>J7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43920</v>
       </c>
       <c r="L7" s="75">
-        <f>K7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43924</v>
       </c>
       <c r="M7" s="75">
-        <f>L7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43928</v>
       </c>
       <c r="N7" s="75">
-        <f>M7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43932</v>
       </c>
       <c r="O7" s="75">
-        <f>N7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43936</v>
       </c>
       <c r="P7" s="75">
-        <f>O7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43940</v>
       </c>
       <c r="Q7" s="56">
-        <f>P7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43944</v>
       </c>
       <c r="R7" s="75">
-        <f>Q7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43948</v>
       </c>
       <c r="S7" s="75">
-        <f>R7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43952</v>
       </c>
       <c r="T7" s="75">
-        <f>S7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43956</v>
       </c>
       <c r="U7" s="75">
-        <f>T7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43960</v>
       </c>
       <c r="V7" s="75">
-        <f>U7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43964</v>
       </c>
       <c r="W7" s="75">
-        <f>V7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43968</v>
       </c>
       <c r="X7" s="76">
-        <f>W7+$B$7</f>
+        <f t="shared" si="0"/>
         <v>43972</v>
       </c>
     </row>
@@ -11028,67 +11024,67 @@
         <v>500</v>
       </c>
       <c r="I8" s="33">
-        <f t="shared" ref="I8:X8" si="0">H8*2</f>
+        <f t="shared" ref="I8:X8" si="1">H8*2</f>
         <v>1000</v>
       </c>
       <c r="J8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="K8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4000</v>
       </c>
       <c r="L8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8000</v>
       </c>
       <c r="M8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16000</v>
       </c>
       <c r="N8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32000</v>
       </c>
       <c r="O8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64000</v>
       </c>
       <c r="P8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>128000</v>
       </c>
       <c r="Q8" s="57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>256000</v>
       </c>
       <c r="R8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>512000</v>
       </c>
       <c r="S8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1024000</v>
       </c>
       <c r="T8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2048000</v>
       </c>
       <c r="U8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4096000</v>
       </c>
       <c r="V8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8192000</v>
       </c>
       <c r="W8" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16384000</v>
       </c>
       <c r="X8" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32768000</v>
       </c>
     </row>
@@ -11102,75 +11098,75 @@
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
       <c r="G9" s="52">
-        <f>G8/$B$1</f>
+        <f t="shared" ref="G9:X9" si="2">G8/$B$1</f>
         <v>9.7531729412339345E-6</v>
       </c>
       <c r="H9" s="53">
-        <f>H8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>1.9506345882467869E-5</v>
       </c>
       <c r="I9" s="53">
-        <f>I8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>3.9012691764935738E-5</v>
       </c>
       <c r="J9" s="53">
-        <f>J8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>7.8025383529871476E-5</v>
       </c>
       <c r="K9" s="53">
-        <f>K8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>1.5605076705974295E-4</v>
       </c>
       <c r="L9" s="53">
-        <f>L8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>3.121015341194859E-4</v>
       </c>
       <c r="M9" s="29">
-        <f>M8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>6.2420306823897181E-4</v>
       </c>
       <c r="N9" s="29">
-        <f>N8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>1.2484061364779436E-3</v>
       </c>
       <c r="O9" s="29">
-        <f>O8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>2.4968122729558872E-3</v>
       </c>
       <c r="P9" s="29">
-        <f>P8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>4.9936245459117744E-3</v>
       </c>
       <c r="Q9" s="58">
-        <f>Q8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>9.9872490918235489E-3</v>
       </c>
       <c r="R9" s="29">
-        <f>R8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>1.9974498183647098E-2</v>
       </c>
       <c r="S9" s="29">
-        <f>S8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>3.9948996367294196E-2</v>
       </c>
       <c r="T9" s="29">
-        <f>T8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>7.9897992734588391E-2</v>
       </c>
       <c r="U9" s="29">
-        <f>U8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>0.15979598546917678</v>
       </c>
       <c r="V9" s="29">
-        <f>V8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>0.31959197093835356</v>
       </c>
       <c r="W9" s="29">
-        <f>W8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>0.63918394187670713</v>
       </c>
       <c r="X9" s="54">
-        <f>X8/$B$1</f>
+        <f t="shared" si="2"/>
         <v>1.2783678837534143</v>
       </c>
     </row>
@@ -11186,75 +11182,75 @@
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
       <c r="G10" s="25">
-        <f>G8*$B$10</f>
+        <f t="shared" ref="G10:X10" si="3">G8*$B$10</f>
         <v>37.5</v>
       </c>
       <c r="H10" s="26">
-        <f>H8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="I10" s="26">
-        <f>I8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="J10" s="26">
-        <f>J8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="K10" s="26">
-        <f>K8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
       <c r="L10" s="26">
-        <f>L8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>1200</v>
       </c>
       <c r="M10" s="26">
-        <f>M8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>2400</v>
       </c>
       <c r="N10" s="26">
-        <f>N8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>4800</v>
       </c>
       <c r="O10" s="26">
-        <f>O8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>9600</v>
       </c>
       <c r="P10" s="26">
-        <f>P8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>19200</v>
       </c>
       <c r="Q10" s="61">
-        <f>Q8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>38400</v>
       </c>
       <c r="R10" s="26">
-        <f>R8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>76800</v>
       </c>
       <c r="S10" s="26">
-        <f>S8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>153600</v>
       </c>
       <c r="T10" s="26">
-        <f>T8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>307200</v>
       </c>
       <c r="U10" s="26">
-        <f>U8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>614400</v>
       </c>
       <c r="V10" s="26">
-        <f>V8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>1228800</v>
       </c>
       <c r="W10" s="26">
-        <f>W8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>2457600</v>
       </c>
       <c r="X10" s="47">
-        <f>X8*$B$10</f>
+        <f t="shared" si="3"/>
         <v>4915200</v>
       </c>
     </row>
@@ -11276,39 +11272,39 @@
         <v>75</v>
       </c>
       <c r="I11" s="24">
-        <f t="shared" ref="I11:Q11" si="1">I10</f>
+        <f t="shared" ref="I11:Q11" si="4">I10</f>
         <v>150</v>
       </c>
       <c r="J11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>600</v>
       </c>
       <c r="L11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1200</v>
       </c>
       <c r="M11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2400</v>
       </c>
       <c r="N11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4800</v>
       </c>
       <c r="O11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9600</v>
       </c>
       <c r="P11" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19200</v>
       </c>
       <c r="Q11" s="65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>38400</v>
       </c>
       <c r="R11" s="66">
@@ -11324,11 +11320,11 @@
         <v>307050</v>
       </c>
       <c r="U11" s="24">
-        <f t="shared" ref="U11:V11" si="2">U10-J10</f>
+        <f t="shared" ref="U11:V11" si="5">U10-J10</f>
         <v>614100</v>
       </c>
       <c r="V11" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1228200</v>
       </c>
       <c r="W11" s="24">
@@ -11352,75 +11348,75 @@
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
       <c r="G12" s="25">
-        <f>G8*$B$12</f>
+        <f t="shared" ref="G12:X12" si="6">G8*$B$12</f>
         <v>12.5</v>
       </c>
       <c r="H12" s="26">
-        <f>H8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="I12" s="26">
-        <f>I8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="J12" s="26">
-        <f>J8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="K12" s="26">
-        <f>K8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="L12" s="26">
-        <f>L8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>400</v>
       </c>
       <c r="M12" s="26">
-        <f>M8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>800</v>
       </c>
       <c r="N12" s="26">
-        <f>N8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>1600</v>
       </c>
       <c r="O12" s="26">
-        <f>O8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>3200</v>
       </c>
       <c r="P12" s="26">
-        <f>P8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>6400</v>
       </c>
       <c r="Q12" s="61">
-        <f>Q8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>12800</v>
       </c>
       <c r="R12" s="26">
-        <f>R8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>25600</v>
       </c>
       <c r="S12" s="26">
-        <f>S8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>51200</v>
       </c>
       <c r="T12" s="26">
-        <f>T8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>102400</v>
       </c>
       <c r="U12" s="26">
-        <f>U8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>204800</v>
       </c>
       <c r="V12" s="26">
-        <f>V8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>409600</v>
       </c>
       <c r="W12" s="26">
-        <f>W8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>819200</v>
       </c>
       <c r="X12" s="47">
-        <f>X8*$B$12</f>
+        <f t="shared" si="6"/>
         <v>1638400</v>
       </c>
     </row>
@@ -11438,43 +11434,43 @@
         <v>7.5</v>
       </c>
       <c r="H13" s="24">
-        <f t="shared" ref="H13:Q13" si="3">H12-H14</f>
+        <f t="shared" ref="H13:Q13" si="7">H12-H14</f>
         <v>15</v>
       </c>
       <c r="I13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="J13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="K13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="L13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="M13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>480</v>
       </c>
       <c r="N13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>960</v>
       </c>
       <c r="O13" s="66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1920</v>
       </c>
       <c r="P13" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3840</v>
       </c>
       <c r="Q13" s="65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7680</v>
       </c>
       <c r="R13" s="24">
@@ -11482,27 +11478,27 @@
         <v>15352.5</v>
       </c>
       <c r="S13" s="24">
-        <f t="shared" ref="S13:X13" si="4">S12-S14-H13</f>
+        <f t="shared" ref="S13:X13" si="8">S12-S14-H13</f>
         <v>30705</v>
       </c>
       <c r="T13" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>61410</v>
       </c>
       <c r="U13" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>122820</v>
       </c>
       <c r="V13" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>245640</v>
       </c>
       <c r="W13" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>491280</v>
       </c>
       <c r="X13" s="49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>982560</v>
       </c>
     </row>
@@ -11518,75 +11514,75 @@
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
       <c r="G14" s="45">
-        <f>G8*$B$14</f>
+        <f t="shared" ref="G14:X14" si="9">G8*$B$14</f>
         <v>5</v>
       </c>
       <c r="H14" s="46">
-        <f>H8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="I14" s="46">
-        <f>I8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="J14" s="46">
-        <f>J8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="K14" s="46">
-        <f>K8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>80</v>
       </c>
       <c r="L14" s="46">
-        <f>L8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>160</v>
       </c>
       <c r="M14" s="46">
-        <f>M8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>320</v>
       </c>
       <c r="N14" s="46">
-        <f>N8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>640</v>
       </c>
       <c r="O14" s="46">
-        <f>O8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>1280</v>
       </c>
       <c r="P14" s="46">
-        <f>P8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>2560</v>
       </c>
       <c r="Q14" s="59">
-        <f>Q8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>5120</v>
       </c>
       <c r="R14" s="46">
-        <f>R8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>10240</v>
       </c>
       <c r="S14" s="46">
-        <f>S8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>20480</v>
       </c>
       <c r="T14" s="46">
-        <f>T8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>40960</v>
       </c>
       <c r="U14" s="46">
-        <f>U8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>81920</v>
       </c>
       <c r="V14" s="46">
-        <f>V8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>163840</v>
       </c>
       <c r="W14" s="46">
-        <f>W8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>327680</v>
       </c>
       <c r="X14" s="49">
-        <f>X8*$B$14</f>
+        <f t="shared" si="9"/>
         <v>655360</v>
       </c>
     </row>
@@ -11672,75 +11668,75 @@
       <c r="E18" s="17"/>
       <c r="F18" s="30"/>
       <c r="G18" s="32">
-        <f>G$8*$D$18</f>
+        <f t="shared" ref="G18:X18" si="10">G$8*$D$18</f>
         <v>7.8475336322869955</v>
       </c>
       <c r="H18" s="33">
-        <f>H$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>15.695067264573991</v>
       </c>
       <c r="I18" s="33">
-        <f>I$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>31.390134529147982</v>
       </c>
       <c r="J18" s="33">
-        <f>J$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>62.780269058295964</v>
       </c>
       <c r="K18" s="33">
-        <f>K$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>125.56053811659193</v>
       </c>
       <c r="L18" s="33">
-        <f>L$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>251.12107623318386</v>
       </c>
       <c r="M18" s="33">
-        <f>M$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>502.24215246636771</v>
       </c>
       <c r="N18" s="33">
-        <f>N$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>1004.4843049327354</v>
       </c>
       <c r="O18" s="33">
-        <f>O$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>2008.9686098654709</v>
       </c>
       <c r="P18" s="33">
-        <f>P$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>4017.9372197309417</v>
       </c>
       <c r="Q18" s="33">
-        <f>Q$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>8035.8744394618834</v>
       </c>
       <c r="R18" s="33">
-        <f>R$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>16071.748878923767</v>
       </c>
       <c r="S18" s="33">
-        <f>S$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>32143.497757847534</v>
       </c>
       <c r="T18" s="33">
-        <f>T$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>64286.995515695067</v>
       </c>
       <c r="U18" s="33">
-        <f>U$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>128573.99103139013</v>
       </c>
       <c r="V18" s="33">
-        <f>V$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>257147.98206278027</v>
       </c>
       <c r="W18" s="33">
-        <f>W$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>514295.96412556054</v>
       </c>
       <c r="X18" s="47">
-        <f>X$8*$D$18</f>
+        <f t="shared" si="10"/>
         <v>1028591.9282511211</v>
       </c>
     </row>
@@ -11757,75 +11753,75 @@
         <v>119082.78306726458</v>
       </c>
       <c r="G19" s="43">
-        <f>G$8*$D$18*$E$19</f>
+        <f t="shared" ref="G19:X19" si="11">G$8*$D$18*$E$19</f>
         <v>1.1614349775784754</v>
       </c>
       <c r="H19" s="44">
-        <f>H$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>2.3228699551569507</v>
       </c>
       <c r="I19" s="44">
-        <f>I$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>4.6457399103139014</v>
       </c>
       <c r="J19" s="44">
-        <f>J$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>9.2914798206278029</v>
       </c>
       <c r="K19" s="44">
-        <f>K$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>18.582959641255606</v>
       </c>
       <c r="L19" s="44">
-        <f>L$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>37.165919282511211</v>
       </c>
       <c r="M19" s="44">
-        <f>M$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>74.331838565022423</v>
       </c>
       <c r="N19" s="44">
-        <f>N$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>148.66367713004485</v>
       </c>
       <c r="O19" s="44">
-        <f>O$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>297.32735426008969</v>
       </c>
       <c r="P19" s="44">
-        <f>P$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>594.65470852017938</v>
       </c>
       <c r="Q19" s="44">
-        <f>Q$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>1189.3094170403588</v>
       </c>
       <c r="R19" s="44">
-        <f>R$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>2378.6188340807175</v>
       </c>
       <c r="S19" s="44">
-        <f>S$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>4757.2376681614351</v>
       </c>
       <c r="T19" s="44">
-        <f>T$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>9514.4753363228701</v>
       </c>
       <c r="U19" s="44">
-        <f>U$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>19028.95067264574</v>
       </c>
       <c r="V19" s="44">
-        <f>V$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>38057.901345291481</v>
       </c>
       <c r="W19" s="44">
-        <f>W$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>76115.802690582961</v>
       </c>
       <c r="X19" s="48">
-        <f>X$8*$D$18*$E$19</f>
+        <f t="shared" si="11"/>
         <v>152231.60538116592</v>
       </c>
     </row>
@@ -11837,7 +11833,7 @@
         <v>6.8733756751875541E-2</v>
       </c>
       <c r="C20" s="22">
-        <f t="shared" ref="C20:C34" si="5">$B$1*B20</f>
+        <f t="shared" ref="C20:C34" si="12">$B$1*B20</f>
         <v>1761830.6669536922</v>
       </c>
       <c r="D20" s="37">
@@ -11847,75 +11843,75 @@
       <c r="E20" s="31"/>
       <c r="F20" s="30"/>
       <c r="G20" s="34">
-        <f>G$8*$D$20</f>
+        <f t="shared" ref="G20:X20" si="13">G$8*$D$20</f>
         <v>14.573991031390134</v>
       </c>
       <c r="H20" s="35">
-        <f>H$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>29.147982062780269</v>
       </c>
       <c r="I20" s="35">
-        <f>I$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>58.295964125560538</v>
       </c>
       <c r="J20" s="35">
-        <f>J$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>116.59192825112108</v>
       </c>
       <c r="K20" s="35">
-        <f>K$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>233.18385650224215</v>
       </c>
       <c r="L20" s="35">
-        <f>L$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>466.3677130044843</v>
       </c>
       <c r="M20" s="35">
-        <f>M$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>932.7354260089686</v>
       </c>
       <c r="N20" s="35">
-        <f>N$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>1865.4708520179372</v>
       </c>
       <c r="O20" s="35">
-        <f>O$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>3730.9417040358744</v>
       </c>
       <c r="P20" s="35">
-        <f>P$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>7461.8834080717488</v>
       </c>
       <c r="Q20" s="35">
-        <f>Q$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>14923.766816143498</v>
       </c>
       <c r="R20" s="35">
-        <f>R$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>29847.533632286995</v>
       </c>
       <c r="S20" s="35">
-        <f>S$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>59695.067264573991</v>
       </c>
       <c r="T20" s="35">
-        <f>T$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>119390.13452914798</v>
       </c>
       <c r="U20" s="35">
-        <f>U$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>238780.26905829596</v>
       </c>
       <c r="V20" s="35">
-        <f>V$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>477560.53811659192</v>
       </c>
       <c r="W20" s="35">
-        <f>W$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>955121.07623318385</v>
       </c>
       <c r="X20" s="48">
-        <f>X$8*$D$20</f>
+        <f t="shared" si="13"/>
         <v>1910242.1524663677</v>
       </c>
     </row>
@@ -11932,75 +11928,75 @@
         <v>119542.56215246637</v>
       </c>
       <c r="G21" s="43">
-        <f>G$8*$D$20*$E$21</f>
+        <f t="shared" ref="G21:X21" si="14">G$8*$D$20*$E$21</f>
         <v>1.1659192825112108</v>
       </c>
       <c r="H21" s="44">
-        <f>H$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>2.3318385650224216</v>
       </c>
       <c r="I21" s="44">
-        <f>I$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>4.6636771300448432</v>
       </c>
       <c r="J21" s="44">
-        <f>J$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>9.3273542600896864</v>
       </c>
       <c r="K21" s="44">
-        <f>K$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>18.654708520179373</v>
       </c>
       <c r="L21" s="44">
-        <f>L$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>37.309417040358746</v>
       </c>
       <c r="M21" s="44">
-        <f>M$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>74.618834080717491</v>
       </c>
       <c r="N21" s="44">
-        <f>N$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>149.23766816143498</v>
       </c>
       <c r="O21" s="44">
-        <f>O$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>298.47533632286996</v>
       </c>
       <c r="P21" s="44">
-        <f>P$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>596.95067264573993</v>
       </c>
       <c r="Q21" s="44">
-        <f>Q$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>1193.9013452914799</v>
       </c>
       <c r="R21" s="44">
-        <f>R$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>2387.8026905829597</v>
       </c>
       <c r="S21" s="44">
-        <f>S$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>4775.6053811659194</v>
       </c>
       <c r="T21" s="44">
-        <f>T$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>9551.2107623318389</v>
       </c>
       <c r="U21" s="44">
-        <f>U$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>19102.421524663678</v>
       </c>
       <c r="V21" s="44">
-        <f>V$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>38204.843049327355</v>
       </c>
       <c r="W21" s="44">
-        <f>W$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>76409.686098654711</v>
       </c>
       <c r="X21" s="48">
-        <f>X$8*$D$20*$E$21</f>
+        <f t="shared" si="14"/>
         <v>152819.37219730942</v>
       </c>
     </row>
@@ -12012,7 +12008,7 @@
         <v>0.10271036487346757</v>
       </c>
       <c r="C22" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>2632742.3263262943</v>
       </c>
       <c r="D22" s="37">
@@ -12022,75 +12018,75 @@
       <c r="E22" s="31"/>
       <c r="F22" s="22"/>
       <c r="G22" s="34">
-        <f>G$8*$D$22</f>
+        <f t="shared" ref="G22:X22" si="15">G$8*$D$22</f>
         <v>36.995515695067269</v>
       </c>
       <c r="H22" s="35">
-        <f>H$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>73.991031390134538</v>
       </c>
       <c r="I22" s="35">
-        <f>I$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>147.98206278026908</v>
       </c>
       <c r="J22" s="35">
-        <f>J$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>295.96412556053815</v>
       </c>
       <c r="K22" s="35">
-        <f>K$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>591.9282511210763</v>
       </c>
       <c r="L22" s="35">
-        <f>L$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>1183.8565022421526</v>
       </c>
       <c r="M22" s="35">
-        <f>M$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>2367.7130044843052</v>
       </c>
       <c r="N22" s="35">
-        <f>N$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>4735.4260089686104</v>
       </c>
       <c r="O22" s="35">
-        <f>O$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>9470.8520179372208</v>
       </c>
       <c r="P22" s="35">
-        <f>P$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>18941.704035874442</v>
       </c>
       <c r="Q22" s="35">
-        <f>Q$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>37883.408071748883</v>
       </c>
       <c r="R22" s="35">
-        <f>R$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>75766.816143497766</v>
       </c>
       <c r="S22" s="35">
-        <f>S$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>151533.63228699553</v>
       </c>
       <c r="T22" s="35">
-        <f>T$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>303067.26457399107</v>
       </c>
       <c r="U22" s="35">
-        <f>U$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>606134.52914798213</v>
       </c>
       <c r="V22" s="35">
-        <f>V$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>1212269.0582959643</v>
       </c>
       <c r="W22" s="35">
-        <f>W$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>2424538.1165919285</v>
       </c>
       <c r="X22" s="48">
-        <f>X$8*$D$22</f>
+        <f t="shared" si="15"/>
         <v>4849076.2331838571</v>
       </c>
     </row>
@@ -12107,75 +12103,75 @@
         <v>136554.38830493274</v>
       </c>
       <c r="G23" s="43">
-        <f>G$8*$D$22*$E$23</f>
+        <f t="shared" ref="G23:X23" si="16">G$8*$D$22*$E$23</f>
         <v>1.3318385650224216</v>
       </c>
       <c r="H23" s="44">
-        <f>H$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>2.6636771300448432</v>
       </c>
       <c r="I23" s="44">
-        <f>I$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>5.3273542600896864</v>
       </c>
       <c r="J23" s="44">
-        <f>J$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>10.654708520179373</v>
       </c>
       <c r="K23" s="44">
-        <f>K$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>21.309417040358746</v>
       </c>
       <c r="L23" s="44">
-        <f>L$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>42.618834080717491</v>
       </c>
       <c r="M23" s="44">
-        <f>M$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>85.237668161434982</v>
       </c>
       <c r="N23" s="44">
-        <f>N$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>170.47533632286996</v>
       </c>
       <c r="O23" s="44">
-        <f>O$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>340.95067264573993</v>
       </c>
       <c r="P23" s="44">
-        <f>P$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>681.90134529147986</v>
       </c>
       <c r="Q23" s="44">
-        <f>Q$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>1363.8026905829597</v>
       </c>
       <c r="R23" s="44">
-        <f>R$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>2727.6053811659194</v>
       </c>
       <c r="S23" s="44">
-        <f>S$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>5455.2107623318389</v>
       </c>
       <c r="T23" s="44">
-        <f>T$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>10910.421524663678</v>
       </c>
       <c r="U23" s="44">
-        <f>U$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>21820.843049327355</v>
       </c>
       <c r="V23" s="44">
-        <f>V$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>43641.686098654711</v>
       </c>
       <c r="W23" s="44">
-        <f>W$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>87283.372197309422</v>
       </c>
       <c r="X23" s="48">
-        <f>X$8*$D$22*$E$23</f>
+        <f t="shared" si="16"/>
         <v>174566.74439461884</v>
       </c>
     </row>
@@ -12187,7 +12183,7 @@
         <v>0.12241761174778311</v>
       </c>
       <c r="C24" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>3137891.9579656119</v>
       </c>
       <c r="D24" s="37">
@@ -12197,75 +12193,75 @@
       <c r="E24" s="31"/>
       <c r="F24" s="22"/>
       <c r="G24" s="34">
-        <f>G$8*$D$24</f>
+        <f t="shared" ref="G24:X24" si="17">G$8*$D$24</f>
         <v>43.721973094170401</v>
       </c>
       <c r="H24" s="35">
-        <f>H$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>87.443946188340803</v>
       </c>
       <c r="I24" s="35">
-        <f>I$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>174.88789237668161</v>
       </c>
       <c r="J24" s="35">
-        <f>J$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>349.77578475336321</v>
       </c>
       <c r="K24" s="35">
-        <f>K$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>699.55156950672642</v>
       </c>
       <c r="L24" s="35">
-        <f>L$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>1399.1031390134528</v>
       </c>
       <c r="M24" s="35">
-        <f>M$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>2798.2062780269057</v>
       </c>
       <c r="N24" s="35">
-        <f>N$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>5596.4125560538114</v>
       </c>
       <c r="O24" s="35">
-        <f>O$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>11192.825112107623</v>
       </c>
       <c r="P24" s="35">
-        <f>P$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>22385.650224215246</v>
       </c>
       <c r="Q24" s="35">
-        <f>Q$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>44771.300448430491</v>
       </c>
       <c r="R24" s="35">
-        <f>R$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>89542.600896860982</v>
       </c>
       <c r="S24" s="35">
-        <f>S$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>179085.20179372196</v>
       </c>
       <c r="T24" s="35">
-        <f>T$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>358170.40358744393</v>
       </c>
       <c r="U24" s="35">
-        <f>U$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>716340.80717488786</v>
       </c>
       <c r="V24" s="35">
-        <f>V$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>1432681.6143497757</v>
       </c>
       <c r="W24" s="35">
-        <f>W$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>2865363.2286995514</v>
       </c>
       <c r="X24" s="48">
-        <f>X$8*$D$24</f>
+        <f t="shared" si="17"/>
         <v>5730726.4573991029</v>
       </c>
     </row>
@@ -12282,75 +12278,75 @@
         <v>58276.999049327358</v>
       </c>
       <c r="G25" s="43">
-        <f>G$8*$D$24*$E$25</f>
+        <f t="shared" ref="G25:X25" si="18">G$8*$D$24*$E$25</f>
         <v>0.56838565022421517</v>
       </c>
       <c r="H25" s="44">
-        <f>H$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>1.1367713004484303</v>
       </c>
       <c r="I25" s="44">
-        <f>I$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>2.2735426008968607</v>
       </c>
       <c r="J25" s="44">
-        <f>J$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>4.5470852017937213</v>
       </c>
       <c r="K25" s="44">
-        <f>K$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>9.0941704035874427</v>
       </c>
       <c r="L25" s="44">
-        <f>L$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>18.188340807174885</v>
       </c>
       <c r="M25" s="44">
-        <f>M$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>36.376681614349771</v>
       </c>
       <c r="N25" s="44">
-        <f>N$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>72.753363228699541</v>
       </c>
       <c r="O25" s="44">
-        <f>O$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>145.50672645739908</v>
       </c>
       <c r="P25" s="44">
-        <f>P$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>291.01345291479817</v>
       </c>
       <c r="Q25" s="44">
-        <f>Q$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>582.02690582959633</v>
       </c>
       <c r="R25" s="44">
-        <f>R$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>1164.0538116591927</v>
       </c>
       <c r="S25" s="44">
-        <f>S$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>2328.1076233183853</v>
       </c>
       <c r="T25" s="44">
-        <f>T$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>4656.2152466367706</v>
       </c>
       <c r="U25" s="44">
-        <f>U$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>9312.4304932735413</v>
       </c>
       <c r="V25" s="44">
-        <f>V$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>18624.860986547083</v>
       </c>
       <c r="W25" s="44">
-        <f>W$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>37249.721973094165</v>
       </c>
       <c r="X25" s="48">
-        <f>X$8*$D$24*$E$25</f>
+        <f t="shared" si="18"/>
         <v>74499.44394618833</v>
       </c>
     </row>
@@ -12362,7 +12358,7 @@
         <v>0.1307371328497558</v>
       </c>
       <c r="C26" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>3351143.6134038097</v>
       </c>
       <c r="D26" s="37">
@@ -12372,75 +12368,75 @@
       <c r="E26" s="31"/>
       <c r="F26" s="22"/>
       <c r="G26" s="34">
-        <f>G$8*$D$26</f>
+        <f t="shared" ref="G26:X26" si="19">G$8*$D$26</f>
         <v>43.721973094170401</v>
       </c>
       <c r="H26" s="35">
-        <f>H$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>87.443946188340803</v>
       </c>
       <c r="I26" s="35">
-        <f>I$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>174.88789237668161</v>
       </c>
       <c r="J26" s="35">
-        <f>J$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>349.77578475336321</v>
       </c>
       <c r="K26" s="35">
-        <f>K$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>699.55156950672642</v>
       </c>
       <c r="L26" s="35">
-        <f>L$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>1399.1031390134528</v>
       </c>
       <c r="M26" s="35">
-        <f>M$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>2798.2062780269057</v>
       </c>
       <c r="N26" s="35">
-        <f>N$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>5596.4125560538114</v>
       </c>
       <c r="O26" s="35">
-        <f>O$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>11192.825112107623</v>
       </c>
       <c r="P26" s="35">
-        <f>P$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>22385.650224215246</v>
       </c>
       <c r="Q26" s="35">
-        <f>Q$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>44771.300448430491</v>
       </c>
       <c r="R26" s="35">
-        <f>R$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>89542.600896860982</v>
       </c>
       <c r="S26" s="35">
-        <f>S$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>179085.20179372196</v>
       </c>
       <c r="T26" s="35">
-        <f>T$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>358170.40358744393</v>
       </c>
       <c r="U26" s="35">
-        <f>U$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>716340.80717488786</v>
       </c>
       <c r="V26" s="35">
-        <f>V$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>1432681.6143497757</v>
       </c>
       <c r="W26" s="35">
-        <f>W$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>2865363.2286995514</v>
       </c>
       <c r="X26" s="48">
-        <f>X$8*$D$26</f>
+        <f t="shared" si="19"/>
         <v>5730726.4573991029</v>
       </c>
     </row>
@@ -12457,75 +12453,75 @@
         <v>17931.384322869955</v>
       </c>
       <c r="G27" s="43">
-        <f>G$8*$D$26*$E$27</f>
+        <f t="shared" ref="G27:X27" si="20">G$8*$D$26*$E$27</f>
         <v>0.17488789237668162</v>
       </c>
       <c r="H27" s="44">
-        <f>H$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>0.34977578475336324</v>
       </c>
       <c r="I27" s="44">
-        <f>I$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>0.69955156950672648</v>
       </c>
       <c r="J27" s="44">
-        <f>J$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>1.399103139013453</v>
       </c>
       <c r="K27" s="44">
-        <f>K$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>2.7982062780269059</v>
       </c>
       <c r="L27" s="44">
-        <f>L$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>5.5964125560538118</v>
       </c>
       <c r="M27" s="44">
-        <f>M$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>11.192825112107624</v>
       </c>
       <c r="N27" s="44">
-        <f>N$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>22.385650224215247</v>
       </c>
       <c r="O27" s="44">
-        <f>O$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>44.771300448430495</v>
       </c>
       <c r="P27" s="44">
-        <f>P$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>89.542600896860989</v>
       </c>
       <c r="Q27" s="44">
-        <f>Q$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>179.08520179372198</v>
       </c>
       <c r="R27" s="44">
-        <f>R$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>358.17040358744396</v>
       </c>
       <c r="S27" s="44">
-        <f>S$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>716.34080717488791</v>
       </c>
       <c r="T27" s="44">
-        <f>T$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>1432.6816143497758</v>
       </c>
       <c r="U27" s="44">
-        <f>U$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>2865.3632286995517</v>
       </c>
       <c r="V27" s="44">
-        <f>V$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>5730.7264573991033</v>
       </c>
       <c r="W27" s="44">
-        <f>W$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>11461.452914798207</v>
       </c>
       <c r="X27" s="48">
-        <f>X$8*$D$26*$E$27</f>
+        <f t="shared" si="20"/>
         <v>22922.905829596413</v>
       </c>
     </row>
@@ -12537,7 +12533,7 @@
         <v>0.14352807031813389</v>
       </c>
       <c r="C28" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>3679009.6715945052</v>
       </c>
       <c r="D28" s="37">
@@ -12547,75 +12543,75 @@
       <c r="E28" s="31"/>
       <c r="F28" s="22"/>
       <c r="G28" s="34">
-        <f>G$8*$D$28</f>
+        <f t="shared" ref="G28:X28" si="21">G$8*$D$28</f>
         <v>48.206278026905828</v>
       </c>
       <c r="H28" s="35">
-        <f>H$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>96.412556053811656</v>
       </c>
       <c r="I28" s="35">
-        <f>I$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>192.82511210762331</v>
       </c>
       <c r="J28" s="35">
-        <f>J$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>385.65022421524662</v>
       </c>
       <c r="K28" s="35">
-        <f>K$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>771.30044843049325</v>
       </c>
       <c r="L28" s="35">
-        <f>L$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>1542.6008968609865</v>
       </c>
       <c r="M28" s="35">
-        <f>M$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>3085.201793721973</v>
       </c>
       <c r="N28" s="35">
-        <f>N$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>6170.403587443946</v>
       </c>
       <c r="O28" s="35">
-        <f>O$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>12340.807174887892</v>
       </c>
       <c r="P28" s="35">
-        <f>P$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>24681.614349775784</v>
       </c>
       <c r="Q28" s="35">
-        <f>Q$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>49363.228699551568</v>
       </c>
       <c r="R28" s="35">
-        <f>R$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>98726.457399103136</v>
       </c>
       <c r="S28" s="35">
-        <f>S$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>197452.91479820627</v>
       </c>
       <c r="T28" s="35">
-        <f>T$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>394905.82959641254</v>
       </c>
       <c r="U28" s="35">
-        <f>U$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>789811.65919282509</v>
       </c>
       <c r="V28" s="35">
-        <f>V$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>1579623.3183856502</v>
       </c>
       <c r="W28" s="35">
-        <f>W$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>3159246.6367713003</v>
       </c>
       <c r="X28" s="48">
-        <f>X$8*$D$28</f>
+        <f t="shared" si="21"/>
         <v>6318493.2735426007</v>
       </c>
     </row>
@@ -12632,75 +12628,75 @@
         <v>9885.2503318385643</v>
       </c>
       <c r="G29" s="43">
-        <f>G$8*$D$28*$E$29</f>
+        <f t="shared" ref="G29:X29" si="22">G$8*$D$28*$E$29</f>
         <v>9.641255605381166E-2</v>
       </c>
       <c r="H29" s="44">
-        <f>H$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>0.19282511210762332</v>
       </c>
       <c r="I29" s="44">
-        <f>I$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>0.38565022421524664</v>
       </c>
       <c r="J29" s="44">
-        <f>J$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>0.77130044843049328</v>
       </c>
       <c r="K29" s="44">
-        <f>K$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>1.5426008968609866</v>
       </c>
       <c r="L29" s="44">
-        <f>L$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>3.0852017937219731</v>
       </c>
       <c r="M29" s="44">
-        <f>M$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>6.1704035874439462</v>
       </c>
       <c r="N29" s="44">
-        <f>N$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>12.340807174887892</v>
       </c>
       <c r="O29" s="44">
-        <f>O$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>24.681614349775785</v>
       </c>
       <c r="P29" s="44">
-        <f>P$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>49.36322869955157</v>
       </c>
       <c r="Q29" s="44">
-        <f>Q$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>98.72645739910314</v>
       </c>
       <c r="R29" s="44">
-        <f>R$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>197.45291479820628</v>
       </c>
       <c r="S29" s="44">
-        <f>S$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>394.90582959641256</v>
       </c>
       <c r="T29" s="44">
-        <f>T$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>789.81165919282512</v>
       </c>
       <c r="U29" s="44">
-        <f>U$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>1579.6233183856502</v>
       </c>
       <c r="V29" s="44">
-        <f>V$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>3159.2466367713005</v>
       </c>
       <c r="W29" s="44">
-        <f>W$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>6318.4932735426009</v>
       </c>
       <c r="X29" s="48">
-        <f>X$8*$D$28*$E$29</f>
+        <f t="shared" si="22"/>
         <v>12636.986547085202</v>
       </c>
     </row>
@@ -12712,7 +12708,7 @@
         <v>0.14477837612990244</v>
       </c>
       <c r="C30" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>3711058.365370932</v>
       </c>
       <c r="D30" s="37">
@@ -12722,75 +12718,75 @@
       <c r="E30" s="31"/>
       <c r="F30" s="22"/>
       <c r="G30" s="34">
-        <f>G$8*$D$30</f>
+        <f t="shared" ref="G30:X30" si="23">G$8*$D$30</f>
         <v>38.116591928251118</v>
       </c>
       <c r="H30" s="35">
-        <f>H$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>76.233183856502237</v>
       </c>
       <c r="I30" s="35">
-        <f>I$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>152.46636771300447</v>
       </c>
       <c r="J30" s="35">
-        <f>J$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>304.93273542600895</v>
       </c>
       <c r="K30" s="35">
-        <f>K$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>609.86547085201789</v>
       </c>
       <c r="L30" s="35">
-        <f>L$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>1219.7309417040358</v>
       </c>
       <c r="M30" s="35">
-        <f>M$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>2439.4618834080716</v>
       </c>
       <c r="N30" s="35">
-        <f>N$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>4878.9237668161431</v>
       </c>
       <c r="O30" s="35">
-        <f>O$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>9757.8475336322863</v>
       </c>
       <c r="P30" s="35">
-        <f>P$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>19515.695067264573</v>
       </c>
       <c r="Q30" s="35">
-        <f>Q$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>39031.390134529145</v>
       </c>
       <c r="R30" s="35">
-        <f>R$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>78062.78026905829</v>
       </c>
       <c r="S30" s="35">
-        <f>S$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>156125.56053811658</v>
       </c>
       <c r="T30" s="35">
-        <f>T$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>312251.12107623316</v>
       </c>
       <c r="U30" s="35">
-        <f>U$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>624502.24215246632</v>
       </c>
       <c r="V30" s="35">
-        <f>V$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>1249004.4843049326</v>
       </c>
       <c r="W30" s="35">
-        <f>W$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>2498008.9686098653</v>
       </c>
       <c r="X30" s="48">
-        <f>X$8*$D$30</f>
+        <f t="shared" si="23"/>
         <v>4996017.9372197306</v>
       </c>
     </row>
@@ -12807,75 +12803,75 @@
         <v>7816.2444484304933</v>
       </c>
       <c r="G31" s="43">
-        <f>G$8*$D$30*$E$31</f>
+        <f t="shared" ref="G31:X31" si="24">G$8*$D$30*$E$31</f>
         <v>7.623318385650224E-2</v>
       </c>
       <c r="H31" s="44">
-        <f>H$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>0.15246636771300448</v>
       </c>
       <c r="I31" s="44">
-        <f>I$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>0.30493273542600896</v>
       </c>
       <c r="J31" s="44">
-        <f>J$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>0.60986547085201792</v>
       </c>
       <c r="K31" s="44">
-        <f>K$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>1.2197309417040358</v>
       </c>
       <c r="L31" s="44">
-        <f>L$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>2.4394618834080717</v>
       </c>
       <c r="M31" s="44">
-        <f>M$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>4.8789237668161434</v>
       </c>
       <c r="N31" s="44">
-        <f>N$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>9.7578475336322867</v>
       </c>
       <c r="O31" s="44">
-        <f>O$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>19.515695067264573</v>
       </c>
       <c r="P31" s="44">
-        <f>P$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>39.031390134529147</v>
       </c>
       <c r="Q31" s="44">
-        <f>Q$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>78.062780269058294</v>
       </c>
       <c r="R31" s="44">
-        <f>R$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>156.12556053811659</v>
       </c>
       <c r="S31" s="44">
-        <f>S$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>312.25112107623318</v>
       </c>
       <c r="T31" s="44">
-        <f>T$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>624.50224215246635</v>
       </c>
       <c r="U31" s="44">
-        <f>U$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>1249.0044843049327</v>
       </c>
       <c r="V31" s="44">
-        <f>V$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>2498.0089686098654</v>
       </c>
       <c r="W31" s="44">
-        <f>W$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>4996.0179372197308</v>
       </c>
       <c r="X31" s="48">
-        <f>X$8*$D$30*$E$31</f>
+        <f t="shared" si="24"/>
         <v>9992.0358744394616</v>
       </c>
     </row>
@@ -12887,7 +12883,7 @@
         <v>0.12034977981552665</v>
       </c>
       <c r="C32" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>3084887.8754809727</v>
       </c>
       <c r="D32" s="37">
@@ -12897,75 +12893,75 @@
       <c r="E32" s="31"/>
       <c r="F32" s="22"/>
       <c r="G32" s="34">
-        <f>G$8*$D$32</f>
+        <f t="shared" ref="G32:X32" si="25">G$8*$D$32</f>
         <v>13.45291479820628</v>
       </c>
       <c r="H32" s="35">
-        <f>H$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>26.905829596412559</v>
       </c>
       <c r="I32" s="35">
-        <f>I$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>53.811659192825118</v>
       </c>
       <c r="J32" s="35">
-        <f>J$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>107.62331838565024</v>
       </c>
       <c r="K32" s="35">
-        <f>K$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>215.24663677130047</v>
       </c>
       <c r="L32" s="35">
-        <f>L$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>430.49327354260095</v>
       </c>
       <c r="M32" s="35">
-        <f>M$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>860.98654708520189</v>
       </c>
       <c r="N32" s="35">
-        <f>N$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>1721.9730941704038</v>
       </c>
       <c r="O32" s="35">
-        <f>O$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>3443.9461883408076</v>
       </c>
       <c r="P32" s="35">
-        <f>P$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>6887.8923766816151</v>
       </c>
       <c r="Q32" s="35">
-        <f>Q$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>13775.78475336323</v>
       </c>
       <c r="R32" s="35">
-        <f>R$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>27551.569506726461</v>
       </c>
       <c r="S32" s="35">
-        <f>S$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>55103.139013452921</v>
       </c>
       <c r="T32" s="35">
-        <f>T$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>110206.27802690584</v>
       </c>
       <c r="U32" s="35">
-        <f>U$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>220412.55605381168</v>
       </c>
       <c r="V32" s="35">
-        <f>V$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>440825.11210762337</v>
       </c>
       <c r="W32" s="35">
-        <f>W$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>881650.22421524674</v>
       </c>
       <c r="X32" s="48">
-        <f>X$8*$D$32</f>
+        <f t="shared" si="25"/>
         <v>1763300.4484304935</v>
       </c>
     </row>
@@ -12982,75 +12978,75 @@
         <v>2758.6745112107624</v>
       </c>
       <c r="G33" s="43">
-        <f>G$8*$D$32*$E$33</f>
+        <f t="shared" ref="G33:X33" si="26">G$8*$D$32*$E$33</f>
         <v>2.6905829596412561E-2</v>
       </c>
       <c r="H33" s="44">
-        <f>H$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>5.3811659192825122E-2</v>
       </c>
       <c r="I33" s="44">
-        <f>I$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>0.10762331838565024</v>
       </c>
       <c r="J33" s="44">
-        <f>J$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>0.21524663677130049</v>
       </c>
       <c r="K33" s="44">
-        <f>K$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>0.43049327354260097</v>
       </c>
       <c r="L33" s="44">
-        <f>L$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>0.86098654708520195</v>
       </c>
       <c r="M33" s="44">
-        <f>M$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>1.7219730941704039</v>
       </c>
       <c r="N33" s="44">
-        <f>N$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>3.4439461883408078</v>
       </c>
       <c r="O33" s="44">
-        <f>O$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>6.8878923766816156</v>
       </c>
       <c r="P33" s="44">
-        <f>P$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>13.775784753363231</v>
       </c>
       <c r="Q33" s="44">
-        <f>Q$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>27.551569506726462</v>
       </c>
       <c r="R33" s="44">
-        <f>R$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>55.103139013452925</v>
       </c>
       <c r="S33" s="44">
-        <f>S$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>110.20627802690585</v>
       </c>
       <c r="T33" s="44">
-        <f>T$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>220.4125560538117</v>
       </c>
       <c r="U33" s="44">
-        <f>U$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>440.8251121076234</v>
       </c>
       <c r="V33" s="44">
-        <f>V$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>881.65022421524679</v>
       </c>
       <c r="W33" s="44">
-        <f>W$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>1763.3004484304936</v>
       </c>
       <c r="X33" s="48">
-        <f>X$8*$D$32*$E$33</f>
+        <f t="shared" si="26"/>
         <v>3526.6008968609872</v>
       </c>
     </row>
@@ -13062,7 +13058,7 @@
         <v>0.12716137671014424</v>
       </c>
       <c r="C34" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>3259487.3862160868</v>
       </c>
       <c r="D34" s="37">
@@ -13072,75 +13068,75 @@
       <c r="E34" s="31"/>
       <c r="F34" s="22"/>
       <c r="G34" s="34">
-        <f>G$8*$D$34</f>
+        <f t="shared" ref="G34:X34" si="27">G$8*$D$34</f>
         <v>3.3632286995515699</v>
       </c>
       <c r="H34" s="35">
-        <f>H$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>6.7264573991031398</v>
       </c>
       <c r="I34" s="35">
-        <f>I$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>13.45291479820628</v>
       </c>
       <c r="J34" s="35">
-        <f>J$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>26.905829596412559</v>
       </c>
       <c r="K34" s="35">
-        <f>K$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>53.811659192825118</v>
       </c>
       <c r="L34" s="35">
-        <f>L$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>107.62331838565024</v>
       </c>
       <c r="M34" s="35">
-        <f>M$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>215.24663677130047</v>
       </c>
       <c r="N34" s="35">
-        <f>N$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>430.49327354260095</v>
       </c>
       <c r="O34" s="35">
-        <f>O$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>860.98654708520189</v>
       </c>
       <c r="P34" s="35">
-        <f>P$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>1721.9730941704038</v>
       </c>
       <c r="Q34" s="35">
-        <f>Q$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>3443.9461883408076</v>
       </c>
       <c r="R34" s="35">
-        <f>R$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>6887.8923766816151</v>
       </c>
       <c r="S34" s="35">
-        <f>S$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>13775.78475336323</v>
       </c>
       <c r="T34" s="35">
-        <f>T$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>27551.569506726461</v>
       </c>
       <c r="U34" s="35">
-        <f>U$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>55103.139013452921</v>
       </c>
       <c r="V34" s="35">
-        <f>V$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>110206.27802690584</v>
       </c>
       <c r="W34" s="35">
-        <f>W$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>220412.55605381168</v>
       </c>
       <c r="X34" s="48">
-        <f>X$8*$D$34</f>
+        <f t="shared" si="27"/>
         <v>440825.11210762337</v>
       </c>
     </row>
@@ -13157,75 +13153,75 @@
         <v>0</v>
       </c>
       <c r="G35" s="45">
-        <f>G$8*$D$34*$E$35</f>
+        <f t="shared" ref="G35:X35" si="28">G$8*$D$34*$E$35</f>
         <v>0</v>
       </c>
       <c r="H35" s="46">
-        <f>H$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="I35" s="46">
-        <f>I$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J35" s="46">
-        <f>J$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="K35" s="46">
-        <f>K$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="L35" s="46">
-        <f>L$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="M35" s="46">
-        <f>M$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="N35" s="46">
-        <f>N$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O35" s="46">
-        <f>O$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P35" s="46">
-        <f>P$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q35" s="46">
-        <f>Q$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="R35" s="46">
-        <f>R$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="S35" s="46">
-        <f>S$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="T35" s="46">
-        <f>T$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="U35" s="46">
-        <f>U$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="V35" s="46">
-        <f>V$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="W35" s="46">
-        <f>W$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="X35" s="49">
-        <f>X$8*$D$34*$E$35</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
@@ -13239,75 +13235,75 @@
       <c r="E36" s="29"/>
       <c r="F36" s="22"/>
       <c r="G36" s="32">
-        <f>SUM(G18,G20,G22,G24,G26,G28,G30,G32,G34)</f>
+        <f t="shared" ref="G36:X36" si="29">SUM(G18,G20,G22,G24,G26,G28,G30,G32,G34)</f>
         <v>250.00000000000003</v>
       </c>
       <c r="H36" s="33">
-        <f>SUM(H18,H20,H22,H24,H26,H28,H30,H32,H34)</f>
+        <f t="shared" si="29"/>
         <v>500.00000000000006</v>
       </c>
       <c r="I36" s="33">
-        <f>SUM(I18,I20,I22,I24,I26,I28,I30,I32,I34)</f>
+        <f t="shared" si="29"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="J36" s="33">
-        <f>SUM(J18,J20,J22,J24,J26,J28,J30,J32,J34)</f>
+        <f t="shared" si="29"/>
         <v>2000.0000000000002</v>
       </c>
       <c r="K36" s="33">
-        <f>SUM(K18,K20,K22,K24,K26,K28,K30,K32,K34)</f>
+        <f t="shared" si="29"/>
         <v>4000.0000000000005</v>
       </c>
       <c r="L36" s="33">
-        <f>SUM(L18,L20,L22,L24,L26,L28,L30,L32,L34)</f>
+        <f t="shared" si="29"/>
         <v>8000.0000000000009</v>
       </c>
       <c r="M36" s="33">
-        <f>SUM(M18,M20,M22,M24,M26,M28,M30,M32,M34)</f>
+        <f t="shared" si="29"/>
         <v>16000.000000000002</v>
       </c>
       <c r="N36" s="33">
-        <f>SUM(N18,N20,N22,N24,N26,N28,N30,N32,N34)</f>
+        <f t="shared" si="29"/>
         <v>32000.000000000004</v>
       </c>
       <c r="O36" s="33">
-        <f>SUM(O18,O20,O22,O24,O26,O28,O30,O32,O34)</f>
+        <f t="shared" si="29"/>
         <v>64000.000000000007</v>
       </c>
       <c r="P36" s="33">
-        <f>SUM(P18,P20,P22,P24,P26,P28,P30,P32,P34)</f>
+        <f t="shared" si="29"/>
         <v>128000.00000000001</v>
       </c>
       <c r="Q36" s="33">
-        <f>SUM(Q18,Q20,Q22,Q24,Q26,Q28,Q30,Q32,Q34)</f>
+        <f t="shared" si="29"/>
         <v>256000.00000000003</v>
       </c>
       <c r="R36" s="33">
-        <f>SUM(R18,R20,R22,R24,R26,R28,R30,R32,R34)</f>
+        <f t="shared" si="29"/>
         <v>512000.00000000006</v>
       </c>
       <c r="S36" s="33">
-        <f>SUM(S18,S20,S22,S24,S26,S28,S30,S32,S34)</f>
+        <f t="shared" si="29"/>
         <v>1024000.0000000001</v>
       </c>
       <c r="T36" s="33">
-        <f>SUM(T18,T20,T22,T24,T26,T28,T30,T32,T34)</f>
+        <f t="shared" si="29"/>
         <v>2048000.0000000002</v>
       </c>
       <c r="U36" s="33">
-        <f>SUM(U18,U20,U22,U24,U26,U28,U30,U32,U34)</f>
+        <f t="shared" si="29"/>
         <v>4096000.0000000005</v>
       </c>
       <c r="V36" s="33">
-        <f>SUM(V18,V20,V22,V24,V26,V28,V30,V32,V34)</f>
+        <f t="shared" si="29"/>
         <v>8192000.0000000009</v>
       </c>
       <c r="W36" s="33">
-        <f>SUM(W18,W20,W22,W24,W26,W28,W30,W32,W34)</f>
+        <f t="shared" si="29"/>
         <v>16384000.000000002</v>
       </c>
       <c r="X36" s="47">
-        <f>SUM(X18,X20,X22,X24,X26,X28,X30,X32,X34)</f>
+        <f t="shared" si="29"/>
         <v>32768000.000000004</v>
       </c>
     </row>
@@ -13321,75 +13317,75 @@
       <c r="E37" s="63"/>
       <c r="F37" s="24"/>
       <c r="G37" s="45">
-        <f>SUM(G19,G21,G23,G25,G27,G29,G31,G33,G35)</f>
+        <f t="shared" ref="G37:X37" si="30">SUM(G19,G21,G23,G25,G27,G29,G31,G33,G35)</f>
         <v>4.6020179372197312</v>
       </c>
       <c r="H37" s="46">
-        <f>SUM(H19,H21,H23,H25,H27,H29,H31,H33,H35)</f>
+        <f t="shared" si="30"/>
         <v>9.2040358744394624</v>
       </c>
       <c r="I37" s="46">
-        <f>SUM(I19,I21,I23,I25,I27,I29,I31,I33,I35)</f>
+        <f t="shared" si="30"/>
         <v>18.408071748878925</v>
       </c>
       <c r="J37" s="46">
-        <f>SUM(J19,J21,J23,J25,J27,J29,J31,J33,J35)</f>
+        <f t="shared" si="30"/>
         <v>36.816143497757849</v>
       </c>
       <c r="K37" s="46">
-        <f>SUM(K19,K21,K23,K25,K27,K29,K31,K33,K35)</f>
+        <f t="shared" si="30"/>
         <v>73.632286995515699</v>
       </c>
       <c r="L37" s="46">
-        <f>SUM(L19,L21,L23,L25,L27,L29,L31,L33,L35)</f>
+        <f t="shared" si="30"/>
         <v>147.2645739910314</v>
       </c>
       <c r="M37" s="46">
-        <f>SUM(M19,M21,M23,M25,M27,M29,M31,M33,M35)</f>
+        <f t="shared" si="30"/>
         <v>294.5291479820628</v>
       </c>
       <c r="N37" s="46">
-        <f>SUM(N19,N21,N23,N25,N27,N29,N31,N33,N35)</f>
+        <f t="shared" si="30"/>
         <v>589.05829596412559</v>
       </c>
       <c r="O37" s="46">
-        <f>SUM(O19,O21,O23,O25,O27,O29,O31,O33,O35)</f>
+        <f t="shared" si="30"/>
         <v>1178.1165919282512</v>
       </c>
       <c r="P37" s="46">
-        <f>SUM(P19,P21,P23,P25,P27,P29,P31,P33,P35)</f>
+        <f t="shared" si="30"/>
         <v>2356.2331838565024</v>
       </c>
       <c r="Q37" s="46">
-        <f>SUM(Q19,Q21,Q23,Q25,Q27,Q29,Q31,Q33,Q35)</f>
+        <f t="shared" si="30"/>
         <v>4712.4663677130047</v>
       </c>
       <c r="R37" s="46">
-        <f>SUM(R19,R21,R23,R25,R27,R29,R31,R33,R35)</f>
+        <f t="shared" si="30"/>
         <v>9424.9327354260095</v>
       </c>
       <c r="S37" s="46">
-        <f>SUM(S19,S21,S23,S25,S27,S29,S31,S33,S35)</f>
+        <f t="shared" si="30"/>
         <v>18849.865470852019</v>
       </c>
       <c r="T37" s="46">
-        <f>SUM(T19,T21,T23,T25,T27,T29,T31,T33,T35)</f>
+        <f t="shared" si="30"/>
         <v>37699.730941704038</v>
       </c>
       <c r="U37" s="46">
-        <f>SUM(U19,U21,U23,U25,U27,U29,U31,U33,U35)</f>
+        <f t="shared" si="30"/>
         <v>75399.461883408076</v>
       </c>
       <c r="V37" s="46">
-        <f>SUM(V19,V21,V23,V25,V27,V29,V31,V33,V35)</f>
+        <f t="shared" si="30"/>
         <v>150798.92376681615</v>
       </c>
       <c r="W37" s="46">
-        <f>SUM(W19,W21,W23,W25,W27,W29,W31,W33,W35)</f>
+        <f t="shared" si="30"/>
         <v>301597.8475336323</v>
       </c>
       <c r="X37" s="49">
-        <f>SUM(X19,X21,X23,X25,X27,X29,X31,X33,X35)</f>
+        <f t="shared" si="30"/>
         <v>603195.69506726461</v>
       </c>
     </row>
@@ -13489,75 +13485,75 @@
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
       <c r="G41" s="32">
-        <f>G$8*$B$41</f>
+        <f t="shared" ref="G41:X41" si="31">G$8*$B$41</f>
         <v>12.5</v>
       </c>
       <c r="H41" s="33">
-        <f>H$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>25</v>
       </c>
       <c r="I41" s="33">
-        <f>I$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>50</v>
       </c>
       <c r="J41" s="33">
-        <f>J$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>100</v>
       </c>
       <c r="K41" s="33">
-        <f>K$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>200</v>
       </c>
       <c r="L41" s="33">
-        <f>L$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>400</v>
       </c>
       <c r="M41" s="33">
-        <f>M$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>800</v>
       </c>
       <c r="N41" s="33">
-        <f>N$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>1600</v>
       </c>
       <c r="O41" s="33">
-        <f>O$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>3200</v>
       </c>
       <c r="P41" s="33">
-        <f>P$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>6400</v>
       </c>
       <c r="Q41" s="33">
-        <f>Q$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>12800</v>
       </c>
       <c r="R41" s="33">
-        <f>R$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>25600</v>
       </c>
       <c r="S41" s="33">
-        <f>S$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>51200</v>
       </c>
       <c r="T41" s="33">
-        <f>T$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>102400</v>
       </c>
       <c r="U41" s="33">
-        <f>U$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>204800</v>
       </c>
       <c r="V41" s="33">
-        <f>V$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>409600</v>
       </c>
       <c r="W41" s="33">
-        <f>W$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>819200</v>
       </c>
       <c r="X41" s="47">
-        <f>X$8*$B$41</f>
+        <f t="shared" si="31"/>
         <v>1638400</v>
       </c>
     </row>
@@ -13575,71 +13571,71 @@
         <v>1.3125</v>
       </c>
       <c r="H42" s="44">
-        <f t="shared" ref="H42:X42" si="6">H41*$C$42</f>
+        <f t="shared" ref="H42:X42" si="32">H41*$C$42</f>
         <v>2.625</v>
       </c>
       <c r="I42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>5.25</v>
       </c>
       <c r="J42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>10.5</v>
       </c>
       <c r="K42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>21</v>
       </c>
       <c r="L42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>42</v>
       </c>
       <c r="M42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>84</v>
       </c>
       <c r="N42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>168</v>
       </c>
       <c r="O42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>336</v>
       </c>
       <c r="P42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>672</v>
       </c>
       <c r="Q42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>1344</v>
       </c>
       <c r="R42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>2688</v>
       </c>
       <c r="S42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>5376</v>
       </c>
       <c r="T42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>10752</v>
       </c>
       <c r="U42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>21504</v>
       </c>
       <c r="V42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>43008</v>
       </c>
       <c r="W42" s="44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>86016</v>
       </c>
       <c r="X42" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="32"/>
         <v>172032</v>
       </c>
     </row>
@@ -13655,75 +13651,75 @@
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
       <c r="G43" s="34">
-        <f>G$8*$B$43</f>
+        <f t="shared" ref="G43:X43" si="33">G$8*$B$43</f>
         <v>11.5</v>
       </c>
       <c r="H43" s="35">
-        <f>H$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>23</v>
       </c>
       <c r="I43" s="35">
-        <f>I$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>46</v>
       </c>
       <c r="J43" s="35">
-        <f>J$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>92</v>
       </c>
       <c r="K43" s="35">
-        <f>K$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>184</v>
       </c>
       <c r="L43" s="35">
-        <f>L$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>368</v>
       </c>
       <c r="M43" s="35">
-        <f>M$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>736</v>
       </c>
       <c r="N43" s="35">
-        <f>N$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>1472</v>
       </c>
       <c r="O43" s="35">
-        <f>O$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>2944</v>
       </c>
       <c r="P43" s="35">
-        <f>P$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>5888</v>
       </c>
       <c r="Q43" s="35">
-        <f>Q$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>11776</v>
       </c>
       <c r="R43" s="35">
-        <f>R$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>23552</v>
       </c>
       <c r="S43" s="35">
-        <f>S$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>47104</v>
       </c>
       <c r="T43" s="35">
-        <f>T$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>94208</v>
       </c>
       <c r="U43" s="35">
-        <f>U$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>188416</v>
       </c>
       <c r="V43" s="35">
-        <f>V$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>376832</v>
       </c>
       <c r="W43" s="35">
-        <f>W$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>753664</v>
       </c>
       <c r="X43" s="48">
-        <f>X$8*$B$43</f>
+        <f t="shared" si="33"/>
         <v>1507328</v>
       </c>
     </row>
@@ -13741,71 +13737,71 @@
         <v>0.83949999999999991</v>
       </c>
       <c r="H44" s="44">
-        <f t="shared" ref="H44:X44" si="7">H43*$C$44</f>
+        <f t="shared" ref="H44:X44" si="34">H43*$C$44</f>
         <v>1.6789999999999998</v>
       </c>
       <c r="I44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>3.3579999999999997</v>
       </c>
       <c r="J44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>6.7159999999999993</v>
       </c>
       <c r="K44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>13.431999999999999</v>
       </c>
       <c r="L44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>26.863999999999997</v>
       </c>
       <c r="M44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>53.727999999999994</v>
       </c>
       <c r="N44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>107.45599999999999</v>
       </c>
       <c r="O44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>214.91199999999998</v>
       </c>
       <c r="P44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>429.82399999999996</v>
       </c>
       <c r="Q44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>859.64799999999991</v>
       </c>
       <c r="R44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>1719.2959999999998</v>
       </c>
       <c r="S44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>3438.5919999999996</v>
       </c>
       <c r="T44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>6877.1839999999993</v>
       </c>
       <c r="U44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>13754.367999999999</v>
       </c>
       <c r="V44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>27508.735999999997</v>
       </c>
       <c r="W44" s="44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>55017.471999999994</v>
       </c>
       <c r="X44" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="34"/>
         <v>110034.94399999999</v>
       </c>
     </row>
@@ -13821,75 +13817,75 @@
       <c r="E45" s="30"/>
       <c r="F45" s="30"/>
       <c r="G45" s="34">
-        <f>G$8*$B$45</f>
+        <f t="shared" ref="G45:X45" si="35">G$8*$B$45</f>
         <v>77.5</v>
       </c>
       <c r="H45" s="35">
-        <f>H$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>155</v>
       </c>
       <c r="I45" s="35">
-        <f>I$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>310</v>
       </c>
       <c r="J45" s="35">
-        <f>J$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>620</v>
       </c>
       <c r="K45" s="35">
-        <f>K$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>1240</v>
       </c>
       <c r="L45" s="35">
-        <f>L$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>2480</v>
       </c>
       <c r="M45" s="35">
-        <f>M$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>4960</v>
       </c>
       <c r="N45" s="35">
-        <f>N$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>9920</v>
       </c>
       <c r="O45" s="35">
-        <f>O$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>19840</v>
       </c>
       <c r="P45" s="35">
-        <f>P$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>39680</v>
       </c>
       <c r="Q45" s="35">
-        <f>Q$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>79360</v>
       </c>
       <c r="R45" s="35">
-        <f>R$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>158720</v>
       </c>
       <c r="S45" s="35">
-        <f>S$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>317440</v>
       </c>
       <c r="T45" s="35">
-        <f>T$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>634880</v>
       </c>
       <c r="U45" s="35">
-        <f>U$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>1269760</v>
       </c>
       <c r="V45" s="35">
-        <f>V$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>2539520</v>
       </c>
       <c r="W45" s="35">
-        <f>W$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>5079040</v>
       </c>
       <c r="X45" s="48">
-        <f>X$8*$B$45</f>
+        <f t="shared" si="35"/>
         <v>10158080</v>
       </c>
     </row>
@@ -13907,71 +13903,71 @@
         <v>4.8825000000000003</v>
       </c>
       <c r="H46" s="44">
-        <f t="shared" ref="H46:X46" si="8">H45*$C$46</f>
+        <f t="shared" ref="H46:X46" si="36">H45*$C$46</f>
         <v>9.7650000000000006</v>
       </c>
       <c r="I46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>19.53</v>
       </c>
       <c r="J46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>39.06</v>
       </c>
       <c r="K46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>78.12</v>
       </c>
       <c r="L46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>156.24</v>
       </c>
       <c r="M46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>312.48</v>
       </c>
       <c r="N46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>624.96</v>
       </c>
       <c r="O46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>1249.92</v>
       </c>
       <c r="P46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>2499.84</v>
       </c>
       <c r="Q46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>4999.68</v>
       </c>
       <c r="R46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>9999.36</v>
       </c>
       <c r="S46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>19998.72</v>
       </c>
       <c r="T46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>39997.440000000002</v>
       </c>
       <c r="U46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>79994.880000000005</v>
       </c>
       <c r="V46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>159989.76000000001</v>
       </c>
       <c r="W46" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>319979.52000000002</v>
       </c>
       <c r="X46" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="36"/>
         <v>639959.04000000004</v>
       </c>
     </row>
@@ -13987,75 +13983,75 @@
       <c r="E47" s="30"/>
       <c r="F47" s="30"/>
       <c r="G47" s="34">
-        <f>G$8*$B$47</f>
+        <f t="shared" ref="G47:X47" si="37">G$8*$B$47</f>
         <v>84.25</v>
       </c>
       <c r="H47" s="35">
-        <f>H$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>168.5</v>
       </c>
       <c r="I47" s="35">
-        <f>I$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>337</v>
       </c>
       <c r="J47" s="35">
-        <f>J$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>674</v>
       </c>
       <c r="K47" s="35">
-        <f>K$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>1348</v>
       </c>
       <c r="L47" s="35">
-        <f>L$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>2696</v>
       </c>
       <c r="M47" s="35">
-        <f>M$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>5392</v>
       </c>
       <c r="N47" s="35">
-        <f>N$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>10784</v>
       </c>
       <c r="O47" s="35">
-        <f>O$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>21568</v>
       </c>
       <c r="P47" s="35">
-        <f>P$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>43136</v>
       </c>
       <c r="Q47" s="35">
-        <f>Q$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>86272</v>
       </c>
       <c r="R47" s="35">
-        <f>R$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>172544</v>
       </c>
       <c r="S47" s="35">
-        <f>S$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>345088</v>
       </c>
       <c r="T47" s="35">
-        <f>T$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>690176</v>
       </c>
       <c r="U47" s="35">
-        <f>U$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>1380352</v>
       </c>
       <c r="V47" s="35">
-        <f>V$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>2760704</v>
       </c>
       <c r="W47" s="35">
-        <f>W$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>5521408</v>
       </c>
       <c r="X47" s="48">
-        <f>X$8*$B$47</f>
+        <f t="shared" si="37"/>
         <v>11042816</v>
       </c>
     </row>
@@ -14073,71 +14069,71 @@
         <v>5.0549999999999997</v>
       </c>
       <c r="H48" s="44">
-        <f t="shared" ref="H48:X48" si="9">H47*$C$48</f>
+        <f t="shared" ref="H48:X48" si="38">H47*$C$48</f>
         <v>10.11</v>
       </c>
       <c r="I48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>20.22</v>
       </c>
       <c r="J48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>40.44</v>
       </c>
       <c r="K48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>80.88</v>
       </c>
       <c r="L48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>161.76</v>
       </c>
       <c r="M48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>323.52</v>
       </c>
       <c r="N48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>647.04</v>
       </c>
       <c r="O48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>1294.08</v>
       </c>
       <c r="P48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>2588.16</v>
       </c>
       <c r="Q48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>5176.32</v>
       </c>
       <c r="R48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>10352.64</v>
       </c>
       <c r="S48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>20705.28</v>
       </c>
       <c r="T48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>41410.559999999998</v>
       </c>
       <c r="U48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>82821.119999999995</v>
       </c>
       <c r="V48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>165642.23999999999</v>
       </c>
       <c r="W48" s="44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>331284.47999999998</v>
       </c>
       <c r="X48" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="38"/>
         <v>662568.95999999996</v>
       </c>
     </row>
@@ -14153,75 +14149,75 @@
       <c r="E49" s="30"/>
       <c r="F49" s="30"/>
       <c r="G49" s="34">
-        <f>G$8*$B$49</f>
+        <f t="shared" ref="G49:X49" si="39">G$8*$B$49</f>
         <v>3.75</v>
       </c>
       <c r="H49" s="35">
-        <f>H$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>7.5</v>
       </c>
       <c r="I49" s="35">
-        <f>I$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>15</v>
       </c>
       <c r="J49" s="35">
-        <f>J$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>30</v>
       </c>
       <c r="K49" s="35">
-        <f>K$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>60</v>
       </c>
       <c r="L49" s="35">
-        <f>L$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>120</v>
       </c>
       <c r="M49" s="35">
-        <f>M$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>240</v>
       </c>
       <c r="N49" s="35">
-        <f>N$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>480</v>
       </c>
       <c r="O49" s="35">
-        <f>O$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>960</v>
       </c>
       <c r="P49" s="35">
-        <f>P$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>1920</v>
       </c>
       <c r="Q49" s="35">
-        <f>Q$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>3840</v>
       </c>
       <c r="R49" s="35">
-        <f>R$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>7680</v>
       </c>
       <c r="S49" s="35">
-        <f>S$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>15360</v>
       </c>
       <c r="T49" s="35">
-        <f>T$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>30720</v>
       </c>
       <c r="U49" s="35">
-        <f>U$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>61440</v>
       </c>
       <c r="V49" s="35">
-        <f>V$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>122880</v>
       </c>
       <c r="W49" s="35">
-        <f>W$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>245760</v>
       </c>
       <c r="X49" s="48">
-        <f>X$8*$B$49</f>
+        <f t="shared" si="39"/>
         <v>491520</v>
       </c>
     </row>
@@ -14239,71 +14235,71 @@
         <v>0.21</v>
       </c>
       <c r="H50" s="44">
-        <f t="shared" ref="H50:X50" si="10">H49*$C$50</f>
+        <f t="shared" ref="H50:X50" si="40">H49*$C$50</f>
         <v>0.42</v>
       </c>
       <c r="I50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>0.84</v>
       </c>
       <c r="J50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>1.68</v>
       </c>
       <c r="K50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>3.36</v>
       </c>
       <c r="L50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>6.72</v>
       </c>
       <c r="M50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>13.44</v>
       </c>
       <c r="N50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>26.88</v>
       </c>
       <c r="O50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>53.76</v>
       </c>
       <c r="P50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>107.52</v>
       </c>
       <c r="Q50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>215.04</v>
       </c>
       <c r="R50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>430.08</v>
       </c>
       <c r="S50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>860.16</v>
       </c>
       <c r="T50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>1720.32</v>
       </c>
       <c r="U50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>3440.64</v>
       </c>
       <c r="V50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>6881.28</v>
       </c>
       <c r="W50" s="44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>13762.56</v>
       </c>
       <c r="X50" s="48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="40"/>
         <v>27525.119999999999</v>
       </c>
     </row>
@@ -14319,75 +14315,75 @@
       <c r="E51" s="30"/>
       <c r="F51" s="30"/>
       <c r="G51" s="34">
-        <f>G$8*$B$51</f>
+        <f t="shared" ref="G51:X51" si="41">G$8*$B$51</f>
         <v>40.25</v>
       </c>
       <c r="H51" s="35">
-        <f>H$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>80.5</v>
       </c>
       <c r="I51" s="35">
-        <f>I$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>161</v>
       </c>
       <c r="J51" s="35">
-        <f>J$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>322</v>
       </c>
       <c r="K51" s="35">
-        <f>K$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>644</v>
       </c>
       <c r="L51" s="35">
-        <f>L$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>1288</v>
       </c>
       <c r="M51" s="35">
-        <f>M$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>2576</v>
       </c>
       <c r="N51" s="35">
-        <f>N$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>5152</v>
       </c>
       <c r="O51" s="35">
-        <f>O$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>10304</v>
       </c>
       <c r="P51" s="35">
-        <f>P$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>20608</v>
       </c>
       <c r="Q51" s="35">
-        <f>Q$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>41216</v>
       </c>
       <c r="R51" s="35">
-        <f>R$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>82432</v>
       </c>
       <c r="S51" s="35">
-        <f>S$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>164864</v>
       </c>
       <c r="T51" s="35">
-        <f>T$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>329728</v>
       </c>
       <c r="U51" s="35">
-        <f>U$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>659456</v>
       </c>
       <c r="V51" s="35">
-        <f>V$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>1318912</v>
       </c>
       <c r="W51" s="35">
-        <f>W$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>2637824</v>
       </c>
       <c r="X51" s="48">
-        <f>X$8*$B$51</f>
+        <f t="shared" si="41"/>
         <v>5275648</v>
       </c>
     </row>
@@ -14467,71 +14463,71 @@
         <v>229.75</v>
       </c>
       <c r="H53" s="33">
-        <f t="shared" ref="H53:X53" si="11">SUM(H41,H43,H45,H47,H49,H51)</f>
+        <f t="shared" ref="H53:X53" si="42">SUM(H41,H43,H45,H47,H49,H51)</f>
         <v>459.5</v>
       </c>
       <c r="I53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>919</v>
       </c>
       <c r="J53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>1838</v>
       </c>
       <c r="K53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>3676</v>
       </c>
       <c r="L53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>7352</v>
       </c>
       <c r="M53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>14704</v>
       </c>
       <c r="N53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>29408</v>
       </c>
       <c r="O53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>58816</v>
       </c>
       <c r="P53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>117632</v>
       </c>
       <c r="Q53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>235264</v>
       </c>
       <c r="R53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>470528</v>
       </c>
       <c r="S53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>941056</v>
       </c>
       <c r="T53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>1882112</v>
       </c>
       <c r="U53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>3764224</v>
       </c>
       <c r="V53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>7528448</v>
       </c>
       <c r="W53" s="33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>15056896</v>
       </c>
       <c r="X53" s="47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="42"/>
         <v>30113792</v>
       </c>
     </row>
@@ -14549,71 +14545,71 @@
         <v>12.299500000000002</v>
       </c>
       <c r="H54" s="46">
-        <f t="shared" ref="H54:X54" si="12">SUM(H42,H44,H46,H48,H50,H52)</f>
+        <f t="shared" ref="H54:X54" si="43">SUM(H42,H44,H46,H48,H50,H52)</f>
         <v>24.599000000000004</v>
       </c>
       <c r="I54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>49.198000000000008</v>
       </c>
       <c r="J54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>98.396000000000015</v>
       </c>
       <c r="K54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>196.79200000000003</v>
       </c>
       <c r="L54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>393.58400000000006</v>
       </c>
       <c r="M54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>787.16800000000012</v>
       </c>
       <c r="N54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>1574.3360000000002</v>
       </c>
       <c r="O54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>3148.6720000000005</v>
       </c>
       <c r="P54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>6297.344000000001</v>
       </c>
       <c r="Q54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>12594.688000000002</v>
       </c>
       <c r="R54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>25189.376000000004</v>
       </c>
       <c r="S54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>50378.752000000008</v>
       </c>
       <c r="T54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>100757.50400000002</v>
       </c>
       <c r="U54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>201515.00800000003</v>
       </c>
       <c r="V54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>403030.01600000006</v>
       </c>
       <c r="W54" s="46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>806060.03200000012</v>
       </c>
       <c r="X54" s="49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="43"/>
         <v>1612120.0640000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with latest AU population stats from the ABS
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13215F4D-211D-45C3-9606-1982CA724F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A5BFB5-6486-492C-AC2D-96D12C2B9AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="165">
   <si>
     <t>Australian Population</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>0-9</t>
-  </si>
-  <si>
-    <t>Pop. 2018</t>
   </si>
   <si>
     <t>0</t>
@@ -433,9 +430,6 @@
     <t>Ages</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
     <t>Total Mortality Count</t>
   </si>
   <si>
@@ -523,20 +517,33 @@
     <t>N.B. the mortality numbers do not model the lag from infection to recovery/death, the mortality count as estimated for the population will be in advance of actuals, so actuals will appear as a lower number for a given week.</t>
   </si>
   <si>
-    <t>Assumes that infection period lasts for 6 weeks, for many younger people it can be over within 2 weeks, for older people and those requiring hospitalisation, it can be in excess of 6 weeks</t>
+    <t>as of 19/3/2020</t>
+  </si>
+  <si>
+    <t>Pop. Sep 2019</t>
+  </si>
+  <si>
+    <t>Population estimated as at 30 June 2019</t>
+  </si>
+  <si>
+    <t>Assumes that infection period lasts for 6 weeks, for many people it can be over within 2 weeks, for others including those requiring hospitalisation, it can be in excess of 6 weeks</t>
+  </si>
+  <si>
+    <t>Infection counts are detected infection counts, total population infection counts will be greater, but without whole population testing or some form of random sampling testing, total population infection numbers remains unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="172" formatCode="[$$-C09]#,##0.00;[Red]&quot;-&quot;[$$-C09]#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +586,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -821,11 +851,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -950,7 +989,6 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -977,10 +1015,25 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="9" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
+    <cellStyle name="Heading" xfId="3" xr:uid="{DB9EF5E1-A693-41C3-82C7-CA90563DBB00}"/>
+    <cellStyle name="Heading1" xfId="4" xr:uid="{33778C9B-2759-42CE-8B12-70EF179014AB}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{F4FF767F-813C-4942-8E90-D60D18A1396E}"/>
+    <cellStyle name="Result" xfId="5" xr:uid="{92363E1D-B163-4931-AE8B-9DBC97E2614C}"/>
+    <cellStyle name="Result2" xfId="6" xr:uid="{346AB93D-4A1D-4E1B-B53F-62B068519100}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -26971,7 +27024,7 @@
   <dimension ref="A1:AD62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26996,55 +27049,61 @@
       <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100">
-        <v>25632684</v>
+      <c r="B1" s="126">
+        <v>25632150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" s="94">
         <v>2.6</v>
       </c>
       <c r="C2" s="95">
         <f>(B1/1000)*B2</f>
-        <v>66644.978400000007</v>
+        <v>66643.590000000011</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="96">
         <v>7.4</v>
       </c>
       <c r="C3" s="91">
         <f>(B1/100000)*B3</f>
-        <v>1896.818616</v>
+        <v>1896.7791000000002</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4" s="97">
         <v>0.15</v>
       </c>
       <c r="C4" s="2"/>
+      <c r="G4" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B5" s="98">
         <v>0.05</v>
@@ -27053,7 +27112,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B6" s="99">
         <v>0.02</v>
@@ -27092,7 +27151,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="81" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="30"/>
@@ -27110,7 +27169,7 @@
       <c r="O9" s="30"/>
       <c r="P9" s="30"/>
       <c r="Q9" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R9" s="30"/>
       <c r="S9" s="30"/>
@@ -27131,22 +27190,22 @@
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="101">
+      <c r="G10" s="100">
         <v>43892</v>
       </c>
-      <c r="H10" s="101">
+      <c r="H10" s="100">
         <f t="shared" ref="H10:X10" si="0">G10+$B$10</f>
         <v>43896</v>
       </c>
-      <c r="I10" s="101">
+      <c r="I10" s="100">
         <f t="shared" si="0"/>
         <v>43900</v>
       </c>
-      <c r="J10" s="101">
+      <c r="J10" s="100">
         <f t="shared" si="0"/>
         <v>43904</v>
       </c>
-      <c r="K10" s="101">
+      <c r="K10" s="100">
         <f t="shared" si="0"/>
         <v>43908</v>
       </c>
@@ -27170,57 +27229,57 @@
         <f t="shared" si="0"/>
         <v>43928</v>
       </c>
-      <c r="Q10" s="114">
+      <c r="Q10" s="113">
         <f t="shared" si="0"/>
         <v>43932</v>
       </c>
-      <c r="R10" s="115">
+      <c r="R10" s="114">
         <f t="shared" si="0"/>
         <v>43936</v>
       </c>
-      <c r="S10" s="116">
+      <c r="S10" s="115">
         <f t="shared" si="0"/>
         <v>43940</v>
       </c>
-      <c r="T10" s="116">
+      <c r="T10" s="115">
         <f t="shared" si="0"/>
         <v>43944</v>
       </c>
-      <c r="U10" s="116">
+      <c r="U10" s="115">
         <f t="shared" si="0"/>
         <v>43948</v>
       </c>
-      <c r="V10" s="116">
+      <c r="V10" s="115">
         <f t="shared" si="0"/>
         <v>43952</v>
       </c>
-      <c r="W10" s="116">
+      <c r="W10" s="115">
         <f t="shared" si="0"/>
         <v>43956</v>
       </c>
-      <c r="X10" s="117">
+      <c r="X10" s="116">
         <f t="shared" si="0"/>
         <v>43960</v>
       </c>
-      <c r="Y10" s="117">
+      <c r="Y10" s="116">
         <f t="shared" ref="Y10" si="1">X10+$B$10</f>
         <v>43964</v>
       </c>
-      <c r="Z10" s="117">
+      <c r="Z10" s="116">
         <f t="shared" ref="Z10" si="2">Y10+$B$10</f>
         <v>43968</v>
       </c>
-      <c r="AA10" s="119">
+      <c r="AA10" s="118">
         <f t="shared" ref="AA10" si="3">Z10+$B$10</f>
         <v>43972</v>
       </c>
-      <c r="AB10" s="113"/>
-      <c r="AC10" s="113"/>
-      <c r="AD10" s="111"/>
+      <c r="AB10" s="112"/>
+      <c r="AC10" s="112"/>
+      <c r="AD10" s="110"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
@@ -27308,11 +27367,11 @@
       </c>
       <c r="AA11" s="47">
         <f>B1</f>
-        <v>25632684</v>
+        <v>25632150</v>
       </c>
       <c r="AB11" s="64"/>
       <c r="AC11" s="64"/>
-      <c r="AD11" s="111"/>
+      <c r="AD11" s="110"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
@@ -27323,97 +27382,97 @@
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
-      <c r="G12" s="103">
+      <c r="G12" s="102">
         <f t="shared" ref="G12:W12" si="8">G11/$B$1</f>
-        <v>1.2191466176542418E-6</v>
-      </c>
-      <c r="H12" s="104">
+        <v>1.2191720163934746E-6</v>
+      </c>
+      <c r="H12" s="103">
         <f t="shared" si="8"/>
-        <v>2.4382932353084836E-6</v>
-      </c>
-      <c r="I12" s="104">
+        <v>2.4383440327869492E-6</v>
+      </c>
+      <c r="I12" s="103">
         <f t="shared" si="8"/>
-        <v>4.8765864706169672E-6</v>
+        <v>4.8766880655738983E-6</v>
       </c>
       <c r="J12" s="51">
         <f t="shared" si="8"/>
-        <v>9.7531729412339345E-6</v>
+        <v>9.7533761311477967E-6</v>
       </c>
       <c r="K12" s="51">
         <f t="shared" si="8"/>
-        <v>1.9506345882467869E-5</v>
+        <v>1.9506752262295593E-5</v>
       </c>
       <c r="L12" s="51">
         <f t="shared" si="8"/>
-        <v>3.9012691764935738E-5</v>
+        <v>3.9013504524591187E-5</v>
       </c>
       <c r="M12" s="51">
         <f t="shared" si="8"/>
-        <v>7.8025383529871476E-5</v>
+        <v>7.8027009049182373E-5</v>
       </c>
       <c r="N12" s="51">
         <f t="shared" si="8"/>
-        <v>1.5605076705974295E-4</v>
+        <v>1.5605401809836475E-4</v>
       </c>
       <c r="O12" s="28">
         <f t="shared" si="8"/>
-        <v>3.121015341194859E-4</v>
+        <v>3.1210803619672949E-4</v>
       </c>
       <c r="P12" s="28">
         <f t="shared" si="8"/>
-        <v>6.2420306823897181E-4</v>
+        <v>6.2421607239345899E-4</v>
       </c>
       <c r="Q12" s="53">
         <f t="shared" si="8"/>
-        <v>1.2484061364779436E-3</v>
+        <v>1.248432144786918E-3</v>
       </c>
       <c r="R12" s="20">
         <f t="shared" si="8"/>
-        <v>2.4968122729558872E-3</v>
+        <v>2.4968642895738359E-3</v>
       </c>
       <c r="S12" s="29">
         <f t="shared" si="8"/>
-        <v>4.9936245459117744E-3</v>
-      </c>
-      <c r="T12" s="125">
+        <v>4.9937285791476719E-3</v>
+      </c>
+      <c r="T12" s="124">
         <f t="shared" si="8"/>
-        <v>9.9872490918235489E-3</v>
-      </c>
-      <c r="U12" s="125">
+        <v>9.9874571582953438E-3</v>
+      </c>
+      <c r="U12" s="124">
         <f t="shared" si="8"/>
-        <v>1.9974498183647098E-2</v>
-      </c>
-      <c r="V12" s="125">
+        <v>1.9974914316590688E-2</v>
+      </c>
+      <c r="V12" s="124">
         <f t="shared" si="8"/>
-        <v>3.9948996367294196E-2</v>
-      </c>
-      <c r="W12" s="125">
+        <v>3.9949828633181375E-2</v>
+      </c>
+      <c r="W12" s="124">
         <f t="shared" si="8"/>
-        <v>7.9897992734588391E-2</v>
-      </c>
-      <c r="X12" s="125">
+        <v>7.989965726636275E-2</v>
+      </c>
+      <c r="X12" s="124">
         <f t="shared" ref="X12:AA12" si="9">X11/$B$1</f>
-        <v>0.15979598546917678</v>
-      </c>
-      <c r="Y12" s="125">
+        <v>0.1597993145327255</v>
+      </c>
+      <c r="Y12" s="124">
         <f t="shared" si="9"/>
-        <v>0.31959197093835356</v>
-      </c>
-      <c r="Z12" s="125">
+        <v>0.319598629065451</v>
+      </c>
+      <c r="Z12" s="124">
         <f t="shared" si="9"/>
-        <v>0.63918394187670713</v>
-      </c>
-      <c r="AA12" s="126">
+        <v>0.639197258130902</v>
+      </c>
+      <c r="AA12" s="125">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AB12" s="39"/>
       <c r="AC12" s="39"/>
-      <c r="AD12" s="111"/>
+      <c r="AD12" s="110"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -27502,15 +27561,15 @@
       </c>
       <c r="AA13" s="48">
         <f>AA11-Q11-AA18</f>
-        <v>25088030.32</v>
+        <v>25087507</v>
       </c>
       <c r="AB13" s="64"/>
       <c r="AC13" s="64"/>
-      <c r="AD13" s="111"/>
+      <c r="AD13" s="110"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="92" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
@@ -27599,15 +27658,15 @@
       </c>
       <c r="AA14" s="47">
         <f t="shared" si="13"/>
-        <v>3844902.5999999996</v>
+        <v>3844822.5</v>
       </c>
       <c r="AB14" s="64"/>
       <c r="AC14" s="64"/>
-      <c r="AD14" s="111"/>
+      <c r="AD14" s="110"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B15" s="56"/>
       <c r="C15" s="57"/>
@@ -27658,7 +27717,7 @@
         <f t="shared" si="14"/>
         <v>4800</v>
       </c>
-      <c r="R15" s="124">
+      <c r="R15" s="123">
         <f>R14-G14</f>
         <v>9595.3125</v>
       </c>
@@ -27696,15 +27755,15 @@
       </c>
       <c r="AA15" s="48">
         <f t="shared" si="16"/>
-        <v>3842502.5999999996</v>
+        <v>3842422.5</v>
       </c>
       <c r="AB15" s="64"/>
       <c r="AC15" s="64"/>
-      <c r="AD15" s="111"/>
+      <c r="AD15" s="110"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -27792,15 +27851,15 @@
       </c>
       <c r="AA16" s="47">
         <f t="shared" si="18"/>
-        <v>1281634.2000000002</v>
+        <v>1281607.5</v>
       </c>
       <c r="AB16" s="64"/>
       <c r="AC16" s="64"/>
-      <c r="AD16" s="111"/>
+      <c r="AD16" s="110"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="57"/>
@@ -27839,7 +27898,7 @@
         <f t="shared" si="19"/>
         <v>120</v>
       </c>
-      <c r="O17" s="112">
+      <c r="O17" s="111">
         <f t="shared" si="19"/>
         <v>240</v>
       </c>
@@ -27851,7 +27910,7 @@
         <f t="shared" si="19"/>
         <v>960</v>
       </c>
-      <c r="R17" s="118">
+      <c r="R17" s="117">
         <f t="shared" ref="R17:W17" si="20">R16-R18-G17</f>
         <v>1919.0625</v>
       </c>
@@ -27889,15 +27948,15 @@
       </c>
       <c r="AA17" s="48">
         <f t="shared" si="21"/>
-        <v>768500.52000000025</v>
+        <v>768484.5</v>
       </c>
       <c r="AB17" s="64"/>
       <c r="AC17" s="64"/>
-      <c r="AD17" s="111"/>
+      <c r="AD17" s="110"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" s="74"/>
       <c r="C18" s="75"/>
@@ -27944,7 +28003,7 @@
         <f t="shared" si="22"/>
         <v>320</v>
       </c>
-      <c r="Q18" s="102">
+      <c r="Q18" s="101">
         <f t="shared" si="22"/>
         <v>640</v>
       </c>
@@ -27986,15 +28045,15 @@
       </c>
       <c r="AA18" s="78">
         <f t="shared" si="23"/>
-        <v>512653.68</v>
+        <v>512643</v>
       </c>
       <c r="AB18" s="64"/>
       <c r="AC18" s="64"/>
-      <c r="AD18" s="111"/>
+      <c r="AD18" s="110"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="81" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="30"/>
@@ -28022,58 +28081,58 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="105">
+      <c r="G21" s="104">
         <v>32</v>
       </c>
-      <c r="H21" s="106">
+      <c r="H21" s="105">
         <v>63</v>
       </c>
-      <c r="I21" s="107">
+      <c r="I21" s="106">
         <v>112</v>
       </c>
-      <c r="J21" s="107">
+      <c r="J21" s="106">
         <v>249</v>
       </c>
-      <c r="K21" s="107">
+      <c r="K21" s="106">
         <v>567</v>
       </c>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
-      <c r="S21" s="107"/>
-      <c r="T21" s="107"/>
-      <c r="U21" s="107"/>
-      <c r="V21" s="107"/>
-      <c r="W21" s="107"/>
-      <c r="X21" s="107"/>
-      <c r="Y21" s="107"/>
-      <c r="Z21" s="107"/>
-      <c r="AA21" s="108"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="106"/>
+      <c r="Q21" s="106"/>
+      <c r="R21" s="106"/>
+      <c r="S21" s="106"/>
+      <c r="T21" s="106"/>
+      <c r="U21" s="106"/>
+      <c r="V21" s="106"/>
+      <c r="W21" s="106"/>
+      <c r="X21" s="106"/>
+      <c r="Y21" s="106"/>
+      <c r="Z21" s="106"/>
+      <c r="AA21" s="107"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B22" s="56"/>
       <c r="C22" s="57"/>
       <c r="D22" s="57"/>
       <c r="E22" s="57"/>
       <c r="F22" s="57"/>
-      <c r="G22" s="109">
+      <c r="G22" s="108">
         <v>1</v>
       </c>
-      <c r="H22" s="110">
+      <c r="H22" s="109">
         <v>2</v>
       </c>
       <c r="I22" s="79">
@@ -28124,8 +28183,8 @@
       <c r="X23" s="49"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="123" t="s">
-        <v>151</v>
+      <c r="A24" s="122" t="s">
+        <v>149</v>
       </c>
       <c r="X24" s="30"/>
     </row>
@@ -28133,14 +28192,14 @@
       <c r="A25" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>23</v>
+      <c r="B25" s="87" t="s">
+        <v>161</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="87" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E25" s="88" t="s">
         <v>3</v>
@@ -28175,11 +28234,12 @@
         <v>14</v>
       </c>
       <c r="B26" s="27">
-        <v>3.9583530803410746E-2</v>
+        <f>'ABS Population by Age Range'!D107</f>
+        <v>4.0260989985204748E-2</v>
       </c>
       <c r="C26" s="26">
         <f>$B$1*B26</f>
-        <v>1014632.1366880938</v>
+        <v>1031975.7344492659</v>
       </c>
       <c r="D26" s="36">
         <f>'AU Infection Rate by Age'!C4</f>
@@ -28188,11 +28248,11 @@
       <c r="E26" s="17"/>
       <c r="F26" s="30"/>
       <c r="G26" s="32">
-        <f t="shared" ref="G26:W26" si="24">G$11*$D$26</f>
+        <f>G$11*$D$26</f>
         <v>0.84046454767726153</v>
       </c>
       <c r="H26" s="33">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="G26:W26" si="24">H$11*$D$26</f>
         <v>1.6809290953545231</v>
       </c>
       <c r="I26" s="33">
@@ -28269,7 +28329,7 @@
       </c>
       <c r="AA26" s="90">
         <f t="shared" si="25"/>
-        <v>689387.5892420538</v>
+        <v>689373.22738386306</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -28282,14 +28342,14 @@
       </c>
       <c r="F27" s="22">
         <f>$B$1*D26*E27</f>
-        <v>102029.36320782396</v>
+        <v>102027.23765281173</v>
       </c>
       <c r="G27" s="43">
-        <f t="shared" ref="G27:W27" si="26">G$11*$D$26*$E$27</f>
+        <f>G$11*$D$26*$E$27</f>
         <v>0.1243887530562347</v>
       </c>
       <c r="H27" s="44">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="G27:W27" si="26">H$11*$D$26*$E$27</f>
         <v>0.2487775061124694</v>
       </c>
       <c r="I27" s="44">
@@ -28364,9 +28424,9 @@
         <f t="shared" si="27"/>
         <v>65215.53056234718</v>
       </c>
-      <c r="AA27" s="120">
+      <c r="AA27" s="119">
         <f t="shared" si="27"/>
-        <v>102029.36320782396</v>
+        <v>102027.23765281173</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
@@ -28374,11 +28434,12 @@
         <v>15</v>
       </c>
       <c r="B28" s="18">
-        <v>6.8733756751875541E-2</v>
+        <f>'ABS Population by Age Range'!D97</f>
+        <v>7.065336711718416E-2</v>
       </c>
       <c r="C28" s="22">
         <f t="shared" ref="C28:C42" si="28">$B$1*B28</f>
-        <v>1761830.6669536922</v>
+        <v>1810997.703952732</v>
       </c>
       <c r="D28" s="37">
         <f>'AU Infection Rate by Age'!C5</f>
@@ -28466,9 +28527,9 @@
         <f t="shared" si="30"/>
         <v>841232.27383863076</v>
       </c>
-      <c r="AA28" s="121">
+      <c r="AA28" s="120">
         <f t="shared" si="30"/>
-        <v>1316103.5794621026</v>
+        <v>1316076.1613691931</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -28481,7 +28542,7 @@
       </c>
       <c r="F29" s="22">
         <f>$B$1*D28*E29</f>
-        <v>105288.28635696821</v>
+        <v>105286.09290953545</v>
       </c>
       <c r="G29" s="43">
         <f t="shared" ref="G29:W29" si="31">G$11*$D$28*$E$29</f>
@@ -28563,9 +28624,9 @@
         <f t="shared" si="32"/>
         <v>67298.581907090469</v>
       </c>
-      <c r="AA29" s="120">
+      <c r="AA29" s="119">
         <f t="shared" si="32"/>
-        <v>105288.28635696821</v>
+        <v>105286.09290953545</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
@@ -28573,11 +28634,12 @@
         <v>16</v>
       </c>
       <c r="B30" s="18">
-        <v>0.10271036487346757</v>
+        <f>'ABS Population by Age Range'!D85</f>
+        <v>0.10301766910746854</v>
       </c>
       <c r="C30" s="22">
         <f t="shared" si="28"/>
-        <v>2632742.3263262943</v>
+        <v>2640564.3472129996</v>
       </c>
       <c r="D30" s="37">
         <f>'AU Infection Rate by Age'!C6</f>
@@ -28665,9 +28727,9 @@
         <f t="shared" si="34"/>
         <v>2603814.1809290955</v>
       </c>
-      <c r="AA30" s="121">
+      <c r="AA30" s="120">
         <f t="shared" si="34"/>
-        <v>4073653.9364303183</v>
+        <v>4073569.0709046456</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
@@ -28680,7 +28742,7 @@
       </c>
       <c r="F31" s="22">
         <f>$B$1*D30*E31</f>
-        <v>146651.54171149145</v>
+        <v>146648.48655256722</v>
       </c>
       <c r="G31" s="43">
         <f t="shared" ref="G31:W31" si="35">G$11*$D$30*$E$31</f>
@@ -28762,9 +28824,9 @@
         <f t="shared" si="36"/>
         <v>93737.310513447432</v>
       </c>
-      <c r="AA31" s="120">
+      <c r="AA31" s="119">
         <f t="shared" si="36"/>
-        <v>146651.54171149145</v>
+        <v>146648.48655256722</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -28772,11 +28834,12 @@
         <v>17</v>
       </c>
       <c r="B32" s="18">
-        <v>0.12241761174778311</v>
+        <f>'ABS Population by Age Range'!D73</f>
+        <v>0.12142789925761971</v>
       </c>
       <c r="C32" s="22">
         <f t="shared" si="28"/>
-        <v>3137891.9579656119</v>
+        <v>3112458.1279561971</v>
       </c>
       <c r="D32" s="37">
         <f>'AU Infection Rate by Age'!C7</f>
@@ -28864,9 +28927,9 @@
         <f t="shared" si="38"/>
         <v>3004400.9779951102</v>
       </c>
-      <c r="AA32" s="121">
+      <c r="AA32" s="120">
         <f t="shared" si="38"/>
-        <v>4700369.9266503667</v>
+        <v>4700272.0048899762</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
@@ -28879,7 +28942,7 @@
       </c>
       <c r="F33" s="22">
         <f>$B$1*D32*E33</f>
-        <v>61104.809046454764</v>
+        <v>61103.536063569685</v>
       </c>
       <c r="G33" s="43">
         <f t="shared" ref="G33:W33" si="39">G$11*$D$32*$E$33</f>
@@ -28961,9 +29024,9 @@
         <f t="shared" si="40"/>
         <v>39057.212713936431</v>
       </c>
-      <c r="AA33" s="120">
+      <c r="AA33" s="119">
         <f t="shared" si="40"/>
-        <v>61104.809046454764</v>
+        <v>61103.536063569685</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
@@ -28971,11 +29034,12 @@
         <v>18</v>
       </c>
       <c r="B34" s="18">
-        <v>0.1307371328497558</v>
+        <f>'ABS Population by Age Range'!D61</f>
+        <v>0.12908272398046944</v>
       </c>
       <c r="C34" s="22">
         <f t="shared" si="28"/>
-        <v>3351143.6134038097</v>
+        <v>3308667.7434759899</v>
       </c>
       <c r="D34" s="37">
         <f>'AU Infection Rate by Age'!C8</f>
@@ -29063,9 +29127,9 @@
         <f t="shared" si="42"/>
         <v>2884224.9388753059</v>
       </c>
-      <c r="AA34" s="121">
+      <c r="AA34" s="120">
         <f t="shared" si="42"/>
-        <v>4512355.1295843525</v>
+        <v>4512261.1246943763</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
@@ -29078,7 +29142,7 @@
       </c>
       <c r="F35" s="22">
         <f>$B$1*D34*E35</f>
-        <v>18049.420518337411</v>
+        <v>18049.044498777504</v>
       </c>
       <c r="G35" s="43">
         <f>G$11*$D$34*$E$35</f>
@@ -29160,9 +29224,9 @@
         <f t="shared" si="44"/>
         <v>11536.899755501225</v>
       </c>
-      <c r="AA35" s="120">
+      <c r="AA35" s="119">
         <f t="shared" si="44"/>
-        <v>18049.420518337411</v>
+        <v>18049.044498777504</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -29170,11 +29234,12 @@
         <v>19</v>
       </c>
       <c r="B36" s="18">
-        <v>0.14352807031813389</v>
+        <f>'ABS Population by Age Range'!D49</f>
+        <v>0.14481341657950456</v>
       </c>
       <c r="C36" s="22">
         <f t="shared" si="28"/>
-        <v>3679009.6715945052</v>
+        <v>3711879.2157783476</v>
       </c>
       <c r="D36" s="37">
         <f>'AU Infection Rate by Age'!C9</f>
@@ -29262,9 +29327,9 @@
         <f t="shared" si="46"/>
         <v>3404987.7750611249</v>
       </c>
-      <c r="AA36" s="121">
+      <c r="AA36" s="120">
         <f t="shared" si="46"/>
-        <v>5327085.9168704161</v>
+        <v>5326974.9388753064</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -29277,7 +29342,7 @@
       </c>
       <c r="F37" s="22">
         <f>$B$1*D36*E37</f>
-        <v>10654.171833740833</v>
+        <v>10653.949877750612</v>
       </c>
       <c r="G37" s="43">
         <f t="shared" ref="G37:W37" si="47">G$11*$D$36*$E$37</f>
@@ -29359,9 +29424,9 @@
         <f t="shared" si="48"/>
         <v>6809.9755501222498</v>
       </c>
-      <c r="AA37" s="120">
+      <c r="AA37" s="119">
         <f t="shared" si="48"/>
-        <v>10654.171833740833</v>
+        <v>10653.949877750612</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
@@ -29369,11 +29434,12 @@
         <v>20</v>
       </c>
       <c r="B38" s="18">
-        <v>0.14477837612990244</v>
+        <f>'ABS Population by Age Range'!D37</f>
+        <v>0.14458334093878666</v>
       </c>
       <c r="C38" s="22">
         <f t="shared" si="28"/>
-        <v>3711058.365370932</v>
+        <v>3705981.8824441205</v>
       </c>
       <c r="D38" s="37">
         <f>'AU Infection Rate by Age'!C10</f>
@@ -29461,9 +29527,9 @@
         <f t="shared" si="50"/>
         <v>2443579.4621026893</v>
       </c>
-      <c r="AA38" s="121">
+      <c r="AA38" s="120">
         <f t="shared" si="50"/>
-        <v>3822967.5403422983</v>
+        <v>3822887.8973105131</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
@@ -29476,7 +29542,7 @@
       </c>
       <c r="F39" s="22">
         <f>$B$1*D38*E39</f>
-        <v>7645.9350806845969</v>
+        <v>7645.7757946210259</v>
       </c>
       <c r="G39" s="43">
         <f t="shared" ref="G39:W39" si="51">G$11*$D$38*$E$39</f>
@@ -29558,9 +29624,9 @@
         <f t="shared" si="52"/>
         <v>4887.1589242053788</v>
       </c>
-      <c r="AA39" s="120">
+      <c r="AA39" s="119">
         <f t="shared" si="52"/>
-        <v>7645.9350806845969</v>
+        <v>7645.7757946210259</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -29568,11 +29634,12 @@
         <v>21</v>
       </c>
       <c r="B40" s="18">
-        <v>0.12034977981552665</v>
+        <f>'ABS Population by Age Range'!D25</f>
+        <v>0.12056476079328157</v>
       </c>
       <c r="C40" s="22">
         <f t="shared" si="28"/>
-        <v>3084887.8754809727</v>
+        <v>3090334.0333675123</v>
       </c>
       <c r="D40" s="37">
         <f>'AU Infection Rate by Age'!C11</f>
@@ -29660,9 +29727,9 @@
         <f t="shared" si="54"/>
         <v>600880.19559902209</v>
       </c>
-      <c r="AA40" s="121">
+      <c r="AA40" s="120">
         <f t="shared" si="54"/>
-        <v>940073.9853300734</v>
+        <v>940054.40097799513</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -29675,7 +29742,7 @@
       </c>
       <c r="F41" s="22">
         <f>$B$1*D40*E41</f>
-        <v>1880.1479706601469</v>
+        <v>1880.1088019559902</v>
       </c>
       <c r="G41" s="43">
         <f t="shared" ref="G41:W41" si="55">G$11*$D$40*$E$41</f>
@@ -29757,9 +29824,9 @@
         <f t="shared" si="56"/>
         <v>1201.7603911980441</v>
       </c>
-      <c r="AA41" s="120">
+      <c r="AA41" s="119">
         <f t="shared" si="56"/>
-        <v>1880.1479706601469</v>
+        <v>1880.1088019559902</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -29767,11 +29834,12 @@
         <v>22</v>
       </c>
       <c r="B42" s="18">
-        <v>0.12716137671014424</v>
+        <f>'ABS Population by Age Range'!D13</f>
+        <v>0.1255958322404806</v>
       </c>
       <c r="C42" s="22">
         <f t="shared" si="28"/>
-        <v>3259487.3862160868</v>
+        <v>3219291.2113628346</v>
       </c>
       <c r="D42" s="37">
         <f>'AU Infection Rate by Age'!C12</f>
@@ -29859,9 +29927,9 @@
         <f t="shared" si="58"/>
         <v>160234.71882640588</v>
       </c>
-      <c r="AA42" s="121">
+      <c r="AA42" s="120">
         <f t="shared" si="58"/>
-        <v>250686.39608801957</v>
+        <v>250681.17359413204</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
@@ -29956,14 +30024,14 @@
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="AA43" s="122">
+      <c r="AA43" s="121">
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="22"/>
@@ -30052,12 +30120,12 @@
       </c>
       <c r="AA44" s="90">
         <f t="shared" si="62"/>
-        <v>25632684</v>
+        <v>25632150.000000004</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B45" s="63"/>
       <c r="C45" s="24"/>
@@ -30144,9 +30212,9 @@
         <f t="shared" si="64"/>
         <v>289744.43031784846</v>
       </c>
-      <c r="AA45" s="122">
+      <c r="AA45" s="121">
         <f t="shared" si="64"/>
-        <v>453303.67572616134</v>
+        <v>453294.23215158924</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -30177,7 +30245,7 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="84" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B47" s="28"/>
       <c r="C47" s="22"/>
@@ -30247,7 +30315,7 @@
       </c>
       <c r="C49" s="22">
         <f>$B$1 * B49</f>
-        <v>1281634.2000000002</v>
+        <v>1281607.5</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30"/>
@@ -30334,7 +30402,7 @@
       </c>
       <c r="AA49" s="90">
         <f t="shared" si="66"/>
-        <v>1281634.2000000002</v>
+        <v>1281607.5</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
@@ -30426,9 +30494,9 @@
         <f t="shared" si="68"/>
         <v>86016</v>
       </c>
-      <c r="AA50" s="120">
+      <c r="AA50" s="119">
         <f t="shared" si="68"/>
-        <v>134571.59100000001</v>
+        <v>134568.78750000001</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
@@ -30440,7 +30508,7 @@
       </c>
       <c r="C51" s="22">
         <f>$B$1 * B51</f>
-        <v>1179103.4639999999</v>
+        <v>1179078.8999999999</v>
       </c>
       <c r="D51" s="66"/>
       <c r="E51" s="30"/>
@@ -30525,9 +30593,9 @@
         <f t="shared" si="70"/>
         <v>753664</v>
       </c>
-      <c r="AA51" s="121">
+      <c r="AA51" s="120">
         <f t="shared" si="70"/>
-        <v>1179103.4639999999</v>
+        <v>1179078.8999999999</v>
       </c>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
@@ -30619,9 +30687,9 @@
         <f t="shared" si="72"/>
         <v>55017.471999999994</v>
       </c>
-      <c r="AA52" s="120">
+      <c r="AA52" s="119">
         <f t="shared" si="72"/>
-        <v>86074.552871999986</v>
+        <v>86072.759699999995</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
@@ -30633,7 +30701,7 @@
       </c>
       <c r="C53" s="22">
         <f>$B$1 * B53</f>
-        <v>7946132.04</v>
+        <v>7945966.5</v>
       </c>
       <c r="D53" s="66"/>
       <c r="E53" s="30"/>
@@ -30718,9 +30786,9 @@
         <f t="shared" si="74"/>
         <v>5079040</v>
       </c>
-      <c r="AA53" s="121">
+      <c r="AA53" s="120">
         <f t="shared" si="74"/>
-        <v>7946132.04</v>
+        <v>7945966.5</v>
       </c>
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.25">
@@ -30812,9 +30880,9 @@
         <f t="shared" si="76"/>
         <v>319979.52000000002</v>
       </c>
-      <c r="AA54" s="120">
+      <c r="AA54" s="119">
         <f t="shared" si="76"/>
-        <v>500606.31852000003</v>
+        <v>500595.88949999999</v>
       </c>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
@@ -30826,7 +30894,7 @@
       </c>
       <c r="C55" s="22">
         <f>$B$1 * B55</f>
-        <v>8638214.5080000013</v>
+        <v>8638034.5500000007</v>
       </c>
       <c r="D55" s="66"/>
       <c r="E55" s="30"/>
@@ -30911,9 +30979,9 @@
         <f t="shared" si="78"/>
         <v>5521408</v>
       </c>
-      <c r="AA55" s="121">
+      <c r="AA55" s="120">
         <f t="shared" si="78"/>
-        <v>8638214.5080000013</v>
+        <v>8638034.5500000007</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
@@ -31005,9 +31073,9 @@
         <f t="shared" si="80"/>
         <v>331284.47999999998</v>
       </c>
-      <c r="AA56" s="120">
+      <c r="AA56" s="119">
         <f t="shared" si="80"/>
-        <v>518292.87048000004</v>
+        <v>518282.07300000003</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -31019,7 +31087,7 @@
       </c>
       <c r="C57" s="22">
         <f>$B$1 * B57</f>
-        <v>384490.26</v>
+        <v>384482.25</v>
       </c>
       <c r="D57" s="66"/>
       <c r="E57" s="30"/>
@@ -31104,9 +31172,9 @@
         <f t="shared" si="82"/>
         <v>245760</v>
       </c>
-      <c r="AA57" s="121">
+      <c r="AA57" s="120">
         <f t="shared" si="82"/>
-        <v>384490.26</v>
+        <v>384482.25</v>
       </c>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
@@ -31198,9 +31266,9 @@
         <f t="shared" si="84"/>
         <v>13762.56</v>
       </c>
-      <c r="AA58" s="120">
+      <c r="AA58" s="119">
         <f t="shared" si="84"/>
-        <v>21531.454560000002</v>
+        <v>21531.006000000001</v>
       </c>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
@@ -31212,7 +31280,7 @@
       </c>
       <c r="C59" s="22">
         <f>$B$1 * B59</f>
-        <v>4126862.1240000003</v>
+        <v>4126776.15</v>
       </c>
       <c r="D59" s="66"/>
       <c r="E59" s="30"/>
@@ -31297,9 +31365,9 @@
         <f t="shared" si="86"/>
         <v>2637824</v>
       </c>
-      <c r="AA59" s="121">
+      <c r="AA59" s="120">
         <f t="shared" si="86"/>
-        <v>4126862.1240000003</v>
+        <v>4126776.15</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
@@ -31371,7 +31439,7 @@
       <c r="Z60" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AA60" s="122" t="s">
+      <c r="AA60" s="121" t="s">
         <v>11</v>
       </c>
     </row>
@@ -31462,14 +31530,14 @@
         <f t="shared" si="88"/>
         <v>15056896</v>
       </c>
-      <c r="AA61" s="121">
+      <c r="AA61" s="120">
         <f>SUM(AA49,AA51,AA53,AA55,AA57,AA59)</f>
-        <v>23556436.596000005</v>
+        <v>23555945.850000001</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B62" s="57"/>
       <c r="C62" s="57"/>
@@ -31556,9 +31624,9 @@
         <f t="shared" si="90"/>
         <v>806060.03200000012</v>
       </c>
-      <c r="AA62" s="122">
+      <c r="AA62" s="121">
         <f>SUM(AA50,AA52,AA54,AA56,AA58,AA60)</f>
-        <v>1261076.787432</v>
+        <v>1261050.5157000001</v>
       </c>
     </row>
   </sheetData>
@@ -31566,958 +31634,1067 @@
     <hyperlink ref="D25" r:id="rId1" display="Infection Rate" xr:uid="{98D6456F-EA03-4FCB-8D3D-1822F6B38CCF}"/>
     <hyperlink ref="E25" r:id="rId2" location="case-fatality-rate-of-covid-19-by-age" xr:uid="{0058192C-B05A-45D2-8597-C1F9B3D9241E}"/>
     <hyperlink ref="E48" r:id="rId3" location="case-fatality-rate-of-covid-19-by-preexisting-health-conditions" xr:uid="{110A2613-24A6-4768-B90C-571B307D13E2}"/>
+    <hyperlink ref="B1" r:id="rId4" display="https://www.abs.gov.au/ausstats/abs@.nsf/0/1647509ef7e25faaca2568a900154b63?opendocument" xr:uid="{63727E5E-0850-4414-8DD8-E50A09A5AEE8}"/>
+    <hyperlink ref="B25" r:id="rId5" xr:uid="{E432DB14-5D35-4B35-8F24-1C070D7F22B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C72C88-CD5D-4DB8-876B-F718C1E8501B}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7">
+        <v>302684</v>
+      </c>
+      <c r="L2" s="127"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="7">
-        <v>303407</v>
-      </c>
+      <c r="B3" s="9">
+        <v>304818</v>
+      </c>
+      <c r="L3" s="127"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="9">
-        <v>308459</v>
-      </c>
+      <c r="B4" s="9">
+        <v>311200</v>
+      </c>
+      <c r="L4" s="127"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="9">
-        <v>323809</v>
-      </c>
+      <c r="B5" s="9">
+        <v>326896</v>
+      </c>
+      <c r="L5" s="127"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="9">
-        <v>318292</v>
-      </c>
+      <c r="B6" s="9">
+        <v>321565</v>
+      </c>
+      <c r="L6" s="127"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="9">
-        <v>318326</v>
-      </c>
+      <c r="B7" s="11">
+        <v>1567163</v>
+      </c>
+      <c r="L7" s="128"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="11">
-        <v>1572293</v>
-      </c>
+      <c r="B8" s="9">
+        <v>321643</v>
+      </c>
+      <c r="L8" s="127"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="9">
-        <v>324001</v>
-      </c>
+      <c r="B9" s="9">
+        <v>326729</v>
+      </c>
+      <c r="L9" s="127"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="9">
-        <v>321028</v>
-      </c>
+      <c r="B10" s="9">
+        <v>323562</v>
+      </c>
+      <c r="L10" s="127"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="9">
-        <v>320255</v>
-      </c>
+      <c r="B11" s="9">
+        <v>322648</v>
+      </c>
+      <c r="L11" s="127"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="9">
-        <v>321787</v>
-      </c>
+      <c r="B12" s="9">
+        <v>324065</v>
+      </c>
+      <c r="L12" s="127"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="9">
-        <v>317469</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>35</v>
-      </c>
       <c r="B13" s="13">
-        <v>1604540</v>
+        <v>1618647</v>
       </c>
       <c r="C13" s="2">
         <f>SUM(B7,B13)</f>
-        <v>3176833</v>
+        <v>3185810</v>
       </c>
       <c r="D13" s="1">
         <f>C13/$B$108</f>
-        <v>0.12716137671014424</v>
-      </c>
+        <v>0.1255958322404806</v>
+      </c>
+      <c r="L13" s="128"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7">
+        <v>319703</v>
+      </c>
+      <c r="L14" s="127"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="7">
-        <v>317746</v>
-      </c>
+      <c r="B15" s="9">
+        <v>319972</v>
+      </c>
+      <c r="L15" s="127"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9">
-        <v>314444</v>
-      </c>
+      <c r="B16" s="9">
+        <v>316523</v>
+      </c>
+      <c r="L16" s="127"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="9">
-        <v>303530</v>
-      </c>
+      <c r="B17" s="9">
+        <v>305472</v>
+      </c>
+      <c r="L17" s="127"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="9">
-        <v>292012</v>
-      </c>
+      <c r="B18" s="9">
+        <v>294067</v>
+      </c>
+      <c r="L18" s="127"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="9">
-        <v>288185</v>
-      </c>
+      <c r="B19" s="11">
+        <v>1555737</v>
+      </c>
+      <c r="L19" s="128"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="11">
-        <v>1515917</v>
-      </c>
+      <c r="B20" s="9">
+        <v>290601</v>
+      </c>
+      <c r="L20" s="127"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="9">
-        <v>285577</v>
-      </c>
+      <c r="B21" s="9">
+        <v>288611</v>
+      </c>
+      <c r="L21" s="127"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="9">
-        <v>286559</v>
-      </c>
+      <c r="B22" s="9">
+        <v>290316</v>
+      </c>
+      <c r="L22" s="127"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="9">
-        <v>294689</v>
-      </c>
+      <c r="B23" s="9">
+        <v>307634</v>
+      </c>
+      <c r="L23" s="127"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="9">
-        <v>306243</v>
-      </c>
+      <c r="B24" s="9">
+        <v>325295</v>
+      </c>
+      <c r="L24" s="127"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="9">
-        <v>317676</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="B25" s="13">
-        <v>1490744</v>
+        <v>1502457</v>
       </c>
       <c r="C25" s="2">
         <f>SUM(B25,B19)</f>
-        <v>3006661</v>
+        <v>3058194</v>
       </c>
       <c r="D25" s="1">
         <f>C25/$B$108</f>
-        <v>0.12034977981552665</v>
-      </c>
+        <v>0.12056476079328157</v>
+      </c>
+      <c r="L25" s="128"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="7">
+        <v>330388</v>
+      </c>
+      <c r="L26" s="127"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="7">
-        <v>324826</v>
-      </c>
+      <c r="B27" s="9">
+        <v>335483</v>
+      </c>
+      <c r="L27" s="127"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="9">
-        <v>332316</v>
-      </c>
+      <c r="B28" s="9">
+        <v>347121</v>
+      </c>
+      <c r="L28" s="127"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="9">
-        <v>345101</v>
-      </c>
+      <c r="B29" s="9">
+        <v>365323</v>
+      </c>
+      <c r="L29" s="127"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="9">
-        <v>366768</v>
-      </c>
+      <c r="B30" s="9">
+        <v>380725</v>
+      </c>
+      <c r="L30" s="127"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="9">
-        <v>370624</v>
-      </c>
+      <c r="B31" s="11">
+        <v>1759040</v>
+      </c>
+      <c r="L31" s="128"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="11">
-        <v>1739635</v>
-      </c>
+      <c r="B32" s="9">
+        <v>379564</v>
+      </c>
+      <c r="L32" s="127"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="9">
-        <v>369083</v>
-      </c>
+      <c r="B33" s="9">
+        <v>376903</v>
+      </c>
+      <c r="L33" s="127"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="9">
-        <v>371226</v>
-      </c>
+      <c r="B34" s="9">
+        <v>378326</v>
+      </c>
+      <c r="L34" s="127"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="9">
-        <v>377728</v>
-      </c>
+      <c r="B35" s="9">
+        <v>384454</v>
+      </c>
+      <c r="L35" s="127"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="9">
-        <v>382958</v>
-      </c>
+      <c r="B36" s="9">
+        <v>389152</v>
+      </c>
+      <c r="L36" s="127"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="9">
-        <v>376323</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="B37" s="13">
-        <v>1877318</v>
+        <v>1908399</v>
       </c>
       <c r="C37" s="2">
         <f>SUM(B31,B37)</f>
-        <v>3616953</v>
+        <v>3667439</v>
       </c>
       <c r="D37" s="1">
         <f>C37/$B$108</f>
-        <v>0.14477837612990244</v>
-      </c>
+        <v>0.14458334093878666</v>
+      </c>
+      <c r="L37" s="128"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="7">
+        <v>381627</v>
+      </c>
+      <c r="L38" s="127"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="7">
-        <v>375913</v>
-      </c>
+      <c r="B39" s="9">
+        <v>380703</v>
+      </c>
+      <c r="L39" s="127"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="9">
-        <v>372184</v>
-      </c>
+      <c r="B40" s="9">
+        <v>376308</v>
+      </c>
+      <c r="L40" s="127"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="9">
-        <v>374909</v>
-      </c>
+      <c r="B41" s="9">
+        <v>378900</v>
+      </c>
+      <c r="L41" s="127"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="9">
-        <v>370727</v>
-      </c>
+      <c r="B42" s="9">
+        <v>374563</v>
+      </c>
+      <c r="L42" s="127"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="9">
-        <v>369093</v>
-      </c>
+      <c r="B43" s="11">
+        <v>1892101</v>
+      </c>
+      <c r="L43" s="128"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="11">
-        <v>1862826</v>
-      </c>
+      <c r="B44" s="9">
+        <v>371946</v>
+      </c>
+      <c r="L44" s="127"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="9">
-        <v>366167</v>
-      </c>
+      <c r="B45" s="9">
+        <v>368877</v>
+      </c>
+      <c r="L45" s="127"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="9">
-        <v>355211</v>
-      </c>
+      <c r="B46" s="9">
+        <v>357736</v>
+      </c>
+      <c r="L46" s="127"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="9">
-        <v>346074</v>
-      </c>
+      <c r="B47" s="9">
+        <v>348170</v>
+      </c>
+      <c r="L47" s="127"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="9">
-        <v>332582</v>
-      </c>
+      <c r="B48" s="9">
+        <v>334445</v>
+      </c>
+      <c r="L48" s="127"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="9">
-        <v>322857</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>71</v>
-      </c>
       <c r="B49" s="13">
-        <v>1722891</v>
+        <v>1781174</v>
       </c>
       <c r="C49" s="2">
         <f>SUM(B43,B49)</f>
-        <v>3585717</v>
+        <v>3673275</v>
       </c>
       <c r="D49" s="1">
         <f>C49/$B$108</f>
-        <v>0.14352807031813389</v>
-      </c>
+        <v>0.14481341657950456</v>
+      </c>
+      <c r="L49" s="128"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="7">
+        <v>324591</v>
+      </c>
+      <c r="L50" s="127"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="7">
-        <v>316895</v>
-      </c>
+      <c r="B51" s="9">
+        <v>318448</v>
+      </c>
+      <c r="L51" s="127"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="9">
-        <v>314772</v>
-      </c>
+      <c r="B52" s="9">
+        <v>315770</v>
+      </c>
+      <c r="L52" s="127"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="9">
-        <v>317141</v>
-      </c>
+      <c r="B53" s="9">
+        <v>318107</v>
+      </c>
+      <c r="L53" s="127"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="9">
-        <v>318159</v>
-      </c>
+      <c r="B54" s="9">
+        <v>318926</v>
+      </c>
+      <c r="L54" s="127"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="9">
-        <v>327088</v>
-      </c>
+      <c r="B55" s="11">
+        <v>1595842</v>
+      </c>
+      <c r="L55" s="128"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="11">
-        <v>1594055</v>
-      </c>
+      <c r="B56" s="9">
+        <v>327436</v>
+      </c>
+      <c r="L56" s="127"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="9">
-        <v>332783</v>
-      </c>
+      <c r="B57" s="9">
+        <v>332934</v>
+      </c>
+      <c r="L57" s="127"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B57" s="9">
-        <v>344220</v>
-      </c>
+      <c r="B58" s="9">
+        <v>344168</v>
+      </c>
+      <c r="L58" s="127"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="9">
-        <v>347838</v>
-      </c>
+      <c r="B59" s="9">
+        <v>347705</v>
+      </c>
+      <c r="L59" s="127"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="9">
-        <v>326482</v>
-      </c>
+      <c r="B60" s="9">
+        <v>326172</v>
+      </c>
+      <c r="L60" s="127"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="9">
-        <v>320787</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="B61" s="13">
-        <v>1672110</v>
+        <v>1678415</v>
       </c>
       <c r="C61" s="2">
         <f>SUM(B55,B61)</f>
-        <v>3266165</v>
+        <v>3274257</v>
       </c>
       <c r="D61" s="1">
         <f>C61/$B$108</f>
-        <v>0.1307371328497558</v>
-      </c>
+        <v>0.12908272398046944</v>
+      </c>
+      <c r="L61" s="128"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="7">
+        <v>320460</v>
+      </c>
+      <c r="L62" s="127"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B62" s="7">
-        <v>310490</v>
-      </c>
+      <c r="B63" s="9">
+        <v>310043</v>
+      </c>
+      <c r="L63" s="127"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="9">
-        <v>301859</v>
-      </c>
+      <c r="B64" s="9">
+        <v>301380</v>
+      </c>
+      <c r="L64" s="127"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B64" s="9">
-        <v>302437</v>
-      </c>
+      <c r="B65" s="9">
+        <v>301965</v>
+      </c>
+      <c r="L65" s="127"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="9">
-        <v>301438</v>
-      </c>
+      <c r="B66" s="9">
+        <v>300916</v>
+      </c>
+      <c r="L66" s="127"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="9">
-        <v>312662</v>
-      </c>
+      <c r="B67" s="11">
+        <v>1534764</v>
+      </c>
+      <c r="L67" s="128"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B67" s="11">
-        <v>1528886</v>
-      </c>
+      <c r="B68" s="9">
+        <v>311890</v>
+      </c>
+      <c r="L68" s="127"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="9">
-        <v>314827</v>
-      </c>
+      <c r="B69" s="9">
+        <v>313933</v>
+      </c>
+      <c r="L69" s="127"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="9">
-        <v>312608</v>
-      </c>
+      <c r="B70" s="9">
+        <v>311527</v>
+      </c>
+      <c r="L70" s="127"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="9">
-        <v>310347</v>
-      </c>
+      <c r="B71" s="9">
+        <v>309248</v>
+      </c>
+      <c r="L71" s="127"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="9">
-        <v>299799</v>
-      </c>
+      <c r="B72" s="9">
+        <v>298726</v>
+      </c>
+      <c r="L72" s="127"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="8" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B72" s="9">
-        <v>291854</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
-        <v>95</v>
-      </c>
       <c r="B73" s="15">
-        <v>1529435</v>
+        <v>1545324</v>
       </c>
       <c r="C73" s="2">
         <f>SUM(B67,B73)</f>
-        <v>3058321</v>
+        <v>3080088</v>
       </c>
       <c r="D73" s="1">
         <f>C73/$B$108</f>
-        <v>0.12241761174778311</v>
-      </c>
+        <v>0.12142789925761971</v>
+      </c>
+      <c r="L73" s="128"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" s="7">
+        <v>290624</v>
+      </c>
+      <c r="L74" s="127"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B74" s="7">
-        <v>286653</v>
-      </c>
+      <c r="B75" s="9">
+        <v>285521</v>
+      </c>
+      <c r="L75" s="127"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B75" s="9">
-        <v>278597</v>
-      </c>
+      <c r="B76" s="9">
+        <v>277305</v>
+      </c>
+      <c r="L76" s="127"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B76" s="9">
-        <v>274229</v>
-      </c>
+      <c r="B77" s="9">
+        <v>272986</v>
+      </c>
+      <c r="L77" s="127"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B77" s="9">
-        <v>263189</v>
-      </c>
+      <c r="B78" s="9">
+        <v>261893</v>
+      </c>
+      <c r="L78" s="127"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B78" s="9">
-        <v>256395</v>
-      </c>
+      <c r="B79" s="11">
+        <v>1388329</v>
+      </c>
+      <c r="L79" s="128"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B79" s="11">
-        <v>1359063</v>
-      </c>
+      <c r="B80" s="9">
+        <v>254839</v>
+      </c>
+      <c r="L80" s="127"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B80" s="9">
-        <v>253278</v>
-      </c>
+      <c r="B81" s="9">
+        <v>251416</v>
+      </c>
+      <c r="L81" s="127"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B81" s="9">
-        <v>245505</v>
-      </c>
+      <c r="B82" s="9">
+        <v>243468</v>
+      </c>
+      <c r="L82" s="127"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="9">
-        <v>242897</v>
-      </c>
+      <c r="B83" s="9">
+        <v>240724</v>
+      </c>
+      <c r="L83" s="127"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B83" s="9">
-        <v>236622</v>
-      </c>
+      <c r="B84" s="9">
+        <v>234326</v>
+      </c>
+      <c r="L84" s="127"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B84" s="9">
-        <v>228616</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>107</v>
-      </c>
       <c r="B85" s="13">
-        <v>1206918</v>
+        <v>1224773</v>
       </c>
       <c r="C85" s="2">
         <f>SUM(B79,B85)</f>
-        <v>2565981</v>
+        <v>2613102</v>
       </c>
       <c r="D85" s="1">
         <f>C85/$B$108</f>
-        <v>0.10271036487346757</v>
-      </c>
+        <v>0.10301766910746854</v>
+      </c>
+      <c r="L85" s="128"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B86" s="7">
+        <v>226082</v>
+      </c>
+      <c r="L86" s="127"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B86" s="7">
-        <v>229044</v>
-      </c>
+      <c r="B87" s="9">
+        <v>226412</v>
+      </c>
+      <c r="L87" s="127"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B87" s="9">
-        <v>233694</v>
-      </c>
+      <c r="B88" s="9">
+        <v>231019</v>
+      </c>
+      <c r="L88" s="127"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B88" s="9">
-        <v>195750</v>
-      </c>
+      <c r="B89" s="9">
+        <v>192937</v>
+      </c>
+      <c r="L89" s="127"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="9">
-        <v>184470</v>
-      </c>
+      <c r="B90" s="9">
+        <v>181454</v>
+      </c>
+      <c r="L90" s="127"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B90" s="9">
-        <v>174168</v>
-      </c>
+      <c r="B91" s="11">
+        <v>1057904</v>
+      </c>
+      <c r="L91" s="128"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B91" s="11">
-        <v>1017126</v>
-      </c>
+      <c r="B92" s="9">
+        <v>171139</v>
+      </c>
+      <c r="L92" s="127"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B92" s="9">
-        <v>155236</v>
-      </c>
+      <c r="B93" s="9">
+        <v>151876</v>
+      </c>
+      <c r="L93" s="127"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B93" s="9">
-        <v>151609</v>
-      </c>
+      <c r="B94" s="9">
+        <v>148212</v>
+      </c>
+      <c r="L94" s="127"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B94" s="9">
-        <v>139284</v>
-      </c>
+      <c r="B95" s="9">
+        <v>135541</v>
+      </c>
+      <c r="L95" s="127"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B95" s="9">
-        <v>131354</v>
-      </c>
+      <c r="B96" s="9">
+        <v>127491</v>
+      </c>
+      <c r="L96" s="127"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B96" s="9">
-        <v>122545</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
-        <v>119</v>
-      </c>
       <c r="B97" s="13">
-        <v>700028</v>
+        <v>734259</v>
       </c>
       <c r="C97" s="2">
         <f>SUM(B91,B97)</f>
-        <v>1717154</v>
+        <v>1792163</v>
       </c>
       <c r="D97" s="1">
         <f>C97/$B$108</f>
-        <v>6.8733756751875541E-2</v>
-      </c>
+        <v>7.065336711718416E-2</v>
+      </c>
+      <c r="L97" s="128"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="7">
+        <v>118484</v>
+      </c>
+      <c r="L98" s="127"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B98" s="7">
-        <v>113813</v>
-      </c>
+      <c r="B99" s="9">
+        <v>109564</v>
+      </c>
+      <c r="L99" s="127"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B99" s="9">
-        <v>106420</v>
-      </c>
+      <c r="B100" s="9">
+        <v>101897</v>
+      </c>
+      <c r="L100" s="127"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B100" s="9">
-        <v>97756</v>
-      </c>
+      <c r="B101" s="9">
+        <v>93053</v>
+      </c>
+      <c r="L101" s="127"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="9">
-        <v>87436</v>
-      </c>
+      <c r="B102" s="9">
+        <v>82541</v>
+      </c>
+      <c r="L102" s="127"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B102" s="9">
-        <v>80415</v>
-      </c>
+      <c r="B103" s="11">
+        <v>505539</v>
+      </c>
+      <c r="L103" s="128"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B103" s="11">
-        <v>485840</v>
-      </c>
+      <c r="B104" s="11">
+        <v>313008</v>
+      </c>
+      <c r="L104" s="128"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="11">
-        <v>309768</v>
-      </c>
+      <c r="B105" s="11">
+        <v>153468</v>
+      </c>
+      <c r="L105" s="128"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B105" s="11">
-        <v>149167</v>
-      </c>
+      <c r="B106" s="11">
+        <v>44201</v>
+      </c>
+      <c r="L106" s="128"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B106" s="11">
-        <v>39704</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>129</v>
-      </c>
       <c r="B107" s="13">
-        <v>4424</v>
+        <v>5027</v>
       </c>
       <c r="C107" s="2">
         <f>SUM(B103:B107)</f>
-        <v>988903</v>
+        <v>1021243</v>
       </c>
       <c r="D107" s="1">
         <f>C107/$B$108</f>
-        <v>3.9583530803410746E-2</v>
-      </c>
+        <v>4.0260989985204748E-2</v>
+      </c>
+      <c r="L107" s="128"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B108" s="5">
-        <v>24982688</v>
-      </c>
+        <v>25365571</v>
+      </c>
+      <c r="L108" s="129"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32529,20 +32706,20 @@
   <dimension ref="A3:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>144</v>
-      </c>
-      <c r="B3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -32655,7 +32832,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B14">
         <f>SUM(B4:B12)</f>

</xml_diff>

<commit_message>
Updated with latest stats
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DCAB75-2C0E-42DA-8ED5-E252CAE1A623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCEC579-96DD-4680-8D68-A29A06CFF583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="309">
   <si>
     <t>Australian Population</t>
   </si>
@@ -961,6 +961,9 @@
   </si>
   <si>
     <t>Three step plan announced to begin opening back up, each state to determine their own timing</t>
+  </si>
+  <si>
+    <t>States begin loosening restrictions, VIC follows a couple of days later</t>
   </si>
 </sst>
 </file>
@@ -2178,46 +2181,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2327,46 +2330,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2476,46 +2479,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11701,46 +11704,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11841,46 +11844,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11984,46 +11987,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12121,46 +12124,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12528,46 +12531,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12677,46 +12680,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12826,46 +12829,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13243,46 +13246,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13383,46 +13386,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13526,46 +13529,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13663,46 +13666,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43919.754608101852</c:v>
+                  <c:v>43922.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43922.754608101852</c:v>
+                  <c:v>43925.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43925.754608101852</c:v>
+                  <c:v>43928.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43928.754608101852</c:v>
+                  <c:v>43931.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43931.754608101852</c:v>
+                  <c:v>43934.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43934.754608101852</c:v>
+                  <c:v>43937.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937.754608101852</c:v>
+                  <c:v>43940.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43940.754608101852</c:v>
+                  <c:v>43943.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43943.754608101852</c:v>
+                  <c:v>43946.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43946.754608101852</c:v>
+                  <c:v>43949.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43949.754608101852</c:v>
+                  <c:v>43952.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43952.754608101852</c:v>
+                  <c:v>43955.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43955.754608101852</c:v>
+                  <c:v>43958.759586689812</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43958.754608101852</c:v>
+                  <c:v>43961.759586689812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -32222,167 +32225,167 @@
       </c>
       <c r="B26" s="102">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>43919.754608101852</v>
+        <v>43922.759586689812</v>
       </c>
       <c r="C26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43920.754608101852</v>
+        <v>43923.759586689812</v>
       </c>
       <c r="D26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43921.754608101852</v>
+        <v>43924.759586689812</v>
       </c>
       <c r="E26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43922.754608101852</v>
+        <v>43925.759586689812</v>
       </c>
       <c r="F26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43923.754608101852</v>
+        <v>43926.759586689812</v>
       </c>
       <c r="G26" s="104">
         <f t="shared" ca="1" si="0"/>
-        <v>43924.754608101852</v>
+        <v>43927.759586689812</v>
       </c>
       <c r="H26" s="103">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>43925.754608101852</v>
+        <v>43928.759586689812</v>
       </c>
       <c r="I26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43926.754608101852</v>
+        <v>43929.759586689812</v>
       </c>
       <c r="J26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43927.754608101852</v>
+        <v>43930.759586689812</v>
       </c>
       <c r="K26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43928.754608101852</v>
+        <v>43931.759586689812</v>
       </c>
       <c r="L26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43929.754608101852</v>
+        <v>43932.759586689812</v>
       </c>
       <c r="M26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43930.754608101852</v>
+        <v>43933.759586689812</v>
       </c>
       <c r="N26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>43931.754608101852</v>
+        <v>43934.759586689812</v>
       </c>
       <c r="O26" s="102">
         <f t="shared" ca="1" si="1"/>
-        <v>43932.754608101852</v>
+        <v>43935.759586689812</v>
       </c>
       <c r="P26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43933.754608101852</v>
+        <v>43936.759586689812</v>
       </c>
       <c r="Q26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43934.754608101852</v>
+        <v>43937.759586689812</v>
       </c>
       <c r="R26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43935.754608101852</v>
+        <v>43938.759586689812</v>
       </c>
       <c r="S26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43936.754608101852</v>
+        <v>43939.759586689812</v>
       </c>
       <c r="T26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43937.754608101852</v>
+        <v>43940.759586689812</v>
       </c>
       <c r="U26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>43938.754608101852</v>
+        <v>43941.759586689812</v>
       </c>
       <c r="V26" s="102">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>43939.754608101852</v>
+        <v>43942.759586689812</v>
       </c>
       <c r="W26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43940.754608101852</v>
+        <v>43943.759586689812</v>
       </c>
       <c r="X26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43941.754608101852</v>
+        <v>43944.759586689812</v>
       </c>
       <c r="Y26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43942.754608101852</v>
+        <v>43945.759586689812</v>
       </c>
       <c r="Z26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43943.754608101852</v>
+        <v>43946.759586689812</v>
       </c>
       <c r="AA26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43944.754608101852</v>
+        <v>43947.759586689812</v>
       </c>
       <c r="AB26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>43945.754608101852</v>
+        <v>43948.759586689812</v>
       </c>
       <c r="AC26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>43946.754608101852</v>
+        <v>43949.759586689812</v>
       </c>
       <c r="AD26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43947.754608101852</v>
+        <v>43950.759586689812</v>
       </c>
       <c r="AE26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43948.754608101852</v>
+        <v>43951.759586689812</v>
       </c>
       <c r="AF26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43949.754608101852</v>
+        <v>43952.759586689812</v>
       </c>
       <c r="AG26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43950.754608101852</v>
+        <v>43953.759586689812</v>
       </c>
       <c r="AH26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43951.754608101852</v>
+        <v>43954.759586689812</v>
       </c>
       <c r="AI26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>43952.754608101852</v>
+        <v>43955.759586689812</v>
       </c>
       <c r="AJ26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>43953.754608101852</v>
+        <v>43956.759586689812</v>
       </c>
       <c r="AK26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43954.754608101852</v>
+        <v>43957.759586689812</v>
       </c>
       <c r="AL26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43955.754608101852</v>
+        <v>43958.759586689812</v>
       </c>
       <c r="AM26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43956.754608101852</v>
+        <v>43959.759586689812</v>
       </c>
       <c r="AN26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43957.754608101852</v>
+        <v>43960.759586689812</v>
       </c>
       <c r="AO26" s="103">
         <f ca="1">AP26-1</f>
-        <v>43958.754608101852</v>
+        <v>43961.759586689812</v>
       </c>
       <c r="AP26" s="124">
         <f ca="1">NOW()</f>
-        <v>43959.754608101852</v>
+        <v>43962.759586689812</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -32901,7 +32904,7 @@
   <dimension ref="A1:AJ94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33211,7 +33214,12 @@
         <v>287</v>
       </c>
       <c r="O18" s="278"/>
-      <c r="P18" s="278"/>
+      <c r="P18" s="278">
+        <v>43961</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>308</v>
+      </c>
       <c r="W18" s="278"/>
       <c r="X18" s="134"/>
       <c r="AA18" s="278"/>
@@ -40818,7 +40826,7 @@
   <dimension ref="B3:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40862,7 +40870,7 @@
         <v>222</v>
       </c>
       <c r="C6" s="179">
-        <v>6913</v>
+        <v>6948</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -40871,7 +40879,7 @@
       </c>
       <c r="C7" s="177">
         <f ca="1">NOW()</f>
-        <v>43959.754608101852</v>
+        <v>43962.759586689812</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -40880,7 +40888,7 @@
       </c>
       <c r="C8" s="178">
         <f ca="1">C7-C5</f>
-        <v>67.754608101851773</v>
+        <v>70.75958668981184</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -40889,7 +40897,7 @@
       </c>
       <c r="C9" s="180">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>8.7367849817001826</v>
+        <v>9.115705248329613</v>
       </c>
       <c r="D9" t="s">
         <v>197</v>
@@ -40922,7 +40930,7 @@
       </c>
       <c r="C12" s="185">
         <f>C6/Projections!B14</f>
-        <v>8534.5679012345681</v>
+        <v>8577.7777777777774</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -40931,7 +40939,7 @@
       </c>
       <c r="C13" s="186">
         <f ca="1">(C4/Projections!B14)*(2^(((C7-21)-C5)/C9))</f>
-        <v>1612.9345963957389</v>
+        <v>1737.3488949699304</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -40940,7 +40948,7 @@
       </c>
       <c r="C14" s="165">
         <f ca="1">C12-C13</f>
-        <v>6921.6333048388296</v>
+        <v>6840.428882807847</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" s="183" t="s">
@@ -40954,7 +40962,7 @@
       </c>
       <c r="C15" s="76">
         <f>C6*Projections!B18</f>
-        <v>6359.96</v>
+        <v>6392.16</v>
       </c>
       <c r="I15" s="176"/>
     </row>
@@ -40964,7 +40972,7 @@
       </c>
       <c r="C16" s="95">
         <f ca="1">(C4*Projections!B18)*(2^(((C7-21)-C5)/C9))</f>
-        <v>1201.9588612341047</v>
+        <v>1294.6723965315923</v>
       </c>
       <c r="I16" s="176"/>
     </row>
@@ -40974,7 +40982,7 @@
       </c>
       <c r="C17" s="95">
         <f ca="1">C15-C16</f>
-        <v>5158.0011387658951</v>
+        <v>5097.4876034684075</v>
       </c>
       <c r="F17" t="s">
         <v>247</v>
@@ -40987,7 +40995,7 @@
       </c>
       <c r="C18" s="76">
         <f>C6*Projections!B19</f>
-        <v>345.65000000000003</v>
+        <v>347.40000000000003</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -40996,7 +41004,7 @@
       </c>
       <c r="C19" s="95">
         <f ca="1">(C4*Projections!B19)*(2^(((C7-49)-C5)/C9))</f>
-        <v>7.0846555437715741</v>
+        <v>8.3693500788690667</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -41005,7 +41013,7 @@
       </c>
       <c r="C20" s="95">
         <f ca="1">C18-C19</f>
-        <v>338.56534445622844</v>
+        <v>339.03064992113099</v>
       </c>
       <c r="F20" t="s">
         <v>252</v>
@@ -41017,7 +41025,7 @@
       </c>
       <c r="C21" s="76">
         <f>C6*Projections!B20</f>
-        <v>207.39</v>
+        <v>208.44</v>
       </c>
       <c r="I21" s="176"/>
     </row>
@@ -41027,7 +41035,7 @@
       </c>
       <c r="C22" s="95">
         <f ca="1">(C4*Projections!B20)*(2^(((C7-49)-C5)/C9))</f>
-        <v>4.2507933262629436</v>
+        <v>5.0216100473214391</v>
       </c>
       <c r="I22" s="176"/>
     </row>
@@ -41037,7 +41045,7 @@
       </c>
       <c r="C23" s="95">
         <f ca="1">C21-C22</f>
-        <v>203.13920667373705</v>
+        <v>203.41838995267855</v>
       </c>
       <c r="I23" s="176"/>
     </row>
@@ -41047,7 +41055,7 @@
       </c>
       <c r="C24" s="76">
         <f>C6*Projections!B21</f>
-        <v>96.781999999999996</v>
+        <v>97.272000000000006</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -41056,7 +41064,7 @@
       </c>
       <c r="C25" s="73">
         <f ca="1">(C4*Projections!B21)*(2^(((C7-42)-C5)/C9))</f>
-        <v>3.456726597095872</v>
+        <v>3.9903624808549458</v>
       </c>
       <c r="F25" t="s">
         <v>258</v>
@@ -41068,7 +41076,7 @@
       </c>
       <c r="C26" s="189">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>72.760645142809835</v>
+        <v>75.849908010544581</v>
       </c>
       <c r="D26" t="s">
         <v>197</v>
@@ -41083,7 +41091,7 @@
       </c>
       <c r="C27" s="188">
         <f ca="1">C7+C26</f>
-        <v>44032.515253244659</v>
+        <v>44038.609494700358</v>
       </c>
       <c r="F27" t="s">
         <v>260</v>
@@ -41095,7 +41103,7 @@
       </c>
       <c r="C28" s="187">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>27.898629935962756</v>
+        <v>29.04219689847401</v>
       </c>
       <c r="D28" t="s">
         <v>197</v>
@@ -41107,7 +41115,7 @@
       </c>
       <c r="C29" s="188">
         <f ca="1">C7+C28</f>
-        <v>43987.653238037812</v>
+        <v>43991.801783588286</v>
       </c>
       <c r="F29" t="s">
         <v>260</v>
@@ -41119,7 +41127,7 @@
       </c>
       <c r="C30" s="187">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>94.492586935119448</v>
+        <v>98.524378798996977</v>
       </c>
       <c r="D30" t="s">
         <v>197</v>
@@ -41131,7 +41139,7 @@
       </c>
       <c r="C31" s="188">
         <f ca="1">C7+C30</f>
-        <v>44054.247195036973</v>
+        <v>44061.283965488808</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -41140,7 +41148,7 @@
       </c>
       <c r="C34" s="177">
         <f ca="1">C7+30</f>
-        <v>43989.754608101852</v>
+        <v>43992.759586689812</v>
       </c>
       <c r="F34" t="s">
         <v>279</v>
@@ -41152,7 +41160,7 @@
       </c>
       <c r="C35" s="95">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>74701.707569381048</v>
+        <v>68007.466050689836</v>
       </c>
       <c r="F35" t="s">
         <v>245</v>
@@ -41164,7 +41172,7 @@
       </c>
       <c r="C36" s="95">
         <f ca="1">C35/Projections!B14</f>
-        <v>92224.330332569181</v>
+        <v>83959.834630481273</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -41173,7 +41181,7 @@
       </c>
       <c r="C37" s="95">
         <f ca="1">C35*Projections!B18</f>
-        <v>68725.570963830571</v>
+        <v>62566.868766634652</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -41182,7 +41190,7 @@
       </c>
       <c r="C38" s="95">
         <f ca="1">C35*Projections!B19</f>
-        <v>3735.0853784690526</v>
+        <v>3400.3733025344918</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -41191,7 +41199,7 @@
       </c>
       <c r="C39" s="95">
         <f ca="1">C35*Projections!B20</f>
-        <v>2241.0512270814315</v>
+        <v>2040.2239815206949</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -41200,7 +41208,7 @@
       </c>
       <c r="C40" s="73">
         <f ca="1">C35*Projections!B21</f>
-        <v>1045.8239059713346</v>
+        <v>952.10452470965777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new cases to charts
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED002B25-F516-4531-98E4-CE2ED4B6217D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8122F73C-5DD2-43AC-A945-8EE8003DEA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="75" windowWidth="37605" windowHeight="21000" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="329">
   <si>
     <t>Australian Population</t>
   </si>
@@ -1019,6 +1019,12 @@
   <si>
     <t>China sentences an Australian, Karm Gilespie in custody for drug smuggling to death, 6 years after arrest, seen as further evidence of China attempting to coerce/punish Australia for its recent actions to call for an inquiry into the origins and handling of the SARS-CoV-2 pandemic</t>
   </si>
+  <si>
+    <t>Govt suggests increasing cyber attacks on Australian govt and business sites are from a foreign actor (implying China), assumption being that it is related to the increasing tensions with China</t>
+  </si>
+  <si>
+    <t>Victorian govt puts further relaxation of distancing rules on hold as the state sees a spike in new COVID-19 cases, state of emergency to stay in place for another four weeks, other states begin to reconsider their scheduled border reopenings.</t>
+  </si>
 </sst>
 </file>
 
@@ -1841,11 +1847,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="12" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1853,6 +1854,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="12" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2227,46 +2233,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2376,46 +2382,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2434,46 +2440,46 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-1.0351966873706051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-2.0703933747412102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-4.1407867494824204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-8.2815734989648409</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-16.563146997929682</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-33.126293995859363</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-66.252587991718727</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-132.50517598343745</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-265.01035196687491</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-530.02070393374981</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-1060.0414078674996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-2120.0828157349993</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>-4240.1656314699985</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-8480.331262939997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2525,46 +2531,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2583,37 +2589,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="3">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>72.463768115942031</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>144.92753623188406</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>285.71428571428572</c:v>
+                  <c:v>289.85507246376812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>571.42857142857144</c:v>
+                  <c:v>579.71014492753625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1142.8571428571429</c:v>
+                  <c:v>1159.4202898550725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2285.7142857142858</c:v>
+                  <c:v>2318.840579710145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4571.4285714285716</c:v>
+                  <c:v>4637.68115942029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9142.8571428571431</c:v>
+                  <c:v>9275.36231884058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18285.714285714286</c:v>
+                  <c:v>18550.72463768116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36571.428571428572</c:v>
+                  <c:v>37101.44927536232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73142.857142857145</c:v>
+                  <c:v>74202.89855072464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2974,7 +2980,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -3123,7 +3129,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -3181,7 +3187,7 @@
                   <c:v>7019</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="#,##0">
-                  <c:v>7400</c:v>
+                  <c:v>7409</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="#,##0">
                   <c:v>7800</c:v>
@@ -3553,7 +3559,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -3578,46 +3584,46 @@
                 <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.4375</c:v>
+                  <c:v>0.43124999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.875</c:v>
+                  <c:v>0.86249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.75</c:v>
+                  <c:v>1.7249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>3.4499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>13.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>55.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.4</c:v>
+                  <c:v>91.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103.60000000000001</c:v>
+                  <c:v>102.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>109.2</c:v>
+                  <c:v>107.64</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>112</c:v>
+                  <c:v>110.39999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3702,7 +3708,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -3760,6 +3766,9 @@
                   <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="#,##0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -4131,7 +4140,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -4189,10 +4198,10 @@
                   <c:v>3648.0224340846935</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5412.5731227783745</c:v>
+                  <c:v>4217.9293984147635</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>914.98907768335982</c:v>
+                  <c:v>1102.9505029517011</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>713.45778394840875</c:v>
@@ -4280,7 +4289,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -4338,10 +4347,10 @@
                   <c:v>3007.9225055713932</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4188.839639512581</c:v>
+                  <c:v>3264.2939799538044</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>669.43398342253204</c:v>
+                  <c:v>810.07029325376584</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -4429,7 +4438,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -4487,13 +4496,13 @@
                   <c:v>640.09992851330003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1223.7334832657932</c:v>
+                  <c:v>953.63541846095893</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>245.55509426082781</c:v>
+                  <c:v>292.88020969793524</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>425.45455935549376</c:v>
+                  <c:v>516.35670124040007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4578,7 +4587,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -4636,10 +4645,10 @@
                   <c:v>640.09992851330003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1223.7334832657932</c:v>
+                  <c:v>953.63541846095893</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>245.55509426082781</c:v>
+                  <c:v>292.88020969793524</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -4727,7 +4736,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -4752,46 +4761,46 @@
                 <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.4375</c:v>
+                  <c:v>0.43124999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.875</c:v>
+                  <c:v>0.86249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.75</c:v>
+                  <c:v>1.7249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>3.4499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>13.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>55.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.4</c:v>
+                  <c:v>91.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103.60000000000001</c:v>
+                  <c:v>102.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>109.2</c:v>
+                  <c:v>107.64</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>112</c:v>
+                  <c:v>110.39999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5158,7 +5167,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -5309,7 +5318,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -5460,7 +5469,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -5612,7 +5621,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -5764,7 +5773,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -5915,7 +5924,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -6064,7 +6073,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -6216,7 +6225,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -6367,7 +6376,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -6798,7 +6807,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -6949,7 +6958,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -7100,7 +7109,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -7252,7 +7261,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -7401,7 +7410,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -7552,7 +7561,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -7701,7 +7710,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -7850,7 +7859,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -8001,7 +8010,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -8432,7 +8441,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -8583,7 +8592,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -8734,7 +8743,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -8883,7 +8892,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -9034,7 +9043,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -9183,7 +9192,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -9614,7 +9623,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -9765,7 +9774,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -9914,7 +9923,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -10065,7 +10074,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -10214,7 +10223,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -10640,7 +10649,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -10789,7 +10798,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -10847,7 +10856,7 @@
                   <c:v>7019</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="#,##0">
-                  <c:v>7400</c:v>
+                  <c:v>7409</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="#,##0">
                   <c:v>7800</c:v>
@@ -11220,7 +11229,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -11245,46 +11254,46 @@
                 <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.4375</c:v>
+                  <c:v>0.43124999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.875</c:v>
+                  <c:v>0.86249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.75</c:v>
+                  <c:v>1.7249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>3.4499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>13.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>55.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.4</c:v>
+                  <c:v>91.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103.60000000000001</c:v>
+                  <c:v>102.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>109.2</c:v>
+                  <c:v>107.64</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>112</c:v>
+                  <c:v>110.39999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11369,7 +11378,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -11427,6 +11436,9 @@
                   <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="#,##0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="#,##0">
                   <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
@@ -11756,46 +11768,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11814,37 +11826,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="3">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>72.463768115942031</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>144.92753623188406</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>285.71428571428572</c:v>
+                  <c:v>289.85507246376812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>571.42857142857144</c:v>
+                  <c:v>579.71014492753625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1142.8571428571429</c:v>
+                  <c:v>1159.4202898550725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2285.7142857142858</c:v>
+                  <c:v>2318.840579710145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4571.4285714285716</c:v>
+                  <c:v>4637.68115942029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9142.8571428571431</c:v>
+                  <c:v>9275.36231884058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18285.714285714286</c:v>
+                  <c:v>18550.72463768116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36571.428571428572</c:v>
+                  <c:v>37101.44927536232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73142.857142857145</c:v>
+                  <c:v>74202.89855072464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11896,46 +11908,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11954,40 +11966,40 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="2">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>72.463768115942031</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>144.92753623188406</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>262.85714285714289</c:v>
+                  <c:v>266.66666666666669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>525.71428571428578</c:v>
+                  <c:v>533.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1051.4285714285716</c:v>
+                  <c:v>1066.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2037.1428571428573</c:v>
+                  <c:v>2066.666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4074.2857142857147</c:v>
+                  <c:v>4133.3333333333339</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8148.5714285714294</c:v>
+                  <c:v>8266.6666666666679</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16297.142857142859</c:v>
+                  <c:v>16533.333333333336</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32594.285714285717</c:v>
+                  <c:v>33066.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>65254.285714285725</c:v>
+                  <c:v>66200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130508.57142857145</c:v>
+                  <c:v>132400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12039,46 +12051,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12097,34 +12109,34 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="4">
-                  <c:v>22.857142857142858</c:v>
+                  <c:v>23.188405797101449</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.714285714285715</c:v>
+                  <c:v>46.376811594202898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.142857142857146</c:v>
+                  <c:v>57.971014492753625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>114.28571428571429</c:v>
+                  <c:v>115.94202898550725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>228.57142857142858</c:v>
+                  <c:v>231.8840579710145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>457.14285714285717</c:v>
+                  <c:v>463.768115942029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>914.28571428571433</c:v>
+                  <c:v>927.536231884058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1828.5714285714287</c:v>
+                  <c:v>1855.072463768116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3657.1428571428573</c:v>
+                  <c:v>3710.144927536232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7314.2857142857147</c:v>
+                  <c:v>7420.289855072464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12176,46 +12188,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12234,28 +12246,28 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="6">
-                  <c:v>34.285714285714285</c:v>
+                  <c:v>34.782608695652172</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68.571428571428569</c:v>
+                  <c:v>69.565217391304344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>137.14285714285714</c:v>
+                  <c:v>139.13043478260869</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>274.28571428571428</c:v>
+                  <c:v>278.26086956521738</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>548.57142857142856</c:v>
+                  <c:v>556.52173913043475</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1097.1428571428571</c:v>
+                  <c:v>1113.0434782608695</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2194.2857142857142</c:v>
+                  <c:v>2226.086956521739</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4388.5714285714284</c:v>
+                  <c:v>4452.173913043478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12583,46 +12595,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12732,46 +12744,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12790,46 +12802,46 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-1.0351966873706051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-2.0703933747412102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-4.1407867494824204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-8.2815734989648409</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-16.563146997929682</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-33.126293995859363</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-66.252587991718727</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-132.50517598343745</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-265.01035196687491</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-530.02070393374981</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-1060.0414078674996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>-2120.0828157349993</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>-4240.1656314699985</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-8480.331262939997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12881,46 +12893,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12939,37 +12951,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="3">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>72.463768115942031</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>144.92753623188406</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>285.71428571428572</c:v>
+                  <c:v>289.85507246376812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>571.42857142857144</c:v>
+                  <c:v>579.71014492753625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1142.8571428571429</c:v>
+                  <c:v>1159.4202898550725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2285.7142857142858</c:v>
+                  <c:v>2318.840579710145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4571.4285714285716</c:v>
+                  <c:v>4637.68115942029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9142.8571428571431</c:v>
+                  <c:v>9275.36231884058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18285.714285714286</c:v>
+                  <c:v>18550.72463768116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36571.428571428572</c:v>
+                  <c:v>37101.44927536232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73142.857142857145</c:v>
+                  <c:v>74202.89855072464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13298,46 +13310,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13356,37 +13368,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="3">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>72.463768115942031</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>144.92753623188406</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>285.71428571428572</c:v>
+                  <c:v>289.85507246376812</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>571.42857142857144</c:v>
+                  <c:v>579.71014492753625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1142.8571428571429</c:v>
+                  <c:v>1159.4202898550725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2285.7142857142858</c:v>
+                  <c:v>2318.840579710145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4571.4285714285716</c:v>
+                  <c:v>4637.68115942029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9142.8571428571431</c:v>
+                  <c:v>9275.36231884058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18285.714285714286</c:v>
+                  <c:v>18550.72463768116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36571.428571428572</c:v>
+                  <c:v>37101.44927536232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73142.857142857145</c:v>
+                  <c:v>74202.89855072464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13438,46 +13450,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13496,40 +13508,40 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="2">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>72.463768115942031</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>142.85714285714286</c:v>
+                  <c:v>144.92753623188406</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>262.85714285714289</c:v>
+                  <c:v>266.66666666666669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>525.71428571428578</c:v>
+                  <c:v>533.33333333333337</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1051.4285714285716</c:v>
+                  <c:v>1066.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2037.1428571428573</c:v>
+                  <c:v>2066.666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4074.2857142857147</c:v>
+                  <c:v>4133.3333333333339</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8148.5714285714294</c:v>
+                  <c:v>8266.6666666666679</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16297.142857142859</c:v>
+                  <c:v>16533.333333333336</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32594.285714285717</c:v>
+                  <c:v>33066.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>65254.285714285725</c:v>
+                  <c:v>66200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130508.57142857145</c:v>
+                  <c:v>132400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13581,46 +13593,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13639,34 +13651,34 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="4">
-                  <c:v>22.857142857142858</c:v>
+                  <c:v>23.188405797101449</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.714285714285715</c:v>
+                  <c:v>46.376811594202898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.142857142857146</c:v>
+                  <c:v>57.971014492753625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>114.28571428571429</c:v>
+                  <c:v>115.94202898550725</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>228.57142857142858</c:v>
+                  <c:v>231.8840579710145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>457.14285714285717</c:v>
+                  <c:v>463.768115942029</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>914.28571428571433</c:v>
+                  <c:v>927.536231884058</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1828.5714285714287</c:v>
+                  <c:v>1855.072463768116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3657.1428571428573</c:v>
+                  <c:v>3710.144927536232</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7314.2857142857147</c:v>
+                  <c:v>7420.289855072464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13718,46 +13730,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43960.943847916664</c:v>
+                  <c:v>43964.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43963.943847916664</c:v>
+                  <c:v>43967.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43966.943847916664</c:v>
+                  <c:v>43970.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43969.943847916664</c:v>
+                  <c:v>43973.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43972.943847916664</c:v>
+                  <c:v>43976.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43975.943847916664</c:v>
+                  <c:v>43979.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43978.943847916664</c:v>
+                  <c:v>43982.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43981.943847916664</c:v>
+                  <c:v>43985.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43984.943847916664</c:v>
+                  <c:v>43988.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43987.943847916664</c:v>
+                  <c:v>43991.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43990.943847916664</c:v>
+                  <c:v>43994.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43993.943847916664</c:v>
+                  <c:v>43997.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43996.943847916664</c:v>
+                  <c:v>44000.917079166669</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43999.943847916664</c:v>
+                  <c:v>44003.917079166669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13776,28 +13788,28 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="6">
-                  <c:v>34.285714285714285</c:v>
+                  <c:v>34.782608695652172</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68.571428571428569</c:v>
+                  <c:v>69.565217391304344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>137.14285714285714</c:v>
+                  <c:v>139.13043478260869</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>274.28571428571428</c:v>
+                  <c:v>278.26086956521738</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>548.57142857142856</c:v>
+                  <c:v>556.52173913043475</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1097.1428571428571</c:v>
+                  <c:v>1113.0434782608695</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2194.2857142857142</c:v>
+                  <c:v>2226.086956521739</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4388.5714285714284</c:v>
+                  <c:v>4452.173913043478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14169,7 +14181,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -14227,10 +14239,10 @@
                   <c:v>3648.0224340846935</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5412.5731227783745</c:v>
+                  <c:v>4217.9293984147635</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>914.98907768335982</c:v>
+                  <c:v>1102.9505029517011</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>713.45778394840875</c:v>
@@ -14318,7 +14330,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -14376,10 +14388,10 @@
                   <c:v>3007.9225055713932</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4188.839639512581</c:v>
+                  <c:v>3264.2939799538044</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>669.43398342253204</c:v>
+                  <c:v>810.07029325376584</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -14467,7 +14479,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -14525,13 +14537,13 @@
                   <c:v>640.09992851330003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1223.7334832657932</c:v>
+                  <c:v>953.63541846095893</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>245.55509426082781</c:v>
+                  <c:v>292.88020969793524</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>425.45455935549376</c:v>
+                  <c:v>516.35670124040007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14616,7 +14628,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -14674,10 +14686,10 @@
                   <c:v>640.09992851330003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1223.7334832657932</c:v>
+                  <c:v>953.63541846095893</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>245.55509426082781</c:v>
+                  <c:v>292.88020969793524</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -14765,7 +14777,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -14790,46 +14802,46 @@
                 <c:formatCode>#,##0_ ;[Red]\-#,##0\ </c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.4375</c:v>
+                  <c:v>0.43124999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.875</c:v>
+                  <c:v>0.86249999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.75</c:v>
+                  <c:v>1.7249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>3.4499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>13.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>55.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84</c:v>
+                  <c:v>82.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>92.4</c:v>
+                  <c:v>91.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>98</c:v>
+                  <c:v>96.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103.60000000000001</c:v>
+                  <c:v>102.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>109.2</c:v>
+                  <c:v>107.64</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>112</c:v>
+                  <c:v>110.39999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15195,7 +15207,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -15346,7 +15358,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -15497,7 +15509,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -15649,7 +15661,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -15801,7 +15813,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -15952,7 +15964,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -16101,7 +16113,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -16253,7 +16265,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -16404,7 +16416,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -16834,7 +16846,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -16985,7 +16997,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -17136,7 +17148,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -17288,7 +17300,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -17437,7 +17449,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -17588,7 +17600,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -17737,7 +17749,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -17886,7 +17898,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -18037,7 +18049,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -18467,7 +18479,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -18618,7 +18630,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -18769,7 +18781,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -18918,7 +18930,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -19069,7 +19081,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -19218,7 +19230,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -19648,7 +19660,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -19799,7 +19811,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -19948,7 +19960,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -20099,7 +20111,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -20248,7 +20260,7 @@
                   <c:v>43966.15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44005.25</c:v>
+                  <c:v>44001.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>44022.5</c:v>
@@ -31654,85 +31666,85 @@
       </c>
       <c r="B18" s="100">
         <f>B17*$E$34</f>
-        <v>0</v>
+        <v>-1.0351966873706051</v>
       </c>
       <c r="C18" s="118"/>
       <c r="D18" s="118"/>
       <c r="E18" s="118">
         <f>E17*$E$34</f>
-        <v>0</v>
+        <v>-2.0703933747412102</v>
       </c>
       <c r="F18" s="118"/>
       <c r="G18" s="45"/>
       <c r="H18" s="118">
         <f>H17*$E$34</f>
-        <v>0</v>
+        <v>-4.1407867494824204</v>
       </c>
       <c r="I18" s="118"/>
       <c r="J18" s="118"/>
       <c r="K18" s="118">
         <f>K17*$E$34</f>
-        <v>0</v>
+        <v>-8.2815734989648409</v>
       </c>
       <c r="L18" s="118"/>
       <c r="M18" s="118"/>
       <c r="N18" s="118">
         <f>N17*$E$34</f>
-        <v>0</v>
+        <v>-16.563146997929682</v>
       </c>
       <c r="O18" s="118"/>
       <c r="P18" s="118"/>
       <c r="Q18" s="118">
         <f>Q17*$E$34</f>
-        <v>0</v>
+        <v>-33.126293995859363</v>
       </c>
       <c r="R18" s="118"/>
       <c r="S18" s="118"/>
       <c r="T18" s="118">
         <f>T17*$E$34</f>
-        <v>0</v>
+        <v>-66.252587991718727</v>
       </c>
       <c r="U18" s="118"/>
       <c r="V18" s="118"/>
       <c r="W18" s="118">
         <f>W17*$E$34</f>
-        <v>0</v>
+        <v>-132.50517598343745</v>
       </c>
       <c r="X18" s="118"/>
       <c r="Y18" s="118"/>
       <c r="Z18" s="118">
         <f>Z17*$E$34</f>
-        <v>0</v>
+        <v>-265.01035196687491</v>
       </c>
       <c r="AA18" s="118"/>
       <c r="AB18" s="118"/>
       <c r="AC18" s="118">
         <f>AC17*$E$34</f>
-        <v>0</v>
+        <v>-530.02070393374981</v>
       </c>
       <c r="AD18" s="118"/>
       <c r="AE18" s="118"/>
       <c r="AF18" s="118">
         <f>AF17*$E$34</f>
-        <v>0</v>
+        <v>-1060.0414078674996</v>
       </c>
       <c r="AG18" s="118"/>
       <c r="AH18" s="118"/>
       <c r="AI18" s="118">
         <f>AI17*$E$34</f>
-        <v>0</v>
+        <v>-2120.0828157349993</v>
       </c>
       <c r="AJ18" s="118"/>
       <c r="AK18" s="118"/>
       <c r="AL18" s="118">
         <f>AL17*$E$34</f>
-        <v>0</v>
+        <v>-4240.1656314699985</v>
       </c>
       <c r="AM18" s="118"/>
       <c r="AN18" s="118"/>
       <c r="AO18" s="118">
         <f>AO17*$E$34</f>
-        <v>0</v>
+        <v>-8480.331262939997</v>
       </c>
       <c r="AP18" s="45"/>
       <c r="AQ18" s="81" t="s">
@@ -31745,85 +31757,85 @@
       </c>
       <c r="B19" s="98">
         <f>B18</f>
-        <v>0</v>
+        <v>-1.0351966873706051</v>
       </c>
       <c r="C19" s="99"/>
       <c r="D19" s="99"/>
       <c r="E19" s="99">
         <f>E18</f>
-        <v>0</v>
+        <v>-2.0703933747412102</v>
       </c>
       <c r="F19" s="99"/>
       <c r="G19" s="46"/>
       <c r="H19" s="99">
         <f>H18</f>
-        <v>0</v>
+        <v>-4.1407867494824204</v>
       </c>
       <c r="I19" s="99"/>
       <c r="J19" s="99"/>
       <c r="K19" s="99">
         <f>K18</f>
-        <v>0</v>
+        <v>-8.2815734989648409</v>
       </c>
       <c r="L19" s="99"/>
       <c r="M19" s="99"/>
       <c r="N19" s="99">
         <f>N18</f>
-        <v>0</v>
+        <v>-16.563146997929682</v>
       </c>
       <c r="O19" s="99"/>
       <c r="P19" s="99"/>
       <c r="Q19" s="99">
         <f>Q18</f>
-        <v>0</v>
+        <v>-33.126293995859363</v>
       </c>
       <c r="R19" s="99"/>
       <c r="S19" s="99"/>
       <c r="T19" s="99">
         <f>T18</f>
-        <v>0</v>
+        <v>-66.252587991718727</v>
       </c>
       <c r="U19" s="99"/>
       <c r="V19" s="99"/>
       <c r="W19" s="135">
         <f>W18-B18</f>
-        <v>0</v>
+        <v>-131.46997929606684</v>
       </c>
       <c r="X19" s="135"/>
       <c r="Y19" s="135"/>
       <c r="Z19" s="135">
         <f>Z18-E18</f>
-        <v>0</v>
+        <v>-262.93995859213368</v>
       </c>
       <c r="AA19" s="135"/>
       <c r="AB19" s="135"/>
       <c r="AC19" s="135">
         <f>AC18-H18</f>
-        <v>0</v>
+        <v>-525.87991718426736</v>
       </c>
       <c r="AD19" s="135"/>
       <c r="AE19" s="135"/>
       <c r="AF19" s="135">
         <f>AF18-K18</f>
-        <v>0</v>
+        <v>-1051.7598343685347</v>
       </c>
       <c r="AG19" s="135"/>
       <c r="AH19" s="135"/>
       <c r="AI19" s="135">
         <f>AI18-N18</f>
-        <v>0</v>
+        <v>-2103.5196687370694</v>
       </c>
       <c r="AJ19" s="135"/>
       <c r="AK19" s="135"/>
       <c r="AL19" s="135">
         <f>AL18-Q18</f>
-        <v>0</v>
+        <v>-4207.0393374741388</v>
       </c>
       <c r="AM19" s="135"/>
       <c r="AN19" s="135"/>
       <c r="AO19" s="135">
         <f>AO18-T18</f>
-        <v>0</v>
+        <v>-8414.0786749482777</v>
       </c>
       <c r="AP19" s="136"/>
       <c r="AQ19" s="59" t="s">
@@ -31845,67 +31857,67 @@
       <c r="J20" s="121"/>
       <c r="K20" s="145">
         <f>B17*(1-E34)</f>
-        <v>71.428571428571431</v>
+        <v>72.463768115942031</v>
       </c>
       <c r="L20" s="142"/>
       <c r="M20" s="143"/>
       <c r="N20" s="144">
         <f>E17*(1-E34)</f>
-        <v>142.85714285714286</v>
+        <v>144.92753623188406</v>
       </c>
       <c r="O20" s="142"/>
       <c r="P20" s="143"/>
       <c r="Q20" s="144">
         <f>H17*(1-E34)</f>
-        <v>285.71428571428572</v>
+        <v>289.85507246376812</v>
       </c>
       <c r="R20" s="142"/>
       <c r="S20" s="143"/>
       <c r="T20" s="144">
         <f>K17*(1-E34)</f>
-        <v>571.42857142857144</v>
+        <v>579.71014492753625</v>
       </c>
       <c r="U20" s="142"/>
       <c r="V20" s="143"/>
       <c r="W20" s="144">
         <f>N17*(1-E34)</f>
-        <v>1142.8571428571429</v>
+        <v>1159.4202898550725</v>
       </c>
       <c r="X20" s="142"/>
       <c r="Y20" s="143"/>
       <c r="Z20" s="144">
         <f>Q17*(1-E34)</f>
-        <v>2285.7142857142858</v>
+        <v>2318.840579710145</v>
       </c>
       <c r="AA20" s="142"/>
       <c r="AB20" s="143"/>
       <c r="AC20" s="144">
         <f>T17*(1-E34)</f>
-        <v>4571.4285714285716</v>
+        <v>4637.68115942029</v>
       </c>
       <c r="AD20" s="142"/>
       <c r="AE20" s="143"/>
       <c r="AF20" s="144">
         <f>W17*(1-E34)</f>
-        <v>9142.8571428571431</v>
+        <v>9275.36231884058</v>
       </c>
       <c r="AG20" s="142"/>
       <c r="AH20" s="143"/>
       <c r="AI20" s="144">
         <f>Z17*(1-E34)</f>
-        <v>18285.714285714286</v>
+        <v>18550.72463768116</v>
       </c>
       <c r="AJ20" s="142"/>
       <c r="AK20" s="143"/>
       <c r="AL20" s="144">
         <f>AC17*(1-E34)</f>
-        <v>36571.428571428572</v>
+        <v>37101.44927536232</v>
       </c>
       <c r="AM20" s="142"/>
       <c r="AN20" s="143"/>
       <c r="AO20" s="144">
         <f>AF17*(1-E34)</f>
-        <v>73142.857142857145</v>
+        <v>74202.89855072464</v>
       </c>
       <c r="AP20" s="91"/>
       <c r="AQ20" t="s">
@@ -31924,73 +31936,73 @@
       <c r="G21" s="94"/>
       <c r="H21" s="137">
         <f>B17-B18</f>
-        <v>71.428571428571431</v>
+        <v>72.463768115942031</v>
       </c>
       <c r="I21" s="137"/>
       <c r="J21" s="137"/>
       <c r="K21" s="137">
         <f>E17-E18</f>
-        <v>142.85714285714286</v>
+        <v>144.92753623188406</v>
       </c>
       <c r="L21" s="137"/>
       <c r="M21" s="137"/>
       <c r="N21" s="137">
         <f>(H17-H18)*$E$35</f>
-        <v>262.85714285714289</v>
+        <v>266.66666666666669</v>
       </c>
       <c r="O21" s="137"/>
       <c r="P21" s="137"/>
       <c r="Q21" s="137">
         <f>(K17-K18)*$E$35</f>
-        <v>525.71428571428578</v>
+        <v>533.33333333333337</v>
       </c>
       <c r="R21" s="137"/>
       <c r="S21" s="137"/>
       <c r="T21" s="137">
         <f>(N17-N18)*$E$35</f>
-        <v>1051.4285714285716</v>
+        <v>1066.6666666666667</v>
       </c>
       <c r="U21" s="137"/>
       <c r="V21" s="137"/>
       <c r="W21" s="137">
         <f>((Q17-Q18)*$E$35)-(H21*$E$35)</f>
-        <v>2037.1428571428573</v>
+        <v>2066.666666666667</v>
       </c>
       <c r="X21" s="137"/>
       <c r="Y21" s="137"/>
       <c r="Z21" s="137">
         <f>((T17-T18)*$E$35)-(K21*$E$35)</f>
-        <v>4074.2857142857147</v>
+        <v>4133.3333333333339</v>
       </c>
       <c r="AA21" s="137"/>
       <c r="AB21" s="137"/>
       <c r="AC21" s="137">
         <f>((W17-W18)*$E$35)-N21</f>
-        <v>8148.5714285714294</v>
+        <v>8266.6666666666679</v>
       </c>
       <c r="AD21" s="137"/>
       <c r="AE21" s="137"/>
       <c r="AF21" s="137">
         <f>((Z17-Z18)*$E$35)-Q21</f>
-        <v>16297.142857142859</v>
+        <v>16533.333333333336</v>
       </c>
       <c r="AG21" s="137"/>
       <c r="AH21" s="137"/>
       <c r="AI21" s="137">
         <f>((AC17-AC18)*$E$35)-T21</f>
-        <v>32594.285714285717</v>
+        <v>33066.666666666672</v>
       </c>
       <c r="AJ21" s="137"/>
       <c r="AK21" s="137"/>
       <c r="AL21" s="137">
         <f>((AF17-AF18)*$E$35)-W21</f>
-        <v>65254.285714285725</v>
+        <v>66200</v>
       </c>
       <c r="AM21" s="137"/>
       <c r="AN21" s="137"/>
       <c r="AO21" s="137">
         <f>((AI17-AI18)*$E$35)-Z21</f>
-        <v>130508.57142857145</v>
+        <v>132400</v>
       </c>
       <c r="AP21" s="138"/>
       <c r="AQ21" s="81" t="s">
@@ -32015,61 +32027,61 @@
       <c r="M22" s="121"/>
       <c r="N22" s="139">
         <f>(H17-H18)*($E$36+$E$37)</f>
-        <v>22.857142857142858</v>
+        <v>23.188405797101449</v>
       </c>
       <c r="O22" s="139"/>
       <c r="P22" s="139"/>
       <c r="Q22" s="139">
         <f>(K17-K18)*($E$36+$E$37)</f>
-        <v>45.714285714285715</v>
+        <v>46.376811594202898</v>
       </c>
       <c r="R22" s="139"/>
       <c r="S22" s="139"/>
       <c r="T22" s="139">
         <f>(N17-N18)*$E$36</f>
-        <v>57.142857142857146</v>
+        <v>57.971014492753625</v>
       </c>
       <c r="U22" s="139"/>
       <c r="V22" s="139"/>
       <c r="W22" s="139">
         <f>(Q17-Q18)*$E$36</f>
-        <v>114.28571428571429</v>
+        <v>115.94202898550725</v>
       </c>
       <c r="X22" s="139"/>
       <c r="Y22" s="139"/>
       <c r="Z22" s="139">
         <f>(T17-T18)*$E$36</f>
-        <v>228.57142857142858</v>
+        <v>231.8840579710145</v>
       </c>
       <c r="AA22" s="139"/>
       <c r="AB22" s="139"/>
       <c r="AC22" s="139">
         <f>(W17-W18)*$E$36</f>
-        <v>457.14285714285717</v>
+        <v>463.768115942029</v>
       </c>
       <c r="AD22" s="139"/>
       <c r="AE22" s="139"/>
       <c r="AF22" s="139">
         <f>(Z17-Z18)*$E$36</f>
-        <v>914.28571428571433</v>
+        <v>927.536231884058</v>
       </c>
       <c r="AG22" s="139"/>
       <c r="AH22" s="139"/>
       <c r="AI22" s="139">
         <f>(AC17-AC18)*$E$36</f>
-        <v>1828.5714285714287</v>
+        <v>1855.072463768116</v>
       </c>
       <c r="AJ22" s="139"/>
       <c r="AK22" s="139"/>
       <c r="AL22" s="139">
         <f>(AF17-AF18)*$E$36</f>
-        <v>3657.1428571428573</v>
+        <v>3710.144927536232</v>
       </c>
       <c r="AM22" s="139"/>
       <c r="AN22" s="139"/>
       <c r="AO22" s="139">
         <f>(AI17-AI18)*$E$36</f>
-        <v>7314.2857142857147</v>
+        <v>7420.289855072464</v>
       </c>
       <c r="AP22" s="140"/>
       <c r="AQ22" s="81" t="s">
@@ -32100,49 +32112,49 @@
       <c r="S23" s="121"/>
       <c r="T23" s="52">
         <f>(N17-N18)*$E$37</f>
-        <v>34.285714285714285</v>
+        <v>34.782608695652172</v>
       </c>
       <c r="U23" s="52"/>
       <c r="V23" s="52"/>
       <c r="W23" s="52">
         <f>(Q17-Q18)*$E$37</f>
-        <v>68.571428571428569</v>
+        <v>69.565217391304344</v>
       </c>
       <c r="X23" s="52"/>
       <c r="Y23" s="52"/>
       <c r="Z23" s="52">
         <f>(T17-T18)*$E$37</f>
-        <v>137.14285714285714</v>
+        <v>139.13043478260869</v>
       </c>
       <c r="AA23" s="52"/>
       <c r="AB23" s="52"/>
       <c r="AC23" s="52">
         <f>(W17-W18)*$E$37</f>
-        <v>274.28571428571428</v>
+        <v>278.26086956521738</v>
       </c>
       <c r="AD23" s="52"/>
       <c r="AE23" s="52"/>
       <c r="AF23" s="52">
         <f>(Z17-Z18)*$E$37</f>
-        <v>548.57142857142856</v>
+        <v>556.52173913043475</v>
       </c>
       <c r="AG23" s="52"/>
       <c r="AH23" s="52"/>
       <c r="AI23" s="52">
         <f>(AC17-AC18)*$E$37</f>
-        <v>1097.1428571428571</v>
+        <v>1113.0434782608695</v>
       </c>
       <c r="AJ23" s="52"/>
       <c r="AK23" s="52"/>
       <c r="AL23" s="52">
         <f>(AF17-AF18)*$E$37</f>
-        <v>2194.2857142857142</v>
+        <v>2226.086956521739</v>
       </c>
       <c r="AM23" s="52"/>
       <c r="AN23" s="52"/>
       <c r="AO23" s="52">
         <f>(AI17-AI18)*$E$37</f>
-        <v>4388.5714285714284</v>
+        <v>4452.173913043478</v>
       </c>
       <c r="AP23" s="141"/>
       <c r="AQ23" s="59" t="s">
@@ -32175,43 +32187,43 @@
       <c r="U24" s="121"/>
       <c r="V24" s="122">
         <f>H21*$E$35</f>
-        <v>65.714285714285722</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="W24" s="122"/>
       <c r="X24" s="122"/>
       <c r="Y24" s="122">
         <f>K21*$E$35</f>
-        <v>131.42857142857144</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="Z24" s="122"/>
       <c r="AA24" s="122"/>
       <c r="AB24" s="122">
         <f>N21</f>
-        <v>262.85714285714289</v>
+        <v>266.66666666666669</v>
       </c>
       <c r="AC24" s="122"/>
       <c r="AD24" s="122"/>
       <c r="AE24" s="122">
         <f>Q21</f>
-        <v>525.71428571428578</v>
+        <v>533.33333333333337</v>
       </c>
       <c r="AF24" s="122"/>
       <c r="AG24" s="122"/>
       <c r="AH24" s="122">
         <f>T21</f>
-        <v>1051.4285714285716</v>
+        <v>1066.6666666666667</v>
       </c>
       <c r="AI24" s="122"/>
       <c r="AJ24" s="122"/>
       <c r="AK24" s="122">
         <f>W21</f>
-        <v>2037.1428571428573</v>
+        <v>2066.666666666667</v>
       </c>
       <c r="AL24" s="122"/>
       <c r="AM24" s="122"/>
       <c r="AN24" s="122">
         <f>Z21</f>
-        <v>4074.2857142857147</v>
+        <v>4133.3333333333339</v>
       </c>
       <c r="AO24" s="122"/>
       <c r="AP24" s="123"/>
@@ -32277,167 +32289,167 @@
       </c>
       <c r="B26" s="102">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>43960.943847916664</v>
+        <v>43964.917079166669</v>
       </c>
       <c r="C26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43961.943847916664</v>
+        <v>43965.917079166669</v>
       </c>
       <c r="D26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43962.943847916664</v>
+        <v>43966.917079166669</v>
       </c>
       <c r="E26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43963.943847916664</v>
+        <v>43967.917079166669</v>
       </c>
       <c r="F26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>43964.943847916664</v>
+        <v>43968.917079166669</v>
       </c>
       <c r="G26" s="104">
         <f t="shared" ca="1" si="0"/>
-        <v>43965.943847916664</v>
+        <v>43969.917079166669</v>
       </c>
       <c r="H26" s="103">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>43966.943847916664</v>
+        <v>43970.917079166669</v>
       </c>
       <c r="I26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43967.943847916664</v>
+        <v>43971.917079166669</v>
       </c>
       <c r="J26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43968.943847916664</v>
+        <v>43972.917079166669</v>
       </c>
       <c r="K26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43969.943847916664</v>
+        <v>43973.917079166669</v>
       </c>
       <c r="L26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43970.943847916664</v>
+        <v>43974.917079166669</v>
       </c>
       <c r="M26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43971.943847916664</v>
+        <v>43975.917079166669</v>
       </c>
       <c r="N26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>43972.943847916664</v>
+        <v>43976.917079166669</v>
       </c>
       <c r="O26" s="102">
         <f t="shared" ca="1" si="1"/>
-        <v>43973.943847916664</v>
+        <v>43977.917079166669</v>
       </c>
       <c r="P26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43974.943847916664</v>
+        <v>43978.917079166669</v>
       </c>
       <c r="Q26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43975.943847916664</v>
+        <v>43979.917079166669</v>
       </c>
       <c r="R26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43976.943847916664</v>
+        <v>43980.917079166669</v>
       </c>
       <c r="S26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43977.943847916664</v>
+        <v>43981.917079166669</v>
       </c>
       <c r="T26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>43978.943847916664</v>
+        <v>43982.917079166669</v>
       </c>
       <c r="U26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>43979.943847916664</v>
+        <v>43983.917079166669</v>
       </c>
       <c r="V26" s="102">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>43980.943847916664</v>
+        <v>43984.917079166669</v>
       </c>
       <c r="W26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43981.943847916664</v>
+        <v>43985.917079166669</v>
       </c>
       <c r="X26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43982.943847916664</v>
+        <v>43986.917079166669</v>
       </c>
       <c r="Y26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43983.943847916664</v>
+        <v>43987.917079166669</v>
       </c>
       <c r="Z26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43984.943847916664</v>
+        <v>43988.917079166669</v>
       </c>
       <c r="AA26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43985.943847916664</v>
+        <v>43989.917079166669</v>
       </c>
       <c r="AB26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>43986.943847916664</v>
+        <v>43990.917079166669</v>
       </c>
       <c r="AC26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>43987.943847916664</v>
+        <v>43991.917079166669</v>
       </c>
       <c r="AD26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43988.943847916664</v>
+        <v>43992.917079166669</v>
       </c>
       <c r="AE26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43989.943847916664</v>
+        <v>43993.917079166669</v>
       </c>
       <c r="AF26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43990.943847916664</v>
+        <v>43994.917079166669</v>
       </c>
       <c r="AG26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43991.943847916664</v>
+        <v>43995.917079166669</v>
       </c>
       <c r="AH26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43992.943847916664</v>
+        <v>43996.917079166669</v>
       </c>
       <c r="AI26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>43993.943847916664</v>
+        <v>43997.917079166669</v>
       </c>
       <c r="AJ26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>43994.943847916664</v>
+        <v>43998.917079166669</v>
       </c>
       <c r="AK26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43995.943847916664</v>
+        <v>43999.917079166669</v>
       </c>
       <c r="AL26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43996.943847916664</v>
+        <v>44000.917079166669</v>
       </c>
       <c r="AM26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43997.943847916664</v>
+        <v>44001.917079166669</v>
       </c>
       <c r="AN26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>43998.943847916664</v>
+        <v>44002.917079166669</v>
       </c>
       <c r="AO26" s="103">
         <f ca="1">AP26-1</f>
-        <v>43999.943847916664</v>
+        <v>44003.917079166669</v>
       </c>
       <c r="AP26" s="124">
         <f ca="1">NOW()</f>
-        <v>44000.943847916664</v>
+        <v>44004.917079166669</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -32683,7 +32695,7 @@
       <c r="D31" s="21"/>
       <c r="E31" s="97">
         <f>VLOOKUP(C31,B43:C54,2,FALSE)</f>
-        <v>1.4E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="21"/>
@@ -32728,7 +32740,7 @@
       <c r="D34" s="28"/>
       <c r="E34" s="154">
         <f>1-Projections!B37</f>
-        <v>0</v>
+        <v>-1.449275362318847E-2</v>
       </c>
       <c r="F34" s="28" t="s">
         <v>193</v>
@@ -32846,7 +32858,7 @@
       </c>
       <c r="C45" s="39">
         <f>Projections!B44</f>
-        <v>1.4E-2</v>
+        <v>1.38E-2</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -32955,8 +32967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BB0FAD-39ED-4D53-8BC6-75164ED434B0}">
   <dimension ref="A1:AJ117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V40" sqref="V40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33184,10 +33196,10 @@
       <c r="M16" s="59"/>
       <c r="N16" s="59"/>
       <c r="O16" s="59"/>
-      <c r="P16" s="301">
+      <c r="P16" s="296">
         <v>43949</v>
       </c>
-      <c r="Q16" s="302" t="s">
+      <c r="Q16" s="297" t="s">
         <v>299</v>
       </c>
       <c r="R16" s="59"/>
@@ -33204,10 +33216,10 @@
     </row>
     <row r="18" spans="15:19" x14ac:dyDescent="0.25">
       <c r="O18" s="278"/>
-      <c r="P18" s="299">
+      <c r="P18" s="294">
         <v>43961</v>
       </c>
-      <c r="Q18" s="300" t="s">
+      <c r="Q18" s="295" t="s">
         <v>307</v>
       </c>
       <c r="S18" s="181"/>
@@ -33289,10 +33301,10 @@
       </c>
     </row>
     <row r="28" spans="15:19" x14ac:dyDescent="0.25">
-      <c r="Q28" s="299">
+      <c r="Q28" s="294">
         <v>43983</v>
       </c>
-      <c r="R28" s="300" t="s">
+      <c r="R28" s="295" t="s">
         <v>318</v>
       </c>
     </row>
@@ -33329,19 +33341,19 @@
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="R33" s="278">
+      <c r="Q33" s="278">
         <v>43995</v>
       </c>
-      <c r="S33" t="s">
+      <c r="R33" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="S34" s="303">
-        <v>44025</v>
-      </c>
-      <c r="T34" s="304" t="s">
-        <v>323</v>
+      <c r="R34" s="278">
+        <v>44001</v>
+      </c>
+      <c r="S34" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
@@ -33354,11 +33366,11 @@
       <c r="C35" t="s">
         <v>151</v>
       </c>
-      <c r="S35" s="303">
-        <v>44032</v>
-      </c>
-      <c r="T35" s="304" t="s">
-        <v>324</v>
+      <c r="R35" s="278">
+        <v>44002</v>
+      </c>
+      <c r="S35" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
@@ -33368,6 +33380,12 @@
       <c r="B36" s="291">
         <v>1.4E-2</v>
       </c>
+      <c r="S36" s="298">
+        <v>44025</v>
+      </c>
+      <c r="T36" s="299" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
@@ -33375,10 +33393,16 @@
       </c>
       <c r="B37" s="170">
         <f>B36/B44</f>
-        <v>1</v>
+        <v>1.0144927536231885</v>
       </c>
       <c r="C37" t="s">
         <v>314</v>
+      </c>
+      <c r="S37" s="298">
+        <v>44032</v>
+      </c>
+      <c r="T37" s="299" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
@@ -33413,6 +33437,10 @@
         <f>(B35/100000)*B40</f>
         <v>1896.9159999999999</v>
       </c>
+      <c r="O40" s="191"/>
+      <c r="P40" s="191"/>
+      <c r="Q40" s="191"/>
+      <c r="R40" s="191"/>
       <c r="X40" s="134"/>
       <c r="Y40" s="278"/>
     </row>
@@ -33471,7 +33499,7 @@
         <v>214</v>
       </c>
       <c r="B44" s="77">
-        <v>1.4E-2</v>
+        <v>1.38E-2</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="194" t="s">
@@ -33618,52 +33646,52 @@
         <v>115</v>
       </c>
       <c r="F48" s="21"/>
-      <c r="G48" s="293">
+      <c r="G48" s="300">
         <v>43892</v>
       </c>
-      <c r="H48" s="294">
+      <c r="H48" s="301">
         <f>G48+HLOOKUP(G48+1, $B$47:$F$48,2,TRUE)</f>
         <v>43896</v>
       </c>
-      <c r="I48" s="294">
+      <c r="I48" s="301">
         <f t="shared" ref="I48:AC48" si="0">H48+HLOOKUP(H48+1, $B$47:$F$48,2,TRUE)</f>
         <v>43900</v>
       </c>
-      <c r="J48" s="294">
+      <c r="J48" s="301">
         <f t="shared" si="0"/>
         <v>43904</v>
       </c>
-      <c r="K48" s="294">
+      <c r="K48" s="301">
         <f t="shared" si="0"/>
         <v>43908</v>
       </c>
-      <c r="L48" s="295">
+      <c r="L48" s="302">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="M48" s="295">
+      <c r="M48" s="302">
         <f t="shared" si="0"/>
         <v>43914</v>
       </c>
-      <c r="N48" s="296">
+      <c r="N48" s="303">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="O48" s="297">
+      <c r="O48" s="304">
         <f>$N$48+(($T$48-$N$48)*(0.09))</f>
         <v>43929.35</v>
       </c>
-      <c r="P48" s="297">
+      <c r="P48" s="304">
         <f>$N$48+(($T$48-$N$48)*0.19)</f>
         <v>43940.85</v>
       </c>
-      <c r="Q48" s="298">
+      <c r="Q48" s="304">
         <f>$N$48+(($T$48-$N$48)*0.41)</f>
         <v>43966.15</v>
       </c>
-      <c r="R48" s="279">
-        <f>$N$48+(($T$48-$N$48)*0.75)</f>
-        <v>44005.25</v>
+      <c r="R48" s="293">
+        <f>$N$48+(($T$48-$N$48)*0.72)</f>
+        <v>44001.8</v>
       </c>
       <c r="S48" s="279">
         <f>$N$48+(($T$48-$N$48)*0.9)</f>
@@ -34029,7 +34057,7 @@
       </c>
       <c r="S51" s="253">
         <f t="shared" si="6"/>
-        <v>378.44490573917221</v>
+        <v>331.11979030206476</v>
       </c>
       <c r="T51" s="252">
         <f>MAX(T49-(T57-T58)-(T59-T60)-(T61-T62),0)</f>
@@ -34147,7 +34175,7 @@
       </c>
       <c r="S52" s="135">
         <f t="shared" si="10"/>
-        <v>7421.5550942608279</v>
+        <v>7468.8802096979352</v>
       </c>
       <c r="T52" s="270">
         <f>T49-T51</f>
@@ -34217,103 +34245,103 @@
       <c r="F53" s="21"/>
       <c r="G53" s="231">
         <f t="shared" ref="G53:AD53" si="12">G49/$B$37</f>
-        <v>31.25</v>
+        <v>30.803571428571427</v>
       </c>
       <c r="H53" s="232">
         <f t="shared" si="12"/>
-        <v>62.5</v>
+        <v>61.607142857142854</v>
       </c>
       <c r="I53" s="232">
         <f t="shared" si="12"/>
-        <v>125</v>
+        <v>123.21428571428571</v>
       </c>
       <c r="J53" s="232">
         <f t="shared" si="12"/>
-        <v>250</v>
+        <v>246.42857142857142</v>
       </c>
       <c r="K53" s="232">
         <f t="shared" si="12"/>
-        <v>500</v>
+        <v>492.85714285714283</v>
       </c>
       <c r="L53" s="231">
         <f t="shared" si="12"/>
-        <v>1000</v>
+        <v>985.71428571428567</v>
       </c>
       <c r="M53" s="232">
         <f t="shared" si="12"/>
-        <v>2000</v>
+        <v>1971.4285714285713</v>
       </c>
       <c r="N53" s="232">
         <f t="shared" si="12"/>
-        <v>4000</v>
+        <v>3942.8571428571427</v>
       </c>
       <c r="O53" s="231">
         <f t="shared" ref="O53:S53" si="13">O49/$B$37</f>
-        <v>6000</v>
+        <v>5914.2857142857138</v>
       </c>
       <c r="P53" s="232">
         <f t="shared" si="13"/>
-        <v>6600</v>
+        <v>6505.7142857142853</v>
       </c>
       <c r="Q53" s="232">
         <f t="shared" ref="Q53:R53" si="14">Q49/$B$37</f>
-        <v>7000</v>
+        <v>6900</v>
       </c>
       <c r="R53" s="232">
         <f t="shared" si="14"/>
-        <v>7400</v>
+        <v>7294.2857142857138</v>
       </c>
       <c r="S53" s="232">
         <f t="shared" si="13"/>
-        <v>7800</v>
+        <v>7688.5714285714284</v>
       </c>
       <c r="T53" s="231">
         <f t="shared" si="12"/>
-        <v>8000</v>
+        <v>7885.7142857142853</v>
       </c>
       <c r="U53" s="232">
         <f t="shared" si="12"/>
-        <v>16000</v>
+        <v>15771.428571428571</v>
       </c>
       <c r="V53" s="232">
         <f t="shared" si="12"/>
-        <v>32000</v>
+        <v>31542.857142857141</v>
       </c>
       <c r="W53" s="232">
         <f t="shared" si="12"/>
-        <v>64000</v>
+        <v>63085.714285714283</v>
       </c>
       <c r="X53" s="232">
         <f t="shared" si="12"/>
-        <v>128000</v>
+        <v>126171.42857142857</v>
       </c>
       <c r="Y53" s="232">
         <f t="shared" si="12"/>
-        <v>256000</v>
+        <v>252342.85714285713</v>
       </c>
       <c r="Z53" s="232">
         <f t="shared" si="12"/>
-        <v>512000</v>
+        <v>504685.71428571426</v>
       </c>
       <c r="AA53" s="232">
         <f t="shared" si="12"/>
-        <v>1024000</v>
+        <v>1009371.4285714285</v>
       </c>
       <c r="AB53" s="232">
         <f t="shared" si="12"/>
-        <v>2048000</v>
+        <v>2018742.857142857</v>
       </c>
       <c r="AC53" s="232">
         <f t="shared" si="12"/>
-        <v>4096000</v>
+        <v>4037485.7142857141</v>
       </c>
       <c r="AD53" s="240">
         <f t="shared" si="12"/>
-        <v>8192000</v>
+        <v>8074971.4285714282</v>
       </c>
       <c r="AE53" s="267">
         <f>AE49/$B$37</f>
-        <v>16384000</v>
+        <v>16149942.857142856</v>
       </c>
       <c r="AF53" s="215">
         <f>AF49</f>
@@ -34321,7 +34349,7 @@
       </c>
       <c r="AG53" s="243">
         <f>($B$35*$B$38)/$B$37</f>
-        <v>5126800</v>
+        <v>5053560</v>
       </c>
       <c r="AH53" s="37"/>
       <c r="AI53" s="37"/>
@@ -34338,110 +34366,110 @@
       <c r="F54" s="28"/>
       <c r="G54" s="210">
         <f>G53/$B$35</f>
-        <v>1.2190840290239525E-6</v>
+        <v>1.2016685428950388E-6</v>
       </c>
       <c r="H54" s="78">
         <f t="shared" ref="H54:AD54" si="15">H53/$B$35</f>
-        <v>2.438168058047905E-6</v>
+        <v>2.4033370857900777E-6</v>
       </c>
       <c r="I54" s="78">
         <f t="shared" si="15"/>
-        <v>4.87633611609581E-6</v>
+        <v>4.8066741715801554E-6</v>
       </c>
       <c r="J54" s="48">
         <f t="shared" si="15"/>
-        <v>9.7526722321916199E-6</v>
+        <v>9.6133483431603108E-6</v>
       </c>
       <c r="K54" s="48">
         <f t="shared" si="15"/>
-        <v>1.950534446438324E-5</v>
+        <v>1.9226696686320622E-5</v>
       </c>
       <c r="L54" s="101">
         <f t="shared" si="15"/>
-        <v>3.901068892876648E-5</v>
+        <v>3.8453393372641243E-5</v>
       </c>
       <c r="M54" s="48">
         <f t="shared" si="15"/>
-        <v>7.8021377857532959E-5</v>
+        <v>7.6906786745282486E-5</v>
       </c>
       <c r="N54" s="26">
         <f t="shared" si="15"/>
-        <v>1.5604275571506592E-4</v>
+        <v>1.5381357349056497E-4</v>
       </c>
       <c r="O54" s="18">
         <f t="shared" ref="O54:S54" si="16">O53/$B$35</f>
-        <v>2.3406413357259889E-4</v>
+        <v>2.3072036023584746E-4</v>
       </c>
       <c r="P54" s="26">
         <f t="shared" si="16"/>
-        <v>2.5747054692985876E-4</v>
+        <v>2.5379239625943219E-4</v>
       </c>
       <c r="Q54" s="26">
         <f t="shared" ref="Q54:R54" si="17">Q53/$B$35</f>
-        <v>2.7307482250136535E-4</v>
+        <v>2.691737536084887E-4</v>
       </c>
       <c r="R54" s="26">
         <f t="shared" si="17"/>
-        <v>2.8867909807287195E-4</v>
+        <v>2.8455511095754521E-4</v>
       </c>
       <c r="S54" s="26">
         <f t="shared" si="16"/>
-        <v>3.0428337364437854E-4</v>
+        <v>2.9993646830660172E-4</v>
       </c>
       <c r="T54" s="20">
         <f t="shared" si="15"/>
-        <v>3.1208551143013184E-4</v>
+        <v>3.0762714698112995E-4</v>
       </c>
       <c r="U54" s="27">
         <f t="shared" si="15"/>
-        <v>6.2417102286026367E-4</v>
+        <v>6.1525429396225989E-4</v>
       </c>
       <c r="V54" s="27">
         <f t="shared" si="15"/>
-        <v>1.2483420457205273E-3</v>
+        <v>1.2305085879245198E-3</v>
       </c>
       <c r="W54" s="27">
         <f t="shared" si="15"/>
-        <v>2.4966840914410547E-3</v>
+        <v>2.4610171758490396E-3</v>
       </c>
       <c r="X54" s="27">
         <f t="shared" si="15"/>
-        <v>4.9933681828821094E-3</v>
+        <v>4.9220343516980791E-3</v>
       </c>
       <c r="Y54" s="87">
         <f t="shared" si="15"/>
-        <v>9.9867363657642188E-3</v>
+        <v>9.8440687033961582E-3</v>
       </c>
       <c r="Z54" s="87">
         <f t="shared" si="15"/>
-        <v>1.9973472731528438E-2</v>
+        <v>1.9688137406792316E-2</v>
       </c>
       <c r="AA54" s="87">
         <f t="shared" si="15"/>
-        <v>3.9946945463056875E-2</v>
+        <v>3.9376274813584633E-2</v>
       </c>
       <c r="AB54" s="87">
         <f t="shared" si="15"/>
-        <v>7.989389092611375E-2</v>
+        <v>7.8752549627169266E-2</v>
       </c>
       <c r="AC54" s="87">
         <f t="shared" si="15"/>
-        <v>0.1597877818522275</v>
+        <v>0.15750509925433853</v>
       </c>
       <c r="AD54" s="269">
         <f t="shared" si="15"/>
-        <v>0.319575563704455</v>
+        <v>0.31501019850867706</v>
       </c>
       <c r="AE54" s="266">
         <f>AE53/$B$35</f>
-        <v>0.63915112740891</v>
+        <v>0.63002039701735413</v>
       </c>
       <c r="AF54" s="193">
         <v>1</v>
       </c>
       <c r="AG54" s="242">
         <f>AG53/B35</f>
-        <v>0.2</v>
+        <v>0.19714285714285715</v>
       </c>
       <c r="AH54" s="37"/>
       <c r="AI54" s="37"/>
@@ -34458,103 +34486,103 @@
       <c r="F55" s="28"/>
       <c r="G55" s="212">
         <f t="shared" ref="G55:AD55" si="18">G53-G49</f>
-        <v>0</v>
+        <v>-0.44642857142857295</v>
       </c>
       <c r="H55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-0.8928571428571459</v>
       </c>
       <c r="I55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-1.7857142857142918</v>
       </c>
       <c r="J55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-3.5714285714285836</v>
       </c>
       <c r="K55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-7.1428571428571672</v>
       </c>
       <c r="L55" s="212">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-14.285714285714334</v>
       </c>
       <c r="M55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-28.571428571428669</v>
       </c>
       <c r="N55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-57.142857142857338</v>
       </c>
       <c r="O55" s="212">
         <f t="shared" ref="O55:S55" si="19">O53-O49</f>
-        <v>0</v>
+        <v>-85.714285714286234</v>
       </c>
       <c r="P55" s="213">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>-94.285714285714675</v>
       </c>
       <c r="Q55" s="213">
         <f t="shared" ref="Q55:R55" si="20">Q53-Q49</f>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="R55" s="213">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>-105.71428571428623</v>
       </c>
       <c r="S55" s="213">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>-111.42857142857156</v>
       </c>
       <c r="T55" s="212">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-114.28571428571468</v>
       </c>
       <c r="U55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-228.57142857142935</v>
       </c>
       <c r="V55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-457.1428571428587</v>
       </c>
       <c r="W55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-914.2857142857174</v>
       </c>
       <c r="X55" s="213">
         <f>X53-X49</f>
-        <v>0</v>
+        <v>-1828.5714285714348</v>
       </c>
       <c r="Y55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-3657.1428571428696</v>
       </c>
       <c r="Z55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-7314.2857142857392</v>
       </c>
       <c r="AA55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-14628.571428571478</v>
       </c>
       <c r="AB55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-29257.142857142957</v>
       </c>
       <c r="AC55" s="213">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-58514.285714285914</v>
       </c>
       <c r="AD55" s="214">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>-117028.57142857183</v>
       </c>
       <c r="AE55" s="267">
         <f>AE53</f>
-        <v>16384000</v>
+        <v>16149942.857142856</v>
       </c>
       <c r="AF55" s="215">
         <f>AF53</f>
@@ -34562,7 +34590,7 @@
       </c>
       <c r="AG55" s="245">
         <f>AG53-AG49</f>
-        <v>0</v>
+        <v>-73240</v>
       </c>
       <c r="AH55" s="37"/>
       <c r="AI55" s="37"/>
@@ -34579,103 +34607,103 @@
       <c r="F56" s="51"/>
       <c r="G56" s="216">
         <f>MIN((1/$B$37)*(2^(((G48 - 14) - $B$45)/$G$74)),G55)</f>
-        <v>0</v>
+        <v>-0.44642857142857295</v>
       </c>
       <c r="H56" s="217">
         <f>MIN((1/$B$37)*(2^(((H48 - 14) - $B$45)/$G$74)),H55)</f>
-        <v>0</v>
+        <v>-0.8928571428571459</v>
       </c>
       <c r="I56" s="217">
         <f t="shared" ref="I56:J56" si="21">MIN((1/$B$37)*(2^(((I48 - 14) - $B$45)/$G$74)),I55)</f>
-        <v>0</v>
+        <v>-1.7857142857142918</v>
       </c>
       <c r="J56" s="217">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>-3.5714285714285836</v>
       </c>
       <c r="K56" s="219">
         <f t="shared" ref="K56:AF56" si="22">MIN(($G$49/$B$37)*(2^(((K48 - 14) - $G$48)/HLOOKUP((K48-14)-$B$45,$G$72:$AG$74,3,TRUE))),K55)</f>
-        <v>0</v>
+        <v>-7.1428571428571672</v>
       </c>
       <c r="L56" s="220">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-14.285714285714334</v>
       </c>
       <c r="M56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-28.571428571428669</v>
       </c>
       <c r="N56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-57.142857142857338</v>
       </c>
       <c r="O56" s="220">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-85.714285714286234</v>
       </c>
       <c r="P56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-94.285714285714675</v>
       </c>
       <c r="Q56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="R56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-105.71428571428623</v>
       </c>
       <c r="S56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-111.42857142857156</v>
       </c>
       <c r="T56" s="220">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-114.28571428571468</v>
       </c>
       <c r="U56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-228.57142857142935</v>
       </c>
       <c r="V56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-457.1428571428587</v>
       </c>
       <c r="W56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-914.2857142857174</v>
       </c>
       <c r="X56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-1828.5714285714348</v>
       </c>
       <c r="Y56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-3657.1428571428696</v>
       </c>
       <c r="Z56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-7314.2857142857392</v>
       </c>
       <c r="AA56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-14628.571428571478</v>
       </c>
       <c r="AB56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-29257.142857142957</v>
       </c>
       <c r="AC56" s="219">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-58514.285714285914</v>
       </c>
       <c r="AD56" s="218">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-117028.57142857183</v>
       </c>
       <c r="AE56" s="267">
         <f t="shared" si="22"/>
-        <v>16384000</v>
+        <v>16149942.857142856</v>
       </c>
       <c r="AF56" s="221">
         <f t="shared" si="22"/>
@@ -34980,11 +35008,11 @@
       </c>
       <c r="R59" s="284">
         <f t="shared" si="27"/>
-        <v>5412.5731227783745</v>
+        <v>4217.9293984147635</v>
       </c>
       <c r="S59" s="284">
         <f t="shared" si="27"/>
-        <v>914.98907768335982</v>
+        <v>1102.9505029517011</v>
       </c>
       <c r="T59" s="285">
         <f t="shared" si="27"/>
@@ -35101,11 +35129,11 @@
       </c>
       <c r="R60" s="219">
         <f t="shared" si="31"/>
-        <v>4188.839639512581</v>
+        <v>3264.2939799538044</v>
       </c>
       <c r="S60" s="219">
         <f t="shared" si="30"/>
-        <v>669.43398342253204</v>
+        <v>810.07029325376584</v>
       </c>
       <c r="T60" s="220">
         <f t="shared" ref="T60:AF60" si="32">MAX(T59-($G$49*$B$42)*(2^(((T48 - 42) - $G$48)/HLOOKUP((T48-42)-$B$45,$G$72:$AG$74,3,TRUE)))-T62,0)</f>
@@ -35218,15 +35246,15 @@
       </c>
       <c r="R61" s="284">
         <f t="shared" si="33"/>
-        <v>1223.7334832657932</v>
+        <v>953.63541846095893</v>
       </c>
       <c r="S61" s="284">
         <f t="shared" si="33"/>
-        <v>245.55509426082781</v>
+        <v>292.88020969793524</v>
       </c>
       <c r="T61" s="285">
         <f t="shared" si="33"/>
-        <v>425.45455935549376</v>
+        <v>516.35670124040007</v>
       </c>
       <c r="U61" s="232">
         <f t="shared" si="33"/>
@@ -35339,11 +35367,11 @@
       </c>
       <c r="R62" s="219">
         <f t="shared" si="37"/>
-        <v>1223.7334832657932</v>
+        <v>953.63541846095893</v>
       </c>
       <c r="S62" s="219">
         <f t="shared" si="36"/>
-        <v>245.55509426082781</v>
+        <v>292.88020969793524</v>
       </c>
       <c r="T62" s="224">
         <f t="shared" ref="T62:AF62" si="38">MAX(T61-($G$49*$B$43)*(2^(((T48 - 35) - $G$48)/HLOOKUP((T48-35)-$B$45,$G$72:$AG$74,3,TRUE))),0)</f>
@@ -35413,111 +35441,111 @@
       <c r="F63" s="21"/>
       <c r="G63" s="225">
         <f t="shared" ref="G63:AF63" si="39">G49*$B$44</f>
-        <v>0.4375</v>
+        <v>0.43124999999999997</v>
       </c>
       <c r="H63" s="226">
         <f t="shared" si="39"/>
-        <v>0.875</v>
+        <v>0.86249999999999993</v>
       </c>
       <c r="I63" s="226">
         <f t="shared" si="39"/>
-        <v>1.75</v>
+        <v>1.7249999999999999</v>
       </c>
       <c r="J63" s="226">
         <f t="shared" si="39"/>
-        <v>3.5</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="K63" s="226">
         <f t="shared" si="39"/>
-        <v>7</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="L63" s="225">
         <f t="shared" si="39"/>
-        <v>14</v>
+        <v>13.799999999999999</v>
       </c>
       <c r="M63" s="226">
         <f t="shared" si="39"/>
-        <v>28</v>
+        <v>27.599999999999998</v>
       </c>
       <c r="N63" s="226">
         <f t="shared" si="39"/>
-        <v>56</v>
+        <v>55.199999999999996</v>
       </c>
       <c r="O63" s="225">
         <f t="shared" ref="O63:S63" si="40">O49*$B$44</f>
-        <v>84</v>
+        <v>82.8</v>
       </c>
       <c r="P63" s="226">
         <f t="shared" si="40"/>
-        <v>92.4</v>
+        <v>91.08</v>
       </c>
       <c r="Q63" s="226">
         <f t="shared" ref="Q63:R63" si="41">Q49*$B$44</f>
-        <v>98</v>
+        <v>96.6</v>
       </c>
       <c r="R63" s="226">
         <f t="shared" si="41"/>
-        <v>103.60000000000001</v>
+        <v>102.12</v>
       </c>
       <c r="S63" s="226">
         <f t="shared" si="40"/>
-        <v>109.2</v>
+        <v>107.64</v>
       </c>
       <c r="T63" s="225">
         <f t="shared" si="39"/>
-        <v>112</v>
+        <v>110.39999999999999</v>
       </c>
       <c r="U63" s="226">
         <f t="shared" si="39"/>
-        <v>224</v>
+        <v>220.79999999999998</v>
       </c>
       <c r="V63" s="226">
         <f t="shared" si="39"/>
-        <v>448</v>
+        <v>441.59999999999997</v>
       </c>
       <c r="W63" s="226">
         <f t="shared" si="39"/>
-        <v>896</v>
+        <v>883.19999999999993</v>
       </c>
       <c r="X63" s="226">
         <f t="shared" si="39"/>
-        <v>1792</v>
+        <v>1766.3999999999999</v>
       </c>
       <c r="Y63" s="226">
         <f t="shared" si="39"/>
-        <v>3584</v>
+        <v>3532.7999999999997</v>
       </c>
       <c r="Z63" s="226">
         <f t="shared" si="39"/>
-        <v>7168</v>
+        <v>7065.5999999999995</v>
       </c>
       <c r="AA63" s="226">
         <f t="shared" si="39"/>
-        <v>14336</v>
+        <v>14131.199999999999</v>
       </c>
       <c r="AB63" s="226">
         <f t="shared" si="39"/>
-        <v>28672</v>
+        <v>28262.399999999998</v>
       </c>
       <c r="AC63" s="226">
         <f t="shared" si="39"/>
-        <v>57344</v>
+        <v>56524.799999999996</v>
       </c>
       <c r="AD63" s="227">
         <f t="shared" si="39"/>
-        <v>114688</v>
+        <v>113049.59999999999</v>
       </c>
       <c r="AE63" s="267">
         <f t="shared" si="39"/>
-        <v>229376</v>
+        <v>226099.19999999998</v>
       </c>
       <c r="AF63" s="222">
         <f t="shared" si="39"/>
-        <v>358876</v>
+        <v>353749.2</v>
       </c>
       <c r="AG63" s="243">
         <f>AG49*B44</f>
-        <v>71775.199999999997</v>
+        <v>70749.84</v>
       </c>
       <c r="AH63" s="57"/>
       <c r="AI63" s="57"/>
@@ -35541,83 +35569,83 @@
       <c r="M64" s="217"/>
       <c r="N64" s="229">
         <f>($G$49*$B$44)*(2^(((N48-35)-$G$48)/$G$74))</f>
-        <v>0.2054237812312126</v>
+        <v>0.20248915578505242</v>
       </c>
       <c r="O64" s="230">
         <f t="shared" ref="O64:S64" si="42">($G$49*$B$44)*(2^(((O48-35)-$G$48)/$G$74))</f>
-        <v>0.54629121045943951</v>
+        <v>0.53848705031001898</v>
       </c>
       <c r="P64" s="229">
         <f t="shared" si="42"/>
-        <v>1.6195514970756304</v>
+        <v>1.596415047117407</v>
       </c>
       <c r="Q64" s="229">
         <f t="shared" ref="Q64:R64" si="43">($G$49*$B$44)*(2^(((Q48-35)-$G$48)/$G$74))</f>
-        <v>17.690087026044658</v>
+        <v>17.437371497101161</v>
       </c>
       <c r="R64" s="229">
         <f t="shared" si="43"/>
-        <v>711.91777364932</v>
+        <v>506.51197992986778</v>
       </c>
       <c r="S64" s="229">
         <f t="shared" si="42"/>
-        <v>3634.0061582451863</v>
+        <v>3582.0917845559693</v>
       </c>
       <c r="T64" s="230">
         <f t="shared" ref="T64:AF64" si="44">($G$49*$B$44)*(2^(((T48-35)-$G$48)/HLOOKUP((T48-35)-$B$45,$G$72:$AG$74,3,TRUE)))</f>
-        <v>999.9683985448753</v>
+        <v>985.68313570851979</v>
       </c>
       <c r="U64" s="229">
         <f t="shared" si="44"/>
-        <v>2338.7146148429342</v>
+        <v>2305.3044060594634</v>
       </c>
       <c r="V64" s="229">
         <f t="shared" si="44"/>
-        <v>1454.0201228155479</v>
+        <v>1433.2484067753255</v>
       </c>
       <c r="W64" s="229">
         <f t="shared" si="44"/>
-        <v>1861.6644940390759</v>
+        <v>1835.0692869813745</v>
       </c>
       <c r="X64" s="229">
         <f t="shared" si="44"/>
-        <v>2942.4726433180176</v>
+        <v>2900.4373198420453</v>
       </c>
       <c r="Y64" s="229">
         <f t="shared" si="44"/>
-        <v>5088.3527835524346</v>
+        <v>5015.6620295016855</v>
       </c>
       <c r="Z64" s="229">
         <f t="shared" si="44"/>
-        <v>9219.4326745938088</v>
+        <v>9087.7264935281819</v>
       </c>
       <c r="AA64" s="229">
         <f t="shared" si="44"/>
-        <v>17166.880665322838</v>
+        <v>16921.639512961083</v>
       </c>
       <c r="AB64" s="229">
         <f t="shared" si="44"/>
-        <v>32525.053102412145</v>
+        <v>32060.409486663397</v>
       </c>
       <c r="AC64" s="229">
         <f t="shared" si="44"/>
-        <v>62349.765442214062</v>
+        <v>61459.054507325287</v>
       </c>
       <c r="AD64" s="228">
         <f t="shared" si="44"/>
-        <v>120517.41072133348</v>
+        <v>118795.73342531442</v>
       </c>
       <c r="AE64" s="268">
         <f t="shared" si="44"/>
-        <v>234370.04903118958</v>
+        <v>231021.90547360116</v>
       </c>
       <c r="AF64" s="221">
         <f t="shared" si="44"/>
-        <v>457873.06298719335</v>
+        <v>451332.01923023345</v>
       </c>
       <c r="AG64" s="246">
         <f>($G$49*$B$44)*(2^(((AG48 - 35) - $G$48)/AG74))</f>
-        <v>251555.45452232275</v>
+        <v>247961.80517200381</v>
       </c>
       <c r="AH64" s="57"/>
       <c r="AI64" s="57"/>
@@ -36096,7 +36124,7 @@
       </c>
       <c r="R71" s="155">
         <f t="shared" si="51"/>
-        <v>21.464285714285715</v>
+        <v>20.971428571428987</v>
       </c>
       <c r="S71" s="155">
         <f t="shared" si="50"/>
@@ -36214,7 +36242,7 @@
       </c>
       <c r="R72" s="259">
         <f t="shared" si="54"/>
-        <v>150.25</v>
+        <v>146.80000000000291</v>
       </c>
       <c r="S72" s="259">
         <f t="shared" si="53"/>
@@ -36319,9 +36347,8 @@
       <c r="Q73" s="162">
         <v>7019</v>
       </c>
-      <c r="R73" s="198">
-        <f>R49</f>
-        <v>7400</v>
+      <c r="R73" s="162">
+        <v>7409</v>
       </c>
       <c r="S73" s="198">
         <f>S49</f>
@@ -36437,9 +36464,9 @@
         <f>(Q48-$G$48)/(LOG(Q73/$G$73)/LOG(2))</f>
         <v>9.5892023611624104</v>
       </c>
-      <c r="R74" s="199">
+      <c r="R74" s="190">
         <f>(R48-$G$48)/(LOG(R73/$G$73)/LOG(2))</f>
-        <v>14.50265416849677</v>
+        <v>14.057694675568982</v>
       </c>
       <c r="S74" s="199">
         <f>(S48-$G$48)/(LOG(S73/$G$73)/LOG(2))</f>
@@ -36544,7 +36571,9 @@
       <c r="Q75" s="262">
         <v>584</v>
       </c>
-      <c r="R75" s="263"/>
+      <c r="R75" s="262">
+        <v>429</v>
+      </c>
       <c r="S75" s="263"/>
       <c r="T75" s="263"/>
       <c r="U75" s="263"/>
@@ -36611,13 +36640,16 @@
         <v>4230</v>
       </c>
       <c r="Q76" s="163">
-        <f t="shared" ref="Q76" si="61">Q73-Q75-Q77</f>
+        <f t="shared" ref="Q76:R76" si="61">Q73-Q75-Q77</f>
         <v>6337</v>
       </c>
-      <c r="R76" s="249">
-        <v>6877</v>
-      </c>
-      <c r="S76" s="249"/>
+      <c r="R76" s="163">
+        <f t="shared" si="61"/>
+        <v>6878</v>
+      </c>
+      <c r="S76" s="249">
+        <v>6903</v>
+      </c>
       <c r="T76" s="249"/>
       <c r="U76" s="200"/>
       <c r="V76" s="200"/>
@@ -36675,10 +36707,12 @@
       <c r="Q77" s="64">
         <v>98</v>
       </c>
-      <c r="R77" s="250">
+      <c r="R77" s="64">
         <v>102</v>
       </c>
-      <c r="S77" s="250"/>
+      <c r="S77" s="250">
+        <v>102</v>
+      </c>
       <c r="T77" s="250"/>
       <c r="U77" s="201"/>
       <c r="V77" s="201"/>
@@ -41090,7 +41124,7 @@
         <v>221</v>
       </c>
       <c r="C6" s="179">
-        <v>7391</v>
+        <v>7474</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -41099,7 +41133,7 @@
       </c>
       <c r="C7" s="177">
         <f ca="1">NOW()</f>
-        <v>44000.943847916664</v>
+        <v>44004.917079166669</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -41108,7 +41142,7 @@
       </c>
       <c r="C8" s="178">
         <f ca="1">C7-C5</f>
-        <v>108.9438479166638</v>
+        <v>112.91707916666928</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -41117,7 +41151,7 @@
       </c>
       <c r="C9" s="180">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>13.875450628119532</v>
+        <v>14.352044900579227</v>
       </c>
       <c r="D9" t="s">
         <v>197</v>
@@ -41150,7 +41184,7 @@
       </c>
       <c r="C12" s="185">
         <f>C6/Projections!B37</f>
-        <v>7391</v>
+        <v>7367.2285714285708</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -41159,7 +41193,7 @@
       </c>
       <c r="C13" s="186">
         <f ca="1">(C4/Projections!B37)*(2^(((C7-21)-C5)/C9))</f>
-        <v>2588.8389413809541</v>
+        <v>2671.9923528723762</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -41168,7 +41202,7 @@
       </c>
       <c r="C14" s="165">
         <f ca="1">C12-C13</f>
-        <v>4802.1610586190454</v>
+        <v>4695.2362185561942</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" s="183" t="s">
@@ -41182,7 +41216,7 @@
       </c>
       <c r="C15" s="76">
         <f>C6*Projections!B41</f>
-        <v>6799.72</v>
+        <v>6876.08</v>
       </c>
       <c r="I15" s="176"/>
     </row>
@@ -41192,7 +41226,7 @@
       </c>
       <c r="C16" s="95">
         <f ca="1">(C4*Projections!B41)*(2^(((C7-21)-C5)/C9))</f>
-        <v>2381.7318260704778</v>
+        <v>2493.8595293475514</v>
       </c>
       <c r="I16" s="176"/>
     </row>
@@ -41202,7 +41236,7 @@
       </c>
       <c r="C17" s="95">
         <f ca="1">C15-C16</f>
-        <v>4417.9881739295224</v>
+        <v>4382.2204706524481</v>
       </c>
       <c r="F17" t="s">
         <v>246</v>
@@ -41215,7 +41249,7 @@
       </c>
       <c r="C18" s="76">
         <f>C6*Projections!B42</f>
-        <v>369.55</v>
+        <v>373.70000000000005</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -41224,7 +41258,7 @@
       </c>
       <c r="C19" s="95">
         <f ca="1">(C4*Projections!B42)*(2^(((C7-49)-C5)/C9))</f>
-        <v>31.960297320178814</v>
+        <v>35.055991372556278</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -41233,7 +41267,7 @@
       </c>
       <c r="C20" s="95">
         <f ca="1">C18-C19</f>
-        <v>337.58970267982119</v>
+        <v>338.64400862744378</v>
       </c>
       <c r="F20" t="s">
         <v>251</v>
@@ -41245,7 +41279,7 @@
       </c>
       <c r="C21" s="76">
         <f>C6*Projections!B43</f>
-        <v>221.73</v>
+        <v>224.22</v>
       </c>
       <c r="I21" s="176"/>
     </row>
@@ -41255,7 +41289,7 @@
       </c>
       <c r="C22" s="95">
         <f ca="1">(C4*Projections!B43)*(2^(((C7-49)-C5)/C9))</f>
-        <v>19.176178392107285</v>
+        <v>21.033594823533765</v>
       </c>
       <c r="I22" s="176"/>
     </row>
@@ -41265,7 +41299,7 @@
       </c>
       <c r="C23" s="95">
         <f ca="1">C21-C22</f>
-        <v>202.5538216078927</v>
+        <v>203.18640517646622</v>
       </c>
       <c r="I23" s="176"/>
     </row>
@@ -41275,7 +41309,7 @@
       </c>
       <c r="C24" s="76">
         <f>C6*Projections!B44</f>
-        <v>103.474</v>
+        <v>103.1412</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -41284,7 +41318,7 @@
       </c>
       <c r="C25" s="73">
         <f ca="1">(C4*Projections!B44)*(2^(((C7-42)-C5)/C9))</f>
-        <v>12.695064118758825</v>
+        <v>13.567327646240859</v>
       </c>
       <c r="F25" t="s">
         <v>257</v>
@@ -41296,7 +41330,7 @@
       </c>
       <c r="C26" s="189">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>114.21747091833404</v>
+        <v>117.90938938071127</v>
       </c>
       <c r="D26" t="s">
         <v>197</v>
@@ -41311,7 +41345,7 @@
       </c>
       <c r="C27" s="188">
         <f ca="1">C7+C26</f>
-        <v>44115.161318834995</v>
+        <v>44122.826468547384</v>
       </c>
       <c r="F27" t="s">
         <v>259</v>
@@ -41323,7 +41357,7 @@
       </c>
       <c r="C28" s="187">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>42.96921673966483</v>
+        <v>44.213898656405789</v>
       </c>
       <c r="D28" t="s">
         <v>197</v>
@@ -41335,7 +41369,7 @@
       </c>
       <c r="C29" s="188">
         <f ca="1">C7+C28</f>
-        <v>44043.913064656328</v>
+        <v>44049.130977823072</v>
       </c>
       <c r="F29" t="s">
         <v>259</v>
@@ -41347,7 +41381,7 @@
       </c>
       <c r="C30" s="187">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>152.94958943006205</v>
+        <v>158.26980730813665</v>
       </c>
       <c r="D30" t="s">
         <v>197</v>
@@ -41359,7 +41393,7 @@
       </c>
       <c r="C31" s="188">
         <f ca="1">C7+C30</f>
-        <v>44153.893437346727</v>
+        <v>44163.186886474803</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -41368,7 +41402,7 @@
       </c>
       <c r="C34" s="177">
         <f ca="1">C7+30</f>
-        <v>44030.943847916664</v>
+        <v>44034.917079166669</v>
       </c>
       <c r="F34" t="s">
         <v>278</v>
@@ -41380,7 +41414,7 @@
       </c>
       <c r="C35" s="95">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>33079.408125427224</v>
+        <v>31826.906398407533</v>
       </c>
       <c r="F35" t="s">
         <v>244</v>
@@ -41392,7 +41426,7 @@
       </c>
       <c r="C36" s="95">
         <f ca="1">C35/Projections!B37</f>
-        <v>33079.408125427224</v>
+        <v>31372.236307001709</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -41401,7 +41435,7 @@
       </c>
       <c r="C37" s="95">
         <f ca="1">C35*Projections!B41</f>
-        <v>30433.055475393048</v>
+        <v>29280.753886534931</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -41410,7 +41444,7 @@
       </c>
       <c r="C38" s="95">
         <f ca="1">C35*Projections!B42</f>
-        <v>1653.9704062713613</v>
+        <v>1591.3453199203768</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -41419,7 +41453,7 @@
       </c>
       <c r="C39" s="95">
         <f ca="1">C35*Projections!B43</f>
-        <v>992.38224376281664</v>
+        <v>954.80719195222593</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -41428,7 +41462,7 @@
       </c>
       <c r="C40" s="73">
         <f ca="1">C35*Projections!B44</f>
-        <v>463.11171375598116</v>
+        <v>439.21130829802394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
State of Covid after Trumps term ends
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B309645F-F9EC-4A56-AE14-057C765329DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DBE198-2D9B-4831-B303-EB602F7FF5D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
+    <workbookView xWindow="2910" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -2299,46 +2299,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2448,46 +2448,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2597,46 +2597,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4075,7 +4075,7 @@
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="#,##0">
-                  <c:v>908</c:v>
+                  <c:v>909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14373,7 +14373,7 @@
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="#,##0">
-                  <c:v>908</c:v>
+                  <c:v>909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14702,46 +14702,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14842,46 +14842,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14985,46 +14985,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15122,46 +15122,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15529,46 +15529,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15678,46 +15678,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15827,46 +15827,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16244,46 +16244,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16384,46 +16384,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16527,46 +16527,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16664,46 +16664,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44149.732850462962</c:v>
+                  <c:v>44178.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44152.732850462962</c:v>
+                  <c:v>44181.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44155.732850462962</c:v>
+                  <c:v>44184.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44158.732850462962</c:v>
+                  <c:v>44187.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44161.732850462962</c:v>
+                  <c:v>44190.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44164.732850462962</c:v>
+                  <c:v>44193.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44167.732850462962</c:v>
+                  <c:v>44196.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44170.732850462962</c:v>
+                  <c:v>44199.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44173.732850462962</c:v>
+                  <c:v>44202.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44176.732850462962</c:v>
+                  <c:v>44205.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44179.732850462962</c:v>
+                  <c:v>44208.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44182.732850462962</c:v>
+                  <c:v>44211.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44185.732850462962</c:v>
+                  <c:v>44214.892302199078</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44188.732850462962</c:v>
+                  <c:v>44217.892302199078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -37611,167 +37611,167 @@
       </c>
       <c r="B26" s="102">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>44149.732850462962</v>
+        <v>44178.892302199078</v>
       </c>
       <c r="C26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44150.732850462962</v>
+        <v>44179.892302199078</v>
       </c>
       <c r="D26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44151.732850462962</v>
+        <v>44180.892302199078</v>
       </c>
       <c r="E26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44152.732850462962</v>
+        <v>44181.892302199078</v>
       </c>
       <c r="F26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44153.732850462962</v>
+        <v>44182.892302199078</v>
       </c>
       <c r="G26" s="104">
         <f t="shared" ca="1" si="0"/>
-        <v>44154.732850462962</v>
+        <v>44183.892302199078</v>
       </c>
       <c r="H26" s="103">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>44155.732850462962</v>
+        <v>44184.892302199078</v>
       </c>
       <c r="I26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44156.732850462962</v>
+        <v>44185.892302199078</v>
       </c>
       <c r="J26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44157.732850462962</v>
+        <v>44186.892302199078</v>
       </c>
       <c r="K26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44158.732850462962</v>
+        <v>44187.892302199078</v>
       </c>
       <c r="L26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44159.732850462962</v>
+        <v>44188.892302199078</v>
       </c>
       <c r="M26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44160.732850462962</v>
+        <v>44189.892302199078</v>
       </c>
       <c r="N26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>44161.732850462962</v>
+        <v>44190.892302199078</v>
       </c>
       <c r="O26" s="102">
         <f t="shared" ca="1" si="1"/>
-        <v>44162.732850462962</v>
+        <v>44191.892302199078</v>
       </c>
       <c r="P26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44163.732850462962</v>
+        <v>44192.892302199078</v>
       </c>
       <c r="Q26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44164.732850462962</v>
+        <v>44193.892302199078</v>
       </c>
       <c r="R26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44165.732850462962</v>
+        <v>44194.892302199078</v>
       </c>
       <c r="S26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.732850462962</v>
+        <v>44195.892302199078</v>
       </c>
       <c r="T26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44167.732850462962</v>
+        <v>44196.892302199078</v>
       </c>
       <c r="U26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>44168.732850462962</v>
+        <v>44197.892302199078</v>
       </c>
       <c r="V26" s="102">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>44169.732850462962</v>
+        <v>44198.892302199078</v>
       </c>
       <c r="W26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44170.732850462962</v>
+        <v>44199.892302199078</v>
       </c>
       <c r="X26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44171.732850462962</v>
+        <v>44200.892302199078</v>
       </c>
       <c r="Y26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44172.732850462962</v>
+        <v>44201.892302199078</v>
       </c>
       <c r="Z26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44173.732850462962</v>
+        <v>44202.892302199078</v>
       </c>
       <c r="AA26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44174.732850462962</v>
+        <v>44203.892302199078</v>
       </c>
       <c r="AB26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>44175.732850462962</v>
+        <v>44204.892302199078</v>
       </c>
       <c r="AC26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>44176.732850462962</v>
+        <v>44205.892302199078</v>
       </c>
       <c r="AD26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44177.732850462962</v>
+        <v>44206.892302199078</v>
       </c>
       <c r="AE26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44178.732850462962</v>
+        <v>44207.892302199078</v>
       </c>
       <c r="AF26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44179.732850462962</v>
+        <v>44208.892302199078</v>
       </c>
       <c r="AG26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44180.732850462962</v>
+        <v>44209.892302199078</v>
       </c>
       <c r="AH26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44181.732850462962</v>
+        <v>44210.892302199078</v>
       </c>
       <c r="AI26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>44182.732850462962</v>
+        <v>44211.892302199078</v>
       </c>
       <c r="AJ26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>44183.732850462962</v>
+        <v>44212.892302199078</v>
       </c>
       <c r="AK26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44184.732850462962</v>
+        <v>44213.892302199078</v>
       </c>
       <c r="AL26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44185.732850462962</v>
+        <v>44214.892302199078</v>
       </c>
       <c r="AM26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44186.732850462962</v>
+        <v>44215.892302199078</v>
       </c>
       <c r="AN26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44187.732850462962</v>
+        <v>44216.892302199078</v>
       </c>
       <c r="AO26" s="103">
         <f ca="1">AP26-1</f>
-        <v>44188.732850462962</v>
+        <v>44217.892302199078</v>
       </c>
       <c r="AP26" s="124">
         <f ca="1">NOW()</f>
-        <v>44189.732850462962</v>
+        <v>44218.892302199078</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -38290,7 +38290,7 @@
   <dimension ref="A1:AW136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ61" sqref="AJ61"/>
+      <selection activeCell="AI97" sqref="AI97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42987,7 +42987,7 @@
         <v>20856</v>
       </c>
       <c r="AH95" s="303">
-        <v>25719</v>
+        <v>25961</v>
       </c>
       <c r="AI95" s="303"/>
       <c r="AJ95" s="200"/>
@@ -43083,7 +43083,7 @@
         <v>600</v>
       </c>
       <c r="AH96" s="304">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="AI96" s="304"/>
       <c r="AJ96" s="201"/>
@@ -48760,7 +48760,7 @@
   <dimension ref="B3:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48804,7 +48804,7 @@
         <v>219</v>
       </c>
       <c r="C6" s="179">
-        <v>28258</v>
+        <v>28755</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -48813,7 +48813,7 @@
       </c>
       <c r="C7" s="177">
         <f ca="1">NOW()</f>
-        <v>44189.732850462962</v>
+        <v>44218.892302199078</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -48822,7 +48822,7 @@
       </c>
       <c r="C8" s="178">
         <f ca="1">C7-C5</f>
-        <v>297.73285046296223</v>
+        <v>326.89230219907768</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -48831,7 +48831,7 @@
       </c>
       <c r="C9" s="180">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>30.42321080493636</v>
+        <v>33.317174950890191</v>
       </c>
       <c r="D9" t="s">
         <v>196</v>
@@ -48864,7 +48864,7 @@
       </c>
       <c r="C12" s="185">
         <f>C6/Projections!B57</f>
-        <v>89012.700000000012</v>
+        <v>90578.25</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -48873,7 +48873,7 @@
       </c>
       <c r="C13" s="186">
         <f ca="1">(C4/Projections!B57)*(2^(((C7-21)-C5)/C9))</f>
-        <v>55164.82852107806</v>
+        <v>58517.134512051554</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -48882,7 +48882,7 @@
       </c>
       <c r="C14" s="165">
         <f ca="1">C12-C13</f>
-        <v>33847.871478921952</v>
+        <v>32061.115487948446</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" s="183" t="s">
@@ -48896,7 +48896,7 @@
       </c>
       <c r="C15" s="76">
         <f>C6*Projections!B61</f>
-        <v>22888.980000000003</v>
+        <v>23291.550000000003</v>
       </c>
       <c r="I15" s="176"/>
     </row>
@@ -48906,7 +48906,7 @@
       </c>
       <c r="C16" s="95">
         <f ca="1">(C4*Projections!B61)*(2^(((C7-21)-C5)/C9))</f>
-        <v>14185.241619705786</v>
+        <v>15047.263160241828</v>
       </c>
       <c r="I16" s="176"/>
     </row>
@@ -48916,7 +48916,7 @@
       </c>
       <c r="C17" s="95">
         <f ca="1">C15-C16</f>
-        <v>8703.7383802942168</v>
+        <v>8244.2868397581751</v>
       </c>
       <c r="F17" t="s">
         <v>244</v>
@@ -48929,7 +48929,7 @@
       </c>
       <c r="C18" s="76">
         <f>C6*Projections!B62</f>
-        <v>3956.1200000000003</v>
+        <v>4025.7000000000003</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -48938,7 +48938,7 @@
       </c>
       <c r="C19" s="95">
         <f ca="1">(C4*Projections!B62)*(2^(((C7-49)-C5)/C9))</f>
-        <v>1295.4683835891587</v>
+        <v>1452.4884933788703</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -48947,7 +48947,7 @@
       </c>
       <c r="C20" s="95">
         <f ca="1">C18-C19</f>
-        <v>2660.6516164108416</v>
+        <v>2573.21150662113</v>
       </c>
       <c r="F20" t="s">
         <v>249</v>
@@ -48959,7 +48959,7 @@
       </c>
       <c r="C21" s="76">
         <f>C6*Projections!B63</f>
-        <v>282.58</v>
+        <v>287.55</v>
       </c>
       <c r="I21" s="176"/>
     </row>
@@ -48969,7 +48969,7 @@
       </c>
       <c r="C22" s="95">
         <f ca="1">(C4*Projections!B63)*(2^(((C7-49)-C5)/C9))</f>
-        <v>92.533455970654202</v>
+        <v>103.74917809849072</v>
       </c>
       <c r="I22" s="176"/>
     </row>
@@ -48979,7 +48979,7 @@
       </c>
       <c r="C23" s="95">
         <f ca="1">C21-C22</f>
-        <v>190.0465440293458</v>
+        <v>183.80082190150929</v>
       </c>
       <c r="I23" s="176"/>
     </row>
@@ -48989,7 +48989,7 @@
       </c>
       <c r="C24" s="76">
         <f>C6*Projections!B64</f>
-        <v>890.12699999999995</v>
+        <v>905.78250000000003</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -48998,7 +48998,7 @@
       </c>
       <c r="C25" s="73">
         <f ca="1">(C4*Projections!B64)*(2^(((C7-42)-C5)/C9))</f>
-        <v>341.87911452634796</v>
+        <v>378.0438495446237</v>
       </c>
       <c r="F25" t="s">
         <v>255</v>
@@ -49010,7 +49010,7 @@
       </c>
       <c r="C26" s="189">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>239.78866111142099</v>
+        <v>261.76016961973738</v>
       </c>
       <c r="D26" t="s">
         <v>196</v>
@@ -49025,7 +49025,7 @@
       </c>
       <c r="C27" s="188">
         <f ca="1">C7+C26</f>
-        <v>44429.521511574385</v>
+        <v>44480.652471818816</v>
       </c>
       <c r="F27" t="s">
         <v>257</v>
@@ -49037,7 +49037,7 @@
       </c>
       <c r="C28" s="187">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>83.570263997272249</v>
+        <v>90.681722293092079</v>
       </c>
       <c r="D28" t="s">
         <v>196</v>
@@ -49049,7 +49049,7 @@
       </c>
       <c r="C29" s="188">
         <f ca="1">C7+C28</f>
-        <v>44273.303114460236</v>
+        <v>44309.574024492169</v>
       </c>
       <c r="F29" t="s">
         <v>257</v>
@@ -49061,7 +49061,7 @@
       </c>
       <c r="C30" s="187">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>226.13165284419628</v>
+        <v>246.80405809481417</v>
       </c>
       <c r="D30" t="s">
         <v>196</v>
@@ -49073,7 +49073,7 @@
       </c>
       <c r="C31" s="188">
         <f ca="1">C7+C30</f>
-        <v>44415.864503307159</v>
+        <v>44465.696360293892</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -49082,7 +49082,7 @@
       </c>
       <c r="C34" s="177">
         <f ca="1">C7+30</f>
-        <v>44219.732850462962</v>
+        <v>44248.892302199078</v>
       </c>
       <c r="F34" t="s">
         <v>275</v>
@@ -49094,7 +49094,7 @@
       </c>
       <c r="C35" s="95">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>55973.678929466732</v>
+        <v>53674.964267053299</v>
       </c>
       <c r="F35" t="s">
         <v>242</v>
@@ -49106,7 +49106,7 @@
       </c>
       <c r="C36" s="95">
         <f ca="1">C35/Projections!B57</f>
-        <v>176317.08862782022</v>
+        <v>169076.1374412179</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -49115,7 +49115,7 @@
       </c>
       <c r="C37" s="95">
         <f ca="1">C35*Projections!B61</f>
-        <v>45338.679932868057</v>
+        <v>43476.721056313174</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -49124,7 +49124,7 @@
       </c>
       <c r="C38" s="95">
         <f ca="1">C35*Projections!B62</f>
-        <v>7836.3150501253431</v>
+        <v>7514.4949973874627</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -49133,7 +49133,7 @@
       </c>
       <c r="C39" s="95">
         <f ca="1">C35*Projections!B63</f>
-        <v>559.73678929466735</v>
+        <v>536.74964267053304</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -49142,7 +49142,7 @@
       </c>
       <c r="C40" s="73">
         <f ca="1">C35*Projections!B64</f>
-        <v>1763.170886278202</v>
+        <v>1690.7613744121788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
US Deaths having passed 500,000
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7141789-3F2E-4727-B1BE-C13888D5A457}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5CA40A-8716-4E03-A074-0C49E1F4785F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
@@ -2298,46 +2298,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2447,46 +2447,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2596,46 +2596,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4074,6 +4074,9 @@
                   <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="#,##0">
+                  <c:v>909</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
                   <c:v>909</c:v>
                 </c:pt>
               </c:numCache>
@@ -14374,6 +14377,9 @@
                 <c:pt idx="22" formatCode="#,##0">
                   <c:v>909</c:v>
                 </c:pt>
+                <c:pt idx="23" formatCode="#,##0">
+                  <c:v>909</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14701,46 +14707,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14841,46 +14847,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14984,46 +14990,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15121,46 +15127,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15528,46 +15534,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15677,46 +15683,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15826,46 +15832,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16243,46 +16249,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16383,46 +16389,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16526,46 +16532,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16663,46 +16669,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44201.687025115738</c:v>
+                  <c:v>44211.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44204.687025115738</c:v>
+                  <c:v>44214.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44207.687025115738</c:v>
+                  <c:v>44217.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44210.687025115738</c:v>
+                  <c:v>44220.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44213.687025115738</c:v>
+                  <c:v>44223.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44216.687025115738</c:v>
+                  <c:v>44226.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44219.687025115738</c:v>
+                  <c:v>44229.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44222.687025115738</c:v>
+                  <c:v>44232.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44225.687025115738</c:v>
+                  <c:v>44235.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44228.687025115738</c:v>
+                  <c:v>44238.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44231.687025115738</c:v>
+                  <c:v>44241.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44234.687025115738</c:v>
+                  <c:v>44244.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44237.687025115738</c:v>
+                  <c:v>44247.87257013889</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44240.687025115738</c:v>
+                  <c:v>44250.87257013889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -37610,167 +37616,167 @@
       </c>
       <c r="B26" s="102">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>44201.687025115738</v>
+        <v>44211.87257013889</v>
       </c>
       <c r="C26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44202.687025115738</v>
+        <v>44212.87257013889</v>
       </c>
       <c r="D26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44203.687025115738</v>
+        <v>44213.87257013889</v>
       </c>
       <c r="E26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44204.687025115738</v>
+        <v>44214.87257013889</v>
       </c>
       <c r="F26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44205.687025115738</v>
+        <v>44215.87257013889</v>
       </c>
       <c r="G26" s="104">
         <f t="shared" ca="1" si="0"/>
-        <v>44206.687025115738</v>
+        <v>44216.87257013889</v>
       </c>
       <c r="H26" s="103">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>44207.687025115738</v>
+        <v>44217.87257013889</v>
       </c>
       <c r="I26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44208.687025115738</v>
+        <v>44218.87257013889</v>
       </c>
       <c r="J26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44209.687025115738</v>
+        <v>44219.87257013889</v>
       </c>
       <c r="K26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44210.687025115738</v>
+        <v>44220.87257013889</v>
       </c>
       <c r="L26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44211.687025115738</v>
+        <v>44221.87257013889</v>
       </c>
       <c r="M26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44212.687025115738</v>
+        <v>44222.87257013889</v>
       </c>
       <c r="N26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>44213.687025115738</v>
+        <v>44223.87257013889</v>
       </c>
       <c r="O26" s="102">
         <f t="shared" ca="1" si="1"/>
-        <v>44214.687025115738</v>
+        <v>44224.87257013889</v>
       </c>
       <c r="P26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44215.687025115738</v>
+        <v>44225.87257013889</v>
       </c>
       <c r="Q26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44216.687025115738</v>
+        <v>44226.87257013889</v>
       </c>
       <c r="R26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44217.687025115738</v>
+        <v>44227.87257013889</v>
       </c>
       <c r="S26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44218.687025115738</v>
+        <v>44228.87257013889</v>
       </c>
       <c r="T26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44219.687025115738</v>
+        <v>44229.87257013889</v>
       </c>
       <c r="U26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>44220.687025115738</v>
+        <v>44230.87257013889</v>
       </c>
       <c r="V26" s="102">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>44221.687025115738</v>
+        <v>44231.87257013889</v>
       </c>
       <c r="W26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44222.687025115738</v>
+        <v>44232.87257013889</v>
       </c>
       <c r="X26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44223.687025115738</v>
+        <v>44233.87257013889</v>
       </c>
       <c r="Y26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44224.687025115738</v>
+        <v>44234.87257013889</v>
       </c>
       <c r="Z26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44225.687025115738</v>
+        <v>44235.87257013889</v>
       </c>
       <c r="AA26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44226.687025115738</v>
+        <v>44236.87257013889</v>
       </c>
       <c r="AB26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>44227.687025115738</v>
+        <v>44237.87257013889</v>
       </c>
       <c r="AC26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>44228.687025115738</v>
+        <v>44238.87257013889</v>
       </c>
       <c r="AD26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44229.687025115738</v>
+        <v>44239.87257013889</v>
       </c>
       <c r="AE26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44230.687025115738</v>
+        <v>44240.87257013889</v>
       </c>
       <c r="AF26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44231.687025115738</v>
+        <v>44241.87257013889</v>
       </c>
       <c r="AG26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44232.687025115738</v>
+        <v>44242.87257013889</v>
       </c>
       <c r="AH26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44233.687025115738</v>
+        <v>44243.87257013889</v>
       </c>
       <c r="AI26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>44234.687025115738</v>
+        <v>44244.87257013889</v>
       </c>
       <c r="AJ26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>44235.687025115738</v>
+        <v>44245.87257013889</v>
       </c>
       <c r="AK26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44236.687025115738</v>
+        <v>44246.87257013889</v>
       </c>
       <c r="AL26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44237.687025115738</v>
+        <v>44247.87257013889</v>
       </c>
       <c r="AM26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44238.687025115738</v>
+        <v>44248.87257013889</v>
       </c>
       <c r="AN26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44239.687025115738</v>
+        <v>44249.87257013889</v>
       </c>
       <c r="AO26" s="103">
         <f ca="1">AP26-1</f>
-        <v>44240.687025115738</v>
+        <v>44250.87257013889</v>
       </c>
       <c r="AP26" s="124">
         <f ca="1">NOW()</f>
-        <v>44241.687025115738</v>
+        <v>44251.87257013889</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -38288,8 +38294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BB0FAD-39ED-4D53-8BC6-75164ED434B0}">
   <dimension ref="A1:AW136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK66" sqref="AK66"/>
+    <sheetView tabSelected="1" topLeftCell="F47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ64" sqref="AJ64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42991,7 +42997,9 @@
         <f t="shared" ref="AH95" si="80">AH92-AH94-AH96</f>
         <v>26035</v>
       </c>
-      <c r="AI95" s="303"/>
+      <c r="AI95" s="303">
+        <v>26156</v>
+      </c>
       <c r="AJ95" s="200"/>
       <c r="AK95" s="200"/>
       <c r="AL95" s="200"/>
@@ -43087,7 +43095,9 @@
       <c r="AH96" s="64">
         <v>909</v>
       </c>
-      <c r="AI96" s="304"/>
+      <c r="AI96" s="304">
+        <v>909</v>
+      </c>
       <c r="AJ96" s="201"/>
       <c r="AK96" s="201"/>
       <c r="AL96" s="201"/>
@@ -48762,7 +48772,7 @@
   <dimension ref="B3:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48806,7 +48816,7 @@
         <v>219</v>
       </c>
       <c r="C6" s="179">
-        <v>28898</v>
+        <v>28939</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -48815,7 +48825,7 @@
       </c>
       <c r="C7" s="177">
         <f ca="1">NOW()</f>
-        <v>44241.687024999999</v>
+        <v>44251.87257013889</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -48824,7 +48834,7 @@
       </c>
       <c r="C8" s="178">
         <f ca="1">C7-C5</f>
-        <v>349.68702499999927</v>
+        <v>359.8725701388903</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -48833,7 +48843,7 @@
       </c>
       <c r="C9" s="180">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>35.614456603332734</v>
+        <v>36.644186695567683</v>
       </c>
       <c r="D9" t="s">
         <v>196</v>
@@ -48866,7 +48876,7 @@
       </c>
       <c r="C12" s="185">
         <f>C6/Projections!B57</f>
-        <v>91028.700000000012</v>
+        <v>91157.85</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -48875,7 +48885,7 @@
       </c>
       <c r="C13" s="186">
         <f ca="1">(C4/Projections!B57)*(2^(((C7-21)-C5)/C9))</f>
-        <v>60489.019853197169</v>
+        <v>61274.562436789267</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -48884,7 +48894,7 @@
       </c>
       <c r="C14" s="165">
         <f ca="1">C12-C13</f>
-        <v>30539.680146802843</v>
+        <v>29883.287563210739</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" s="183" t="s">
@@ -48898,7 +48908,7 @@
       </c>
       <c r="C15" s="76">
         <f>C6*Projections!B61</f>
-        <v>23407.38</v>
+        <v>23440.59</v>
       </c>
       <c r="I15" s="176"/>
     </row>
@@ -48908,7 +48918,7 @@
       </c>
       <c r="C16" s="95">
         <f ca="1">(C4*Projections!B61)*(2^(((C7-21)-C5)/C9))</f>
-        <v>15554.319390822129</v>
+        <v>15756.316055174382</v>
       </c>
       <c r="I16" s="176"/>
     </row>
@@ -48918,7 +48928,7 @@
       </c>
       <c r="C17" s="95">
         <f ca="1">C15-C16</f>
-        <v>7853.0606091778718</v>
+        <v>7684.2739448256179</v>
       </c>
       <c r="F17" t="s">
         <v>244</v>
@@ -48931,7 +48941,7 @@
       </c>
       <c r="C18" s="76">
         <f>C6*Projections!B62</f>
-        <v>4045.7200000000003</v>
+        <v>4051.4600000000005</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -48940,7 +48950,7 @@
       </c>
       <c r="C19" s="95">
         <f ca="1">(C4*Projections!B62)*(2^(((C7-49)-C5)/C9))</f>
-        <v>1558.9241025851998</v>
+        <v>1603.5378933122947</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -48949,7 +48959,7 @@
       </c>
       <c r="C20" s="95">
         <f ca="1">C18-C19</f>
-        <v>2486.7958974148005</v>
+        <v>2447.9221066877058</v>
       </c>
       <c r="F20" t="s">
         <v>249</v>
@@ -48961,7 +48971,7 @@
       </c>
       <c r="C21" s="76">
         <f>C6*Projections!B63</f>
-        <v>288.98</v>
+        <v>289.39</v>
       </c>
       <c r="I21" s="176"/>
     </row>
@@ -48971,7 +48981,7 @@
       </c>
       <c r="C22" s="95">
         <f ca="1">(C4*Projections!B63)*(2^(((C7-49)-C5)/C9))</f>
-        <v>111.35172161322855</v>
+        <v>114.53842095087819</v>
       </c>
       <c r="I22" s="176"/>
     </row>
@@ -48981,7 +48991,7 @@
       </c>
       <c r="C23" s="95">
         <f ca="1">C21-C22</f>
-        <v>177.62827838677146</v>
+        <v>174.8515790491218</v>
       </c>
       <c r="I23" s="176"/>
     </row>
@@ -48991,7 +49001,7 @@
       </c>
       <c r="C24" s="76">
         <f>C6*Projections!B64</f>
-        <v>910.28700000000003</v>
+        <v>911.57849999999996</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -49000,7 +49010,7 @@
       </c>
       <c r="C25" s="73">
         <f ca="1">(C4*Projections!B64)*(2^(((C7-42)-C5)/C9))</f>
-        <v>401.95251857935796</v>
+        <v>411.87588362603867</v>
       </c>
       <c r="F25" t="s">
         <v>255</v>
@@ -49012,7 +49022,7 @@
       </c>
       <c r="C26" s="189">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>279.55413794186632</v>
+        <v>287.562007010326</v>
       </c>
       <c r="D26" t="s">
         <v>196</v>
@@ -49027,7 +49037,7 @@
       </c>
       <c r="C27" s="188">
         <f ca="1">C7+C26</f>
-        <v>44521.241162941864</v>
+        <v>44539.434577149215</v>
       </c>
       <c r="F27" t="s">
         <v>257</v>
@@ -49039,7 +49049,7 @@
       </c>
       <c r="C28" s="187">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>96.679511054643925</v>
+        <v>99.399878238422644</v>
       </c>
       <c r="D28" t="s">
         <v>196</v>
@@ -49051,7 +49061,7 @@
       </c>
       <c r="C29" s="188">
         <f ca="1">C7+C28</f>
-        <v>44338.366536054644</v>
+        <v>44351.272448377313</v>
       </c>
       <c r="F29" t="s">
         <v>257</v>
@@ -49063,7 +49073,7 @@
       </c>
       <c r="C30" s="187">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>263.56677449811332</v>
+        <v>271.11239674874605</v>
       </c>
       <c r="D30" t="s">
         <v>196</v>
@@ -49075,7 +49085,7 @@
       </c>
       <c r="C31" s="188">
         <f ca="1">C7+C30</f>
-        <v>44505.25379949811</v>
+        <v>44522.984966887634</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -49084,7 +49094,7 @@
       </c>
       <c r="C34" s="177">
         <f ca="1">C7+30</f>
-        <v>44271.687024999999</v>
+        <v>44281.87257013889</v>
       </c>
       <c r="F34" t="s">
         <v>275</v>
@@ -49096,7 +49106,7 @@
       </c>
       <c r="C35" s="95">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>51813.362451880748</v>
+        <v>51042.493722432126</v>
       </c>
       <c r="F35" t="s">
         <v>242</v>
@@ -49108,7 +49118,7 @@
       </c>
       <c r="C36" s="95">
         <f ca="1">C35/Projections!B57</f>
-        <v>163212.09172342435</v>
+        <v>160783.85522566122</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -49117,7 +49127,7 @@
       </c>
       <c r="C37" s="95">
         <f ca="1">C35*Projections!B61</f>
-        <v>41968.823586023405</v>
+        <v>41344.419915170023</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -49126,7 +49136,7 @@
       </c>
       <c r="C38" s="95">
         <f ca="1">C35*Projections!B62</f>
-        <v>7253.8707432633055</v>
+        <v>7145.9491211404984</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -49135,7 +49145,7 @@
       </c>
       <c r="C39" s="95">
         <f ca="1">C35*Projections!B63</f>
-        <v>518.13362451880744</v>
+        <v>510.42493722432124</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -49144,7 +49154,7 @@
       </c>
       <c r="C40" s="73">
         <f ca="1">C35*Projections!B64</f>
-        <v>1632.1209172342435</v>
+        <v>1607.838552256612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Year since first US COVID death
</commit_message>
<xml_diff>
--- a/Australian COVID-19 Infection Projections 20200315.xlsx
+++ b/Australian COVID-19 Infection Projections 20200315.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5CA40A-8716-4E03-A074-0C49E1F4785F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5156D8-20C9-4119-B5FC-FEC97212B58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
@@ -2298,46 +2298,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2447,46 +2447,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2596,46 +2596,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14707,46 +14707,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14847,46 +14847,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14990,46 +14990,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15127,46 +15127,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15534,46 +15534,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15683,46 +15683,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15832,46 +15832,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16249,46 +16249,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16389,46 +16389,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16532,46 +16532,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16669,46 +16669,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>44211.87257013889</c:v>
+                  <c:v>44216.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44214.87257013889</c:v>
+                  <c:v>44219.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44217.87257013889</c:v>
+                  <c:v>44222.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44220.87257013889</c:v>
+                  <c:v>44225.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44223.87257013889</c:v>
+                  <c:v>44228.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44226.87257013889</c:v>
+                  <c:v>44231.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44229.87257013889</c:v>
+                  <c:v>44234.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44232.87257013889</c:v>
+                  <c:v>44237.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44235.87257013889</c:v>
+                  <c:v>44240.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44238.87257013889</c:v>
+                  <c:v>44243.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44241.87257013889</c:v>
+                  <c:v>44246.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44244.87257013889</c:v>
+                  <c:v>44249.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44247.87257013889</c:v>
+                  <c:v>44252.878484606481</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44250.87257013889</c:v>
+                  <c:v>44255.878484606481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -37616,167 +37616,167 @@
       </c>
       <c r="B26" s="102">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>44211.87257013889</v>
+        <v>44216.878484606481</v>
       </c>
       <c r="C26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44212.87257013889</v>
+        <v>44217.878484606481</v>
       </c>
       <c r="D26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44213.87257013889</v>
+        <v>44218.878484606481</v>
       </c>
       <c r="E26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44214.87257013889</v>
+        <v>44219.878484606481</v>
       </c>
       <c r="F26" s="103">
         <f t="shared" ca="1" si="0"/>
-        <v>44215.87257013889</v>
+        <v>44220.878484606481</v>
       </c>
       <c r="G26" s="104">
         <f t="shared" ca="1" si="0"/>
-        <v>44216.87257013889</v>
+        <v>44221.878484606481</v>
       </c>
       <c r="H26" s="103">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>44217.87257013889</v>
+        <v>44222.878484606481</v>
       </c>
       <c r="I26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44218.87257013889</v>
+        <v>44223.878484606481</v>
       </c>
       <c r="J26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44219.87257013889</v>
+        <v>44224.878484606481</v>
       </c>
       <c r="K26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44220.87257013889</v>
+        <v>44225.878484606481</v>
       </c>
       <c r="L26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44221.87257013889</v>
+        <v>44226.878484606481</v>
       </c>
       <c r="M26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44222.87257013889</v>
+        <v>44227.878484606481</v>
       </c>
       <c r="N26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>44223.87257013889</v>
+        <v>44228.878484606481</v>
       </c>
       <c r="O26" s="102">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.87257013889</v>
+        <v>44229.878484606481</v>
       </c>
       <c r="P26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44225.87257013889</v>
+        <v>44230.878484606481</v>
       </c>
       <c r="Q26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44226.87257013889</v>
+        <v>44231.878484606481</v>
       </c>
       <c r="R26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44227.87257013889</v>
+        <v>44232.878484606481</v>
       </c>
       <c r="S26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44228.87257013889</v>
+        <v>44233.878484606481</v>
       </c>
       <c r="T26" s="103">
         <f t="shared" ca="1" si="1"/>
-        <v>44229.87257013889</v>
+        <v>44234.878484606481</v>
       </c>
       <c r="U26" s="104">
         <f t="shared" ca="1" si="1"/>
-        <v>44230.87257013889</v>
+        <v>44235.878484606481</v>
       </c>
       <c r="V26" s="102">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>44231.87257013889</v>
+        <v>44236.878484606481</v>
       </c>
       <c r="W26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44232.87257013889</v>
+        <v>44237.878484606481</v>
       </c>
       <c r="X26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44233.87257013889</v>
+        <v>44238.878484606481</v>
       </c>
       <c r="Y26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44234.87257013889</v>
+        <v>44239.878484606481</v>
       </c>
       <c r="Z26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44235.87257013889</v>
+        <v>44240.878484606481</v>
       </c>
       <c r="AA26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44236.87257013889</v>
+        <v>44241.878484606481</v>
       </c>
       <c r="AB26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>44237.87257013889</v>
+        <v>44242.878484606481</v>
       </c>
       <c r="AC26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>44238.87257013889</v>
+        <v>44243.878484606481</v>
       </c>
       <c r="AD26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44239.87257013889</v>
+        <v>44244.878484606481</v>
       </c>
       <c r="AE26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44240.87257013889</v>
+        <v>44245.878484606481</v>
       </c>
       <c r="AF26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44241.87257013889</v>
+        <v>44246.878484606481</v>
       </c>
       <c r="AG26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44242.87257013889</v>
+        <v>44247.878484606481</v>
       </c>
       <c r="AH26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44243.87257013889</v>
+        <v>44248.878484606481</v>
       </c>
       <c r="AI26" s="104">
         <f t="shared" ca="1" si="2"/>
-        <v>44244.87257013889</v>
+        <v>44249.878484606481</v>
       </c>
       <c r="AJ26" s="102">
         <f t="shared" ca="1" si="2"/>
-        <v>44245.87257013889</v>
+        <v>44250.878484606481</v>
       </c>
       <c r="AK26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44246.87257013889</v>
+        <v>44251.878484606481</v>
       </c>
       <c r="AL26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44247.87257013889</v>
+        <v>44252.878484606481</v>
       </c>
       <c r="AM26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44248.87257013889</v>
+        <v>44253.878484606481</v>
       </c>
       <c r="AN26" s="103">
         <f t="shared" ca="1" si="2"/>
-        <v>44249.87257013889</v>
+        <v>44254.878484606481</v>
       </c>
       <c r="AO26" s="103">
         <f ca="1">AP26-1</f>
-        <v>44250.87257013889</v>
+        <v>44255.878484606481</v>
       </c>
       <c r="AP26" s="124">
         <f ca="1">NOW()</f>
-        <v>44251.87257013889</v>
+        <v>44256.878484606481</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -38295,7 +38295,7 @@
   <dimension ref="A1:AW136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ64" sqref="AJ64"/>
+      <selection activeCell="AJ62" sqref="AJ62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42998,7 +42998,7 @@
         <v>26035</v>
       </c>
       <c r="AI95" s="303">
-        <v>26156</v>
+        <v>26175</v>
       </c>
       <c r="AJ95" s="200"/>
       <c r="AK95" s="200"/>
@@ -48772,7 +48772,7 @@
   <dimension ref="B3:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48816,7 +48816,7 @@
         <v>219</v>
       </c>
       <c r="C6" s="179">
-        <v>28939</v>
+        <v>28975</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -48825,7 +48825,7 @@
       </c>
       <c r="C7" s="177">
         <f ca="1">NOW()</f>
-        <v>44251.87257013889</v>
+        <v>44256.878484606481</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -48834,7 +48834,7 @@
       </c>
       <c r="C8" s="178">
         <f ca="1">C7-C5</f>
-        <v>359.8725701388903</v>
+        <v>364.87848460648092</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -48843,7 +48843,7 @@
       </c>
       <c r="C9" s="180">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>36.644186695567683</v>
+        <v>37.147131891250361</v>
       </c>
       <c r="D9" t="s">
         <v>196</v>
@@ -48876,7 +48876,7 @@
       </c>
       <c r="C12" s="185">
         <f>C6/Projections!B57</f>
-        <v>91157.85</v>
+        <v>91271.25</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -48885,7 +48885,7 @@
       </c>
       <c r="C13" s="186">
         <f ca="1">(C4/Projections!B57)*(2^(((C7-21)-C5)/C9))</f>
-        <v>61274.562436789267</v>
+        <v>61681.631979166312</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="81" customFormat="1" x14ac:dyDescent="0.25">
@@ -48894,7 +48894,7 @@
       </c>
       <c r="C14" s="165">
         <f ca="1">C12-C13</f>
-        <v>29883.287563210739</v>
+        <v>29589.618020833688</v>
       </c>
       <c r="E14" s="182"/>
       <c r="F14" s="183" t="s">
@@ -48908,7 +48908,7 @@
       </c>
       <c r="C15" s="76">
         <f>C6*Projections!B61</f>
-        <v>23440.59</v>
+        <v>23469.75</v>
       </c>
       <c r="I15" s="176"/>
     </row>
@@ -48918,7 +48918,7 @@
       </c>
       <c r="C16" s="95">
         <f ca="1">(C4*Projections!B61)*(2^(((C7-21)-C5)/C9))</f>
-        <v>15756.316055174382</v>
+        <v>15860.991080357051</v>
       </c>
       <c r="I16" s="176"/>
     </row>
@@ -48928,7 +48928,7 @@
       </c>
       <c r="C17" s="95">
         <f ca="1">C15-C16</f>
-        <v>7684.2739448256179</v>
+        <v>7608.758919642949</v>
       </c>
       <c r="F17" t="s">
         <v>244</v>
@@ -48941,7 +48941,7 @@
       </c>
       <c r="C18" s="76">
         <f>C6*Projections!B62</f>
-        <v>4051.4600000000005</v>
+        <v>4056.5000000000005</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -48950,7 +48950,7 @@
       </c>
       <c r="C19" s="95">
         <f ca="1">(C4*Projections!B62)*(2^(((C7-49)-C5)/C9))</f>
-        <v>1603.5378933122947</v>
+        <v>1625.8075931015642</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -48959,7 +48959,7 @@
       </c>
       <c r="C20" s="95">
         <f ca="1">C18-C19</f>
-        <v>2447.9221066877058</v>
+        <v>2430.6924068984363</v>
       </c>
       <c r="F20" t="s">
         <v>249</v>
@@ -48971,7 +48971,7 @@
       </c>
       <c r="C21" s="76">
         <f>C6*Projections!B63</f>
-        <v>289.39</v>
+        <v>289.75</v>
       </c>
       <c r="I21" s="176"/>
     </row>
@@ -48981,7 +48981,7 @@
       </c>
       <c r="C22" s="95">
         <f ca="1">(C4*Projections!B63)*(2^(((C7-49)-C5)/C9))</f>
-        <v>114.53842095087819</v>
+        <v>116.12911379296885</v>
       </c>
       <c r="I22" s="176"/>
     </row>
@@ -48991,7 +48991,7 @@
       </c>
       <c r="C23" s="95">
         <f ca="1">C21-C22</f>
-        <v>174.8515790491218</v>
+        <v>173.62088620703116</v>
       </c>
       <c r="I23" s="176"/>
     </row>
@@ -49001,7 +49001,7 @@
       </c>
       <c r="C24" s="76">
         <f>C6*Projections!B64</f>
-        <v>911.57849999999996</v>
+        <v>912.71249999999998</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -49010,7 +49010,7 @@
       </c>
       <c r="C25" s="73">
         <f ca="1">(C4*Projections!B64)*(2^(((C7-42)-C5)/C9))</f>
-        <v>411.87588362603867</v>
+        <v>416.84799141167741</v>
       </c>
       <c r="F25" t="s">
         <v>255</v>
@@ -49022,7 +49022,7 @@
       </c>
       <c r="C26" s="189">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>287.562007010326</v>
+        <v>291.44219807432393</v>
       </c>
       <c r="D26" t="s">
         <v>196</v>
@@ -49037,7 +49037,7 @@
       </c>
       <c r="C27" s="188">
         <f ca="1">C7+C26</f>
-        <v>44539.434577149215</v>
+        <v>44548.320682680802</v>
       </c>
       <c r="F27" t="s">
         <v>257</v>
@@ -49049,7 +49049,7 @@
       </c>
       <c r="C28" s="187">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>99.399878238422644</v>
+        <v>100.69752491519039</v>
       </c>
       <c r="D28" t="s">
         <v>196</v>
@@ -49061,7 +49061,7 @@
       </c>
       <c r="C29" s="188">
         <f ca="1">C7+C28</f>
-        <v>44351.272448377313</v>
+        <v>44357.576009521668</v>
       </c>
       <c r="F29" t="s">
         <v>257</v>
@@ -49073,7 +49073,7 @@
       </c>
       <c r="C30" s="187">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>271.11239674874605</v>
+        <v>274.76681523602815</v>
       </c>
       <c r="D30" t="s">
         <v>196</v>
@@ -49085,7 +49085,7 @@
       </c>
       <c r="C31" s="188">
         <f ca="1">C7+C30</f>
-        <v>44522.984966887634</v>
+        <v>44531.645299842508</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -49094,7 +49094,7 @@
       </c>
       <c r="C34" s="177">
         <f ca="1">C7+30</f>
-        <v>44281.87257013889</v>
+        <v>44286.878484606481</v>
       </c>
       <c r="F34" t="s">
         <v>275</v>
@@ -49106,7 +49106,7 @@
       </c>
       <c r="C35" s="95">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>51042.493722432126</v>
+        <v>50714.842017994022</v>
       </c>
       <c r="F35" t="s">
         <v>242</v>
@@ -49118,7 +49118,7 @@
       </c>
       <c r="C36" s="95">
         <f ca="1">C35/Projections!B57</f>
-        <v>160783.85522566122</v>
+        <v>159751.75235668119</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -49127,7 +49127,7 @@
       </c>
       <c r="C37" s="95">
         <f ca="1">C35*Projections!B61</f>
-        <v>41344.419915170023</v>
+        <v>41079.022034575159</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -49136,7 +49136,7 @@
       </c>
       <c r="C38" s="95">
         <f ca="1">C35*Projections!B62</f>
-        <v>7145.9491211404984</v>
+        <v>7100.0778825191637</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -49145,7 +49145,7 @@
       </c>
       <c r="C39" s="95">
         <f ca="1">C35*Projections!B63</f>
-        <v>510.42493722432124</v>
+        <v>507.14842017994022</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -49154,7 +49154,7 @@
       </c>
       <c r="C40" s="73">
         <f ca="1">C35*Projections!B64</f>
-        <v>1607.838552256612</v>
+        <v>1597.5175235668116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>